<commit_message>
updating path to helper methods
</commit_message>
<xml_diff>
--- a/projects/m0.xlsx
+++ b/projects/m0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25125" windowHeight="15585" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="25125" windowHeight="15585" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2224" uniqueCount="745">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2231" uniqueCount="748">
   <si>
     <t>type</t>
   </si>
@@ -1906,6 +1906,9 @@
     <t>retail</t>
   </si>
   <si>
+    <t>0.3.0</t>
+  </si>
+  <si>
     <t>bool</t>
   </si>
   <si>
@@ -1999,6 +2002,9 @@
     <t>../seeds/EmptySeedModel.osm</t>
   </si>
   <si>
+    <t>Directory</t>
+  </si>
+  <si>
     <t>../weather/*</t>
   </si>
   <si>
@@ -2053,9 +2059,6 @@
     <t>../analysis</t>
   </si>
   <si>
-    <t>SPtMasterTable_15084_2013_amy.epw</t>
-  </si>
-  <si>
     <t>calibration_reports.electric_bill_consumption_modeled</t>
   </si>
   <si>
@@ -2203,9 +2206,6 @@
     <t>standard_reports.total_building_area</t>
   </si>
   <si>
-    <t>0.3.5</t>
-  </si>
-  <si>
     <t>1.8.0-pre12</t>
   </si>
   <si>
@@ -2276,6 +2276,15 @@
   </si>
   <si>
     <t>Envelope Aspect Ratio</t>
+  </si>
+  <si>
+    <t>USA_MA_Boston-Logan.Intl.AP.725090_TMY3.epw</t>
+  </si>
+  <si>
+    <t>../../../GitHub/cofee-measures/lib/</t>
+  </si>
+  <si>
+    <t>cofee</t>
   </si>
 </sst>
 </file>
@@ -6462,8 +6471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6499,7 +6508,7 @@
         <v>436</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>720</v>
+        <v>621</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>437</v>
@@ -6510,7 +6519,7 @@
         <v>456</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>457</v>
@@ -6603,7 +6612,7 @@
         <v>39</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>471</v>
@@ -6617,7 +6626,7 @@
         <v>722</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -6625,10 +6634,10 @@
         <v>26</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -6693,7 +6702,7 @@
         <v>451</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -6782,7 +6791,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>31</v>
@@ -6795,7 +6804,7 @@
         <v>29</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -6809,7 +6818,7 @@
         <v>38</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="E39" s="13" t="s">
         <v>449</v>
@@ -6820,10 +6829,10 @@
         <v>32</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>620</v>
@@ -6837,7 +6846,7 @@
         <v>34</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="13" t="s">
@@ -6845,8 +6854,15 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="31"/>
-      <c r="C43" s="31"/>
+      <c r="A43" s="31" t="s">
+        <v>653</v>
+      </c>
+      <c r="B43" s="26" t="s">
+        <v>747</v>
+      </c>
+      <c r="C43" s="25" t="s">
+        <v>746</v>
+      </c>
     </row>
     <row r="44" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="26"/>
@@ -6878,9 +6894,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H24" sqref="H24"/>
+      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7038,13 +7054,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>68</v>
@@ -7057,16 +7073,16 @@
         <v>21</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="F5" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
     </row>
     <row r="6" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -7074,16 +7090,16 @@
         <v>21</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="F6" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H6" s="31" t="s">
-        <v>670</v>
+        <v>745</v>
       </c>
     </row>
     <row r="7" spans="1:25" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -7164,7 +7180,7 @@
         <v>728</v>
       </c>
       <c r="F10" s="31" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="H10" s="31" t="b">
         <v>1</v>
@@ -7249,7 +7265,7 @@
         <v>728</v>
       </c>
       <c r="F14" s="31" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="H14" s="31" t="b">
         <v>0</v>
@@ -7334,7 +7350,7 @@
         <v>728</v>
       </c>
       <c r="F18" s="31" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="H18" s="31" t="b">
         <v>0</v>
@@ -7361,6 +7377,9 @@
       <c r="H19" s="38"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B20" s="31" t="s">
+        <v>21</v>
+      </c>
       <c r="D20" s="31" t="s">
         <v>738</v>
       </c>
@@ -7383,6 +7402,9 @@
       <c r="Q20" s="2"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B21" s="31" t="s">
+        <v>21</v>
+      </c>
       <c r="D21" s="31" t="s">
         <v>740</v>
       </c>
@@ -7393,7 +7415,7 @@
         <v>619</v>
       </c>
       <c r="G21" s="31" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="H21" s="4">
         <v>10</v>
@@ -7406,6 +7428,9 @@
       <c r="P21" s="3"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B22" s="31" t="s">
+        <v>21</v>
+      </c>
       <c r="D22" s="31" t="s">
         <v>742</v>
       </c>
@@ -7416,7 +7441,7 @@
         <v>619</v>
       </c>
       <c r="G22" s="31" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="H22" s="4">
         <v>10</v>
@@ -7424,6 +7449,9 @@
       <c r="I22" s="31"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B23" s="31" t="s">
+        <v>21</v>
+      </c>
       <c r="D23" s="31" t="s">
         <v>744</v>
       </c>
@@ -8052,7 +8080,7 @@
         <v>459</v>
       </c>
       <c r="B2" s="44" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="C2" s="43" t="s">
         <v>460</v>
@@ -8064,38 +8092,38 @@
         <v>11</v>
       </c>
       <c r="F2" s="43" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="G2" s="43" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="H2" s="43" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="I2" s="43" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="J2" s="43" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="K2" s="43" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="L2" s="43"/>
     </row>
     <row r="3" spans="1:12" s="14" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="44" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="D3" s="44"/>
       <c r="E3" s="44" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="F3" s="44" t="s">
         <v>461</v>
@@ -8113,21 +8141,21 @@
         <v>619</v>
       </c>
       <c r="K3" s="44" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="L3" s="44" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="40" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="D4" s="40" t="s">
         <v>468</v>
@@ -8151,13 +8179,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="40" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="D5" s="40" t="s">
         <v>468</v>
@@ -8181,13 +8209,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="40" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="D6" s="40" t="s">
         <v>468</v>
@@ -8211,13 +8239,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="40" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="D7" s="40" t="s">
         <v>468</v>
@@ -8241,11 +8269,11 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="40" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="B8" s="40"/>
       <c r="C8" s="40" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="D8" s="40" t="s">
         <v>468</v>
@@ -8269,11 +8297,11 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="40" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="B9" s="40"/>
       <c r="C9" s="40" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="D9" s="40" t="s">
         <v>468</v>
@@ -8297,11 +8325,11 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="40" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="B10" s="40"/>
       <c r="C10" s="40" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="D10" s="40" t="s">
         <v>468</v>
@@ -8325,11 +8353,11 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="B11" s="40"/>
       <c r="C11" s="40" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="D11" s="40" t="s">
         <v>468</v>
@@ -8353,11 +8381,11 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="B12" s="40"/>
       <c r="C12" s="40" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="D12" s="40" t="s">
         <v>468</v>
@@ -8381,11 +8409,11 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="40" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="B13" s="40"/>
       <c r="C13" s="40" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="D13" s="40" t="s">
         <v>468</v>
@@ -8409,11 +8437,11 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="40" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="B14" s="40"/>
       <c r="C14" s="40" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="D14" s="40" t="s">
         <v>468</v>
@@ -8437,11 +8465,11 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="40" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="B15" s="40"/>
       <c r="C15" s="40" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="D15" s="40" t="s">
         <v>468</v>
@@ -8465,11 +8493,11 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="40" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B16" s="40"/>
       <c r="C16" s="40" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D16" s="40" t="s">
         <v>468</v>
@@ -8493,11 +8521,11 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="40" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="B17" s="40"/>
       <c r="C17" s="40" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="D17" s="40" t="s">
         <v>468</v>
@@ -8521,11 +8549,11 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="40" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="B18" s="40"/>
       <c r="C18" s="40" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="D18" s="40" t="s">
         <v>468</v>
@@ -8549,11 +8577,11 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="40" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="B19" s="40"/>
       <c r="C19" s="40" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="D19" s="40" t="s">
         <v>468</v>
@@ -8577,11 +8605,11 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="40" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="B20" s="40"/>
       <c r="C20" s="40" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="D20" s="40" t="s">
         <v>468</v>
@@ -8605,11 +8633,11 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="40" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B21" s="40"/>
       <c r="C21" s="40" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="D21" s="40" t="s">
         <v>468</v>
@@ -8633,14 +8661,14 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="40" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="B22" s="40"/>
       <c r="C22" s="40" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="D22" s="40" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="E22" s="40" t="s">
         <v>64</v>
@@ -8661,14 +8689,14 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="40" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="B23" s="40"/>
       <c r="C23" s="40" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="D23" s="40" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="E23" s="40" t="s">
         <v>64</v>
@@ -8689,14 +8717,14 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="40" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="B24" s="40"/>
       <c r="C24" s="40" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="D24" s="40" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="E24" s="40" t="s">
         <v>64</v>
@@ -8717,14 +8745,14 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="40" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="B25" s="40"/>
       <c r="C25" s="40" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="D25" s="40" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="E25" s="40" t="s">
         <v>64</v>
@@ -8745,14 +8773,14 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="40" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="B26" s="40"/>
       <c r="C26" s="40" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="D26" s="40" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="E26" s="40" t="s">
         <v>64</v>
@@ -8773,14 +8801,14 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="40" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="B27" s="40"/>
       <c r="C27" s="40" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D27" s="40" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="E27" s="40" t="s">
         <v>64</v>
@@ -8801,14 +8829,14 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="40" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="B28" s="40"/>
       <c r="C28" s="40" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="D28" s="40" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="E28" s="40" t="s">
         <v>64</v>
@@ -8831,14 +8859,14 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="40" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="B29" s="40"/>
       <c r="C29" s="40" t="s">
+        <v>676</v>
+      </c>
+      <c r="D29" s="40" t="s">
         <v>675</v>
-      </c>
-      <c r="D29" s="40" t="s">
-        <v>674</v>
       </c>
       <c r="E29" s="40" t="s">
         <v>64</v>
@@ -8861,14 +8889,14 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="40" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="B30" s="40"/>
       <c r="C30" s="40" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="D30" s="40" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="E30" s="40" t="s">
         <v>64</v>
@@ -8891,14 +8919,14 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="40" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="B31" s="40"/>
       <c r="C31" s="40" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="D31" s="40" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="E31" s="40" t="s">
         <v>64</v>
@@ -17594,7 +17622,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>557</v>

</xml_diff>

<commit_message>
added most measures prior to hvac to spreadsheet
I still need to add swh, exhaust, and exterior lights once I finish
those measures.
</commit_message>
<xml_diff>
--- a/projects/m0.xlsx
+++ b/projects/m0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25125" windowHeight="15585" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="540" windowWidth="25125" windowHeight="15525" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$89</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$55</definedName>
     <definedName name="AnalysisType">Lookups!$A$17:$A$23</definedName>
     <definedName name="instance_defs">Lookups!$A$2:$D$9</definedName>
     <definedName name="instance_types">Lookups!$A$2:$A$9</definedName>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2231" uniqueCount="748">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2363" uniqueCount="818">
   <si>
     <t>type</t>
   </si>
@@ -1987,6 +1987,45 @@
     <t>Total Electricity Intensity</t>
   </si>
   <si>
+    <t>SpaceTypeAndConstructionSetWizard</t>
+  </si>
+  <si>
+    <t>buildingType</t>
+  </si>
+  <si>
+    <t>Building Type</t>
+  </si>
+  <si>
+    <t>Template</t>
+  </si>
+  <si>
+    <t>template</t>
+  </si>
+  <si>
+    <t>ASHRAE Climate Zone</t>
+  </si>
+  <si>
+    <t>climateZone</t>
+  </si>
+  <si>
+    <t>createSpaceTypes</t>
+  </si>
+  <si>
+    <t>createConstructionSet</t>
+  </si>
+  <si>
+    <t>ASHRAE 169-2006-5B</t>
+  </si>
+  <si>
+    <t>Create Space Types</t>
+  </si>
+  <si>
+    <t>Create Construction Set</t>
+  </si>
+  <si>
+    <t>Space Type And Construction Set Wizard</t>
+  </si>
+  <si>
     <t>OSM</t>
   </si>
   <si>
@@ -2032,6 +2071,9 @@
     <t>Weather File Name</t>
   </si>
   <si>
+    <t>Office</t>
+  </si>
+  <si>
     <t>ft</t>
   </si>
   <si>
@@ -2059,6 +2101,12 @@
     <t>../analysis</t>
   </si>
   <si>
+    <t>Rotate Building</t>
+  </si>
+  <si>
+    <t>DOE Ref 1980-2004</t>
+  </si>
+  <si>
     <t>calibration_reports.electric_bill_consumption_modeled</t>
   </si>
   <si>
@@ -2285,13 +2333,175 @@
   </si>
   <si>
     <t>cofee</t>
+  </si>
+  <si>
+    <t>AddPeopleToSpaceTypes</t>
+  </si>
+  <si>
+    <t>AddVentilationToSpaceTypes</t>
+  </si>
+  <si>
+    <t>AddInfiltrationToSpaceTypes</t>
+  </si>
+  <si>
+    <t>AddInternalMassToSpaceTypes</t>
+  </si>
+  <si>
+    <t>SurfaceMatching</t>
+  </si>
+  <si>
+    <t>AddThermostats</t>
+  </si>
+  <si>
+    <t>AddElevatorsToBuilding</t>
+  </si>
+  <si>
+    <t>AddLampsToSpacesBySpaceType</t>
+  </si>
+  <si>
+    <t>AddElecEquipToSpacesBySpaceType</t>
+  </si>
+  <si>
+    <t>AddGasEquipToSpacesBySpaceType</t>
+  </si>
+  <si>
+    <t>add_people_to_space_types</t>
+  </si>
+  <si>
+    <t>Add People to Space Types</t>
+  </si>
+  <si>
+    <t>multiplier_occ</t>
+  </si>
+  <si>
+    <t>Occupancy Multiplier</t>
+  </si>
+  <si>
+    <t>6 digit structure id</t>
+  </si>
+  <si>
+    <t>multiplier_ventilation</t>
+  </si>
+  <si>
+    <t>Ventilation Multiplier</t>
+  </si>
+  <si>
+    <t>Add Infiltration to Space Types</t>
+  </si>
+  <si>
+    <t>Add Ventilation to Space Types</t>
+  </si>
+  <si>
+    <t>add_infiltration_to_space_types</t>
+  </si>
+  <si>
+    <t>add_ventilation_to_space_types</t>
+  </si>
+  <si>
+    <t>add_internal_mass_to_space_types</t>
+  </si>
+  <si>
+    <t>add _thermostats</t>
+  </si>
+  <si>
+    <t>add_fenestration_and_overhangs_by_space_type</t>
+  </si>
+  <si>
+    <t>add_elevators_to_building</t>
+  </si>
+  <si>
+    <t>add_lamps_to_spaces_by_space_type</t>
+  </si>
+  <si>
+    <t>add_elec_equip_to_spaces_by_space_type</t>
+  </si>
+  <si>
+    <t>add_gas_equip_to_spaces_by_space_type</t>
+  </si>
+  <si>
+    <t>multiplier_infiltration</t>
+  </si>
+  <si>
+    <t>Infiltration Multiplier</t>
+  </si>
+  <si>
+    <t>Add Internal Mass to Space Types</t>
+  </si>
+  <si>
+    <t>multiplier_int_mass</t>
+  </si>
+  <si>
+    <t>Internal Mass Multiplier</t>
+  </si>
+  <si>
+    <t>Surface Matching</t>
+  </si>
+  <si>
+    <t>Add Thermostats</t>
+  </si>
+  <si>
+    <t>Hours of Operation Start</t>
+  </si>
+  <si>
+    <t>Hours of Operation Finish</t>
+  </si>
+  <si>
+    <t>hoo_start</t>
+  </si>
+  <si>
+    <t>hoo_finish</t>
+  </si>
+  <si>
+    <t>deg</t>
+  </si>
+  <si>
+    <t>Add Fenestration And Overhangs By SpaceType</t>
+  </si>
+  <si>
+    <t>AddFenestrationAndOverhangsBySpaceType</t>
+  </si>
+  <si>
+    <t>Add Elevators To Building</t>
+  </si>
+  <si>
+    <t>Elevator Efficiency Multiplier</t>
+  </si>
+  <si>
+    <t>multiplier_elevator_eff</t>
+  </si>
+  <si>
+    <t>Add Lamps to Spaces by Space Type</t>
+  </si>
+  <si>
+    <t>Lighting Multiplier</t>
+  </si>
+  <si>
+    <t>multiplier_lighting</t>
+  </si>
+  <si>
+    <t>multiplier_elec_equip</t>
+  </si>
+  <si>
+    <t>Electric Equipment Multiplier</t>
+  </si>
+  <si>
+    <t>Add Elec Equip to Spaces by Space Type</t>
+  </si>
+  <si>
+    <t>Add Gas Equip to Spaces by Space Type</t>
+  </si>
+  <si>
+    <t>multiplier_gas_equip</t>
+  </si>
+  <si>
+    <t>Gas Equipment Multiplier</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2355,6 +2565,13 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -4238,7 +4455,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -4334,6 +4551,9 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1801">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -6471,7 +6691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView topLeftCell="A21" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
@@ -6519,7 +6739,7 @@
         <v>456</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>649</v>
+        <v>662</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>457</v>
@@ -6530,7 +6750,7 @@
         <v>469</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>721</v>
+        <v>737</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>614</v>
@@ -6612,7 +6832,7 @@
         <v>39</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>670</v>
+        <v>684</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>471</v>
@@ -6623,10 +6843,10 @@
         <v>25</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>722</v>
+        <v>738</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>665</v>
+        <v>679</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -6634,10 +6854,10 @@
         <v>26</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>671</v>
+        <v>685</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>665</v>
+        <v>679</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -6702,7 +6922,7 @@
         <v>451</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>651</v>
+        <v>664</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -6791,7 +7011,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>664</v>
+        <v>678</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>31</v>
@@ -6804,7 +7024,7 @@
         <v>29</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>654</v>
+        <v>667</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -6818,7 +7038,7 @@
         <v>38</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>664</v>
+        <v>678</v>
       </c>
       <c r="E39" s="13" t="s">
         <v>449</v>
@@ -6829,10 +7049,10 @@
         <v>32</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>648</v>
+        <v>661</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>652</v>
+        <v>665</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>620</v>
@@ -6846,7 +7066,7 @@
         <v>34</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>669</v>
+        <v>683</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="13" t="s">
@@ -6855,13 +7075,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
-        <v>653</v>
+        <v>666</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>747</v>
+        <v>763</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>746</v>
+        <v>762</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -6892,11 +7112,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y162"/>
+  <dimension ref="A1:Y128"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7054,13 +7274,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>659</v>
+        <v>672</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>660</v>
+        <v>673</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>660</v>
+        <v>673</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>68</v>
@@ -7073,16 +7293,16 @@
         <v>21</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>666</v>
+        <v>680</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>667</v>
+        <v>681</v>
       </c>
       <c r="F5" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>668</v>
+        <v>682</v>
       </c>
     </row>
     <row r="6" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -7090,16 +7310,16 @@
         <v>21</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>662</v>
+        <v>675</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>661</v>
+        <v>674</v>
       </c>
       <c r="F6" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H6" s="31" t="s">
-        <v>745</v>
+        <v>761</v>
       </c>
     </row>
     <row r="7" spans="1:25" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -7107,13 +7327,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>725</v>
+        <v>741</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>724</v>
+        <v>740</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>723</v>
+        <v>739</v>
       </c>
       <c r="E7" s="37" t="s">
         <v>68</v>
@@ -7126,16 +7346,16 @@
         <v>21</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>729</v>
+        <v>745</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>726</v>
+        <v>742</v>
       </c>
       <c r="F8" s="31" t="s">
         <v>618</v>
       </c>
       <c r="H8" s="31" t="s">
-        <v>734</v>
+        <v>750</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
@@ -7151,10 +7371,10 @@
         <v>21</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>730</v>
+        <v>746</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>727</v>
+        <v>743</v>
       </c>
       <c r="F9" s="31" t="s">
         <v>619</v>
@@ -7174,10 +7394,10 @@
         <v>21</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>731</v>
+        <v>747</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>728</v>
+        <v>744</v>
       </c>
       <c r="F10" s="31" t="s">
         <v>622</v>
@@ -7192,13 +7412,13 @@
         <v>1</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>725</v>
+        <v>741</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>724</v>
+        <v>740</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>723</v>
+        <v>739</v>
       </c>
       <c r="E11" s="37" t="s">
         <v>68</v>
@@ -7211,16 +7431,16 @@
         <v>21</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>729</v>
+        <v>745</v>
       </c>
       <c r="E12" s="31" t="s">
-        <v>726</v>
+        <v>742</v>
       </c>
       <c r="F12" s="31" t="s">
         <v>618</v>
       </c>
       <c r="H12" s="31" t="s">
-        <v>732</v>
+        <v>748</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -7236,10 +7456,10 @@
         <v>21</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>730</v>
+        <v>746</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>727</v>
+        <v>743</v>
       </c>
       <c r="F13" s="31" t="s">
         <v>619</v>
@@ -7259,10 +7479,10 @@
         <v>21</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>731</v>
+        <v>747</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>728</v>
+        <v>744</v>
       </c>
       <c r="F14" s="31" t="s">
         <v>622</v>
@@ -7277,13 +7497,13 @@
         <v>1</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>725</v>
+        <v>741</v>
       </c>
       <c r="C15" s="37" t="s">
-        <v>724</v>
+        <v>740</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>723</v>
+        <v>739</v>
       </c>
       <c r="E15" s="37" t="s">
         <v>68</v>
@@ -7296,16 +7516,16 @@
         <v>21</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>729</v>
+        <v>745</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>726</v>
+        <v>742</v>
       </c>
       <c r="F16" s="31" t="s">
         <v>618</v>
       </c>
       <c r="H16" s="31" t="s">
-        <v>733</v>
+        <v>749</v>
       </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
@@ -7321,10 +7541,10 @@
         <v>21</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>730</v>
+        <v>746</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>727</v>
+        <v>743</v>
       </c>
       <c r="F17" s="31" t="s">
         <v>619</v>
@@ -7344,10 +7564,10 @@
         <v>21</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>731</v>
+        <v>747</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>728</v>
+        <v>744</v>
       </c>
       <c r="F18" s="31" t="s">
         <v>622</v>
@@ -7362,13 +7582,13 @@
         <v>1</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>737</v>
+        <v>753</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>735</v>
+        <v>751</v>
       </c>
       <c r="D19" s="37" t="s">
-        <v>736</v>
+        <v>752</v>
       </c>
       <c r="E19" s="37" t="s">
         <v>68</v>
@@ -7381,10 +7601,10 @@
         <v>21</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>738</v>
+        <v>778</v>
       </c>
       <c r="E20" s="31" t="s">
-        <v>738</v>
+        <v>754</v>
       </c>
       <c r="F20" s="31" t="s">
         <v>619</v>
@@ -7406,16 +7626,16 @@
         <v>21</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>740</v>
+        <v>756</v>
       </c>
       <c r="E21" s="31" t="s">
-        <v>739</v>
+        <v>755</v>
       </c>
       <c r="F21" s="31" t="s">
         <v>619</v>
       </c>
       <c r="G21" s="31" t="s">
-        <v>663</v>
+        <v>677</v>
       </c>
       <c r="H21" s="4">
         <v>10</v>
@@ -7432,16 +7652,16 @@
         <v>21</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>742</v>
+        <v>758</v>
       </c>
       <c r="E22" s="31" t="s">
-        <v>741</v>
+        <v>757</v>
       </c>
       <c r="F22" s="31" t="s">
         <v>619</v>
       </c>
       <c r="G22" s="31" t="s">
-        <v>663</v>
+        <v>677</v>
       </c>
       <c r="H22" s="4">
         <v>10</v>
@@ -7453,10 +7673,10 @@
         <v>21</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>744</v>
+        <v>760</v>
       </c>
       <c r="E23" s="31" t="s">
-        <v>743</v>
+        <v>759</v>
       </c>
       <c r="F23" s="31" t="s">
         <v>619</v>
@@ -7467,166 +7687,726 @@
       <c r="I23" s="31"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H24" s="31"/>
+      <c r="B24" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="49" t="s">
+        <v>799</v>
+      </c>
+      <c r="E24" s="49" t="s">
+        <v>801</v>
+      </c>
+      <c r="F24" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H24" s="4">
+        <v>8</v>
+      </c>
       <c r="I24" s="31"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H25" s="31"/>
+      <c r="B25" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="49" t="s">
+        <v>800</v>
+      </c>
+      <c r="E25" s="49" t="s">
+        <v>802</v>
+      </c>
+      <c r="F25" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H25" s="4">
+        <v>17</v>
+      </c>
       <c r="I25" s="31"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H26" s="31"/>
-      <c r="I26" s="31"/>
+    <row r="26" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B26" s="37" t="s">
+        <v>775</v>
+      </c>
+      <c r="C26" s="37" t="s">
+        <v>774</v>
+      </c>
+      <c r="D26" s="37" t="s">
+        <v>764</v>
+      </c>
+      <c r="E26" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
+      <c r="B27" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="31" t="s">
+        <v>777</v>
+      </c>
+      <c r="E27" s="31" t="s">
+        <v>776</v>
+      </c>
+      <c r="F27" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H27" s="31">
+        <v>1</v>
+      </c>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="P27" s="39"/>
+      <c r="Q27" s="2"/>
+    </row>
+    <row r="28" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B28" s="37" t="s">
+        <v>782</v>
+      </c>
+      <c r="C28" s="37" t="s">
+        <v>784</v>
+      </c>
+      <c r="D28" s="37" t="s">
+        <v>765</v>
+      </c>
+      <c r="E28" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
+      <c r="B29" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="31" t="s">
+        <v>780</v>
+      </c>
+      <c r="E29" s="31" t="s">
+        <v>779</v>
+      </c>
+      <c r="F29" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H29" s="31">
+        <v>1</v>
+      </c>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="P29" s="39"/>
+      <c r="Q29" s="2"/>
+    </row>
+    <row r="30" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B30" s="37" t="s">
+        <v>781</v>
+      </c>
+      <c r="C30" s="37" t="s">
+        <v>783</v>
+      </c>
+      <c r="D30" s="37" t="s">
+        <v>766</v>
+      </c>
+      <c r="E30" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
-    </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H33" s="31"/>
-      <c r="I33" s="31"/>
-    </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H34" s="31"/>
-      <c r="I34" s="31"/>
-    </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H35" s="31"/>
-      <c r="I35" s="31"/>
-    </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H36" s="31"/>
-      <c r="I36" s="31"/>
-    </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H37" s="31"/>
+      <c r="B31" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="31" t="s">
+        <v>793</v>
+      </c>
+      <c r="E31" s="31" t="s">
+        <v>792</v>
+      </c>
+      <c r="F31" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H31" s="31">
+        <v>1</v>
+      </c>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="P31" s="39"/>
+      <c r="Q31" s="2"/>
+    </row>
+    <row r="32" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B32" s="37" t="s">
+        <v>794</v>
+      </c>
+      <c r="C32" s="37" t="s">
+        <v>785</v>
+      </c>
+      <c r="D32" s="37" t="s">
+        <v>767</v>
+      </c>
+      <c r="E32" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B33" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="31" t="s">
+        <v>796</v>
+      </c>
+      <c r="E33" s="31" t="s">
+        <v>795</v>
+      </c>
+      <c r="F33" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H33" s="31">
+        <v>1</v>
+      </c>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="P33" s="39"/>
+      <c r="Q33" s="2"/>
+    </row>
+    <row r="34" spans="1:17" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="47" t="b">
+        <v>1</v>
+      </c>
+      <c r="B34" s="47" t="s">
+        <v>660</v>
+      </c>
+      <c r="C34" s="47" t="s">
+        <v>648</v>
+      </c>
+      <c r="D34" s="47" t="s">
+        <v>648</v>
+      </c>
+      <c r="E34" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="G34" s="48"/>
+      <c r="H34" s="48"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B35" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="31" t="s">
+        <v>650</v>
+      </c>
+      <c r="E35" s="31" t="s">
+        <v>649</v>
+      </c>
+      <c r="F35" s="31" t="s">
+        <v>618</v>
+      </c>
+      <c r="H35" s="31" t="s">
+        <v>676</v>
+      </c>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="P35" s="39"/>
+      <c r="Q35" s="2"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B36" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" s="31" t="s">
+        <v>651</v>
+      </c>
+      <c r="E36" s="31" t="s">
+        <v>652</v>
+      </c>
+      <c r="F36" s="31" t="s">
+        <v>618</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>687</v>
+      </c>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="3"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B37" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="31" t="s">
+        <v>653</v>
+      </c>
+      <c r="E37" s="31" t="s">
+        <v>654</v>
+      </c>
+      <c r="F37" s="31" t="s">
+        <v>618</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>657</v>
+      </c>
       <c r="I37" s="31"/>
     </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H38" s="31"/>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B38" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" s="31" t="s">
+        <v>658</v>
+      </c>
+      <c r="E38" s="31" t="s">
+        <v>655</v>
+      </c>
+      <c r="F38" s="31" t="s">
+        <v>622</v>
+      </c>
+      <c r="H38" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="I38" s="31"/>
     </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H39" s="31"/>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B39" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" s="31" t="s">
+        <v>659</v>
+      </c>
+      <c r="E39" s="31" t="s">
+        <v>656</v>
+      </c>
+      <c r="F39" s="31" t="s">
+        <v>622</v>
+      </c>
+      <c r="H39" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="I39" s="31"/>
     </row>
-    <row r="40" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H40" s="31"/>
-      <c r="I40" s="31"/>
-    </row>
-    <row r="41" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H41" s="31"/>
-      <c r="I41" s="31"/>
-    </row>
-    <row r="42" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H42" s="31"/>
-      <c r="I42" s="31"/>
-    </row>
-    <row r="43" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H43" s="31"/>
-      <c r="I43" s="31"/>
-    </row>
-    <row r="44" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H44" s="31"/>
-      <c r="I44" s="31"/>
-    </row>
-    <row r="45" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H45" s="31"/>
-      <c r="I45" s="31"/>
-    </row>
-    <row r="46" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H46" s="31"/>
-      <c r="I46" s="31"/>
-    </row>
-    <row r="47" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H47" s="31"/>
-      <c r="I47" s="31"/>
-    </row>
-    <row r="48" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H48" s="31"/>
-      <c r="I48" s="31"/>
-    </row>
-    <row r="49" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H49" s="31"/>
-      <c r="I49" s="31"/>
-    </row>
-    <row r="50" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H50" s="31"/>
-      <c r="I50" s="31"/>
-    </row>
-    <row r="51" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H51" s="31"/>
-      <c r="I51" s="31"/>
-    </row>
-    <row r="52" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H52" s="31"/>
-      <c r="I52" s="31"/>
-    </row>
-    <row r="53" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H53" s="31"/>
-      <c r="I53" s="31"/>
-    </row>
-    <row r="54" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H54" s="31"/>
-      <c r="I54" s="31"/>
-    </row>
-    <row r="55" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H55" s="31"/>
-      <c r="I55" s="31"/>
-    </row>
-    <row r="56" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B40" s="37" t="s">
+        <v>797</v>
+      </c>
+      <c r="C40" s="37" t="s">
+        <v>768</v>
+      </c>
+      <c r="D40" s="37" t="s">
+        <v>768</v>
+      </c>
+      <c r="E40" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G40" s="38"/>
+      <c r="H40" s="38"/>
+    </row>
+    <row r="41" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B41" s="37" t="s">
+        <v>798</v>
+      </c>
+      <c r="C41" s="37" t="s">
+        <v>786</v>
+      </c>
+      <c r="D41" s="37" t="s">
+        <v>769</v>
+      </c>
+      <c r="E41" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+    </row>
+    <row r="42" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B42" s="37" t="s">
+        <v>686</v>
+      </c>
+      <c r="C42" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="D42" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="E42" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G42" s="38"/>
+      <c r="H42" s="38"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B43" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D43" s="31" t="s">
+        <v>341</v>
+      </c>
+      <c r="E43" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="F43" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="G43" s="31" t="s">
+        <v>803</v>
+      </c>
+      <c r="H43" s="31">
+        <v>0</v>
+      </c>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="P43" s="39"/>
+      <c r="Q43" s="2"/>
+    </row>
+    <row r="44" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B44" s="37" t="s">
+        <v>804</v>
+      </c>
+      <c r="C44" s="37" t="s">
+        <v>787</v>
+      </c>
+      <c r="D44" s="37" t="s">
+        <v>805</v>
+      </c>
+      <c r="E44" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+    </row>
+    <row r="45" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B45" s="37" t="s">
+        <v>806</v>
+      </c>
+      <c r="C45" s="37" t="s">
+        <v>788</v>
+      </c>
+      <c r="D45" s="37" t="s">
+        <v>770</v>
+      </c>
+      <c r="E45" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G45" s="38"/>
+      <c r="H45" s="38"/>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B46" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" s="31" t="s">
+        <v>807</v>
+      </c>
+      <c r="E46" s="31" t="s">
+        <v>808</v>
+      </c>
+      <c r="F46" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H46" s="31">
+        <v>1</v>
+      </c>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="3"/>
+      <c r="N46" s="3"/>
+      <c r="P46" s="39"/>
+      <c r="Q46" s="2"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B47" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D47" s="31" t="s">
+        <v>754</v>
+      </c>
+      <c r="E47" s="31" t="s">
+        <v>754</v>
+      </c>
+      <c r="F47" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H47" s="31">
+        <v>999999</v>
+      </c>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
+      <c r="P47" s="39"/>
+      <c r="Q47" s="2"/>
+    </row>
+    <row r="48" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B48" s="37" t="s">
+        <v>809</v>
+      </c>
+      <c r="C48" s="37" t="s">
+        <v>789</v>
+      </c>
+      <c r="D48" s="37" t="s">
+        <v>771</v>
+      </c>
+      <c r="E48" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G48" s="38"/>
+      <c r="H48" s="38"/>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B49" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D49" s="31" t="s">
+        <v>810</v>
+      </c>
+      <c r="E49" s="31" t="s">
+        <v>811</v>
+      </c>
+      <c r="F49" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H49" s="31">
+        <v>1</v>
+      </c>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
+      <c r="N49" s="3"/>
+      <c r="P49" s="39"/>
+      <c r="Q49" s="2"/>
+    </row>
+    <row r="50" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B50" s="37" t="s">
+        <v>814</v>
+      </c>
+      <c r="C50" s="37" t="s">
+        <v>790</v>
+      </c>
+      <c r="D50" s="37" t="s">
+        <v>772</v>
+      </c>
+      <c r="E50" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G50" s="38"/>
+      <c r="H50" s="38"/>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B51" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D51" s="31" t="s">
+        <v>813</v>
+      </c>
+      <c r="E51" s="31" t="s">
+        <v>812</v>
+      </c>
+      <c r="F51" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H51" s="31">
+        <v>1</v>
+      </c>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="3"/>
+      <c r="P51" s="39"/>
+      <c r="Q51" s="2"/>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B52" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D52" s="31" t="s">
+        <v>754</v>
+      </c>
+      <c r="E52" s="31" t="s">
+        <v>754</v>
+      </c>
+      <c r="F52" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H52" s="31">
+        <v>999999</v>
+      </c>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
+      <c r="N52" s="3"/>
+      <c r="P52" s="39"/>
+      <c r="Q52" s="2"/>
+    </row>
+    <row r="53" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B53" s="37" t="s">
+        <v>815</v>
+      </c>
+      <c r="C53" s="37" t="s">
+        <v>791</v>
+      </c>
+      <c r="D53" s="37" t="s">
+        <v>773</v>
+      </c>
+      <c r="E53" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G53" s="38"/>
+      <c r="H53" s="38"/>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B54" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D54" s="31" t="s">
+        <v>817</v>
+      </c>
+      <c r="E54" s="31" t="s">
+        <v>816</v>
+      </c>
+      <c r="F54" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H54" s="31">
+        <v>1</v>
+      </c>
+      <c r="I54" s="3"/>
+      <c r="J54" s="3"/>
+      <c r="K54" s="3"/>
+      <c r="L54" s="3"/>
+      <c r="M54" s="3"/>
+      <c r="N54" s="3"/>
+      <c r="P54" s="39"/>
+      <c r="Q54" s="2"/>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B55" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D55" s="31" t="s">
+        <v>754</v>
+      </c>
+      <c r="E55" s="31" t="s">
+        <v>754</v>
+      </c>
+      <c r="F55" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H55" s="31">
+        <v>999999</v>
+      </c>
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="3"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3"/>
+      <c r="N55" s="3"/>
+      <c r="P55" s="39"/>
+      <c r="Q55" s="2"/>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H56" s="31"/>
       <c r="I56" s="31"/>
     </row>
-    <row r="57" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H57" s="31"/>
       <c r="I57" s="31"/>
     </row>
-    <row r="58" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H58" s="31"/>
       <c r="I58" s="31"/>
     </row>
-    <row r="59" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H59" s="31"/>
       <c r="I59" s="31"/>
     </row>
-    <row r="60" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H60" s="31"/>
       <c r="I60" s="31"/>
     </row>
-    <row r="61" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H61" s="31"/>
       <c r="I61" s="31"/>
     </row>
-    <row r="62" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H62" s="31"/>
       <c r="I62" s="31"/>
     </row>
-    <row r="63" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H63" s="31"/>
       <c r="I63" s="31"/>
     </row>
-    <row r="64" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H64" s="31"/>
       <c r="I64" s="31"/>
     </row>
@@ -7886,149 +8666,13 @@
       <c r="H128" s="31"/>
       <c r="I128" s="31"/>
     </row>
-    <row r="129" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H129" s="31"/>
-      <c r="I129" s="31"/>
-    </row>
-    <row r="130" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H130" s="31"/>
-      <c r="I130" s="31"/>
-    </row>
-    <row r="131" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H131" s="31"/>
-      <c r="I131" s="31"/>
-    </row>
-    <row r="132" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H132" s="31"/>
-      <c r="I132" s="31"/>
-    </row>
-    <row r="133" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H133" s="31"/>
-      <c r="I133" s="31"/>
-    </row>
-    <row r="134" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H134" s="31"/>
-      <c r="I134" s="31"/>
-    </row>
-    <row r="135" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H135" s="31"/>
-      <c r="I135" s="31"/>
-    </row>
-    <row r="136" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H136" s="31"/>
-      <c r="I136" s="31"/>
-    </row>
-    <row r="137" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H137" s="31"/>
-      <c r="I137" s="31"/>
-    </row>
-    <row r="138" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H138" s="31"/>
-      <c r="I138" s="31"/>
-    </row>
-    <row r="139" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H139" s="31"/>
-      <c r="I139" s="31"/>
-    </row>
-    <row r="140" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H140" s="31"/>
-      <c r="I140" s="31"/>
-    </row>
-    <row r="141" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H141" s="31"/>
-      <c r="I141" s="31"/>
-    </row>
-    <row r="142" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H142" s="31"/>
-      <c r="I142" s="31"/>
-    </row>
-    <row r="143" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H143" s="31"/>
-      <c r="I143" s="31"/>
-    </row>
-    <row r="144" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H144" s="31"/>
-      <c r="I144" s="31"/>
-    </row>
-    <row r="145" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H145" s="31"/>
-      <c r="I145" s="31"/>
-    </row>
-    <row r="146" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H146" s="31"/>
-      <c r="I146" s="31"/>
-    </row>
-    <row r="147" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H147" s="31"/>
-      <c r="I147" s="31"/>
-    </row>
-    <row r="148" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H148" s="31"/>
-      <c r="I148" s="31"/>
-    </row>
-    <row r="149" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H149" s="31"/>
-      <c r="I149" s="31"/>
-    </row>
-    <row r="150" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H150" s="31"/>
-      <c r="I150" s="31"/>
-    </row>
-    <row r="151" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H151" s="31"/>
-      <c r="I151" s="31"/>
-    </row>
-    <row r="152" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H152" s="31"/>
-      <c r="I152" s="31"/>
-    </row>
-    <row r="153" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H153" s="31"/>
-      <c r="I153" s="31"/>
-    </row>
-    <row r="154" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H154" s="31"/>
-      <c r="I154" s="31"/>
-    </row>
-    <row r="155" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H155" s="31"/>
-      <c r="I155" s="31"/>
-    </row>
-    <row r="156" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H156" s="31"/>
-      <c r="I156" s="31"/>
-    </row>
-    <row r="157" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H157" s="31"/>
-      <c r="I157" s="31"/>
-    </row>
-    <row r="158" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H158" s="31"/>
-      <c r="I158" s="31"/>
-    </row>
-    <row r="159" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H159" s="31"/>
-      <c r="I159" s="31"/>
-    </row>
-    <row r="160" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H160" s="31"/>
-      <c r="I160" s="31"/>
-    </row>
-    <row r="161" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H161" s="31"/>
-      <c r="I161" s="31"/>
-    </row>
-    <row r="162" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H162" s="31"/>
-      <c r="I162" s="31"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A2:Z89"/>
+  <autoFilter ref="A2:Z55"/>
   <mergeCells count="1">
     <mergeCell ref="T1:Y1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -8269,11 +8913,11 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="40" t="s">
-        <v>689</v>
+        <v>705</v>
       </c>
       <c r="B8" s="40"/>
       <c r="C8" s="40" t="s">
-        <v>690</v>
+        <v>706</v>
       </c>
       <c r="D8" s="40" t="s">
         <v>468</v>
@@ -8297,11 +8941,11 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="40" t="s">
-        <v>691</v>
+        <v>707</v>
       </c>
       <c r="B9" s="40"/>
       <c r="C9" s="40" t="s">
-        <v>692</v>
+        <v>708</v>
       </c>
       <c r="D9" s="40" t="s">
         <v>468</v>
@@ -8325,11 +8969,11 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="40" t="s">
-        <v>693</v>
+        <v>709</v>
       </c>
       <c r="B10" s="40"/>
       <c r="C10" s="40" t="s">
-        <v>694</v>
+        <v>710</v>
       </c>
       <c r="D10" s="40" t="s">
         <v>468</v>
@@ -8353,11 +8997,11 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
-        <v>695</v>
+        <v>711</v>
       </c>
       <c r="B11" s="40"/>
       <c r="C11" s="40" t="s">
-        <v>696</v>
+        <v>712</v>
       </c>
       <c r="D11" s="40" t="s">
         <v>468</v>
@@ -8381,11 +9025,11 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
-        <v>697</v>
+        <v>713</v>
       </c>
       <c r="B12" s="40"/>
       <c r="C12" s="40" t="s">
-        <v>698</v>
+        <v>714</v>
       </c>
       <c r="D12" s="40" t="s">
         <v>468</v>
@@ -8409,11 +9053,11 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="40" t="s">
-        <v>699</v>
+        <v>715</v>
       </c>
       <c r="B13" s="40"/>
       <c r="C13" s="40" t="s">
-        <v>700</v>
+        <v>716</v>
       </c>
       <c r="D13" s="40" t="s">
         <v>468</v>
@@ -8437,11 +9081,11 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="40" t="s">
-        <v>701</v>
+        <v>717</v>
       </c>
       <c r="B14" s="40"/>
       <c r="C14" s="40" t="s">
-        <v>702</v>
+        <v>718</v>
       </c>
       <c r="D14" s="40" t="s">
         <v>468</v>
@@ -8465,11 +9109,11 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="40" t="s">
-        <v>703</v>
+        <v>719</v>
       </c>
       <c r="B15" s="40"/>
       <c r="C15" s="40" t="s">
-        <v>704</v>
+        <v>720</v>
       </c>
       <c r="D15" s="40" t="s">
         <v>468</v>
@@ -8493,11 +9137,11 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="40" t="s">
-        <v>705</v>
+        <v>721</v>
       </c>
       <c r="B16" s="40"/>
       <c r="C16" s="40" t="s">
-        <v>706</v>
+        <v>722</v>
       </c>
       <c r="D16" s="40" t="s">
         <v>468</v>
@@ -8521,11 +9165,11 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="40" t="s">
-        <v>707</v>
+        <v>723</v>
       </c>
       <c r="B17" s="40"/>
       <c r="C17" s="40" t="s">
-        <v>708</v>
+        <v>724</v>
       </c>
       <c r="D17" s="40" t="s">
         <v>468</v>
@@ -8549,11 +9193,11 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="40" t="s">
-        <v>709</v>
+        <v>725</v>
       </c>
       <c r="B18" s="40"/>
       <c r="C18" s="40" t="s">
-        <v>710</v>
+        <v>726</v>
       </c>
       <c r="D18" s="40" t="s">
         <v>468</v>
@@ -8577,11 +9221,11 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="40" t="s">
-        <v>711</v>
+        <v>727</v>
       </c>
       <c r="B19" s="40"/>
       <c r="C19" s="40" t="s">
-        <v>712</v>
+        <v>728</v>
       </c>
       <c r="D19" s="40" t="s">
         <v>468</v>
@@ -8605,11 +9249,11 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="40" t="s">
-        <v>713</v>
+        <v>729</v>
       </c>
       <c r="B20" s="40"/>
       <c r="C20" s="40" t="s">
-        <v>714</v>
+        <v>730</v>
       </c>
       <c r="D20" s="40" t="s">
         <v>468</v>
@@ -8633,11 +9277,11 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="40" t="s">
-        <v>715</v>
+        <v>731</v>
       </c>
       <c r="B21" s="40"/>
       <c r="C21" s="40" t="s">
-        <v>716</v>
+        <v>732</v>
       </c>
       <c r="D21" s="40" t="s">
         <v>468</v>
@@ -8661,14 +9305,14 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="40" t="s">
-        <v>683</v>
+        <v>699</v>
       </c>
       <c r="B22" s="40"/>
       <c r="C22" s="40" t="s">
-        <v>717</v>
+        <v>733</v>
       </c>
       <c r="D22" s="40" t="s">
-        <v>684</v>
+        <v>700</v>
       </c>
       <c r="E22" s="40" t="s">
         <v>64</v>
@@ -8689,14 +9333,14 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="40" t="s">
-        <v>685</v>
+        <v>701</v>
       </c>
       <c r="B23" s="40"/>
       <c r="C23" s="40" t="s">
-        <v>718</v>
+        <v>734</v>
       </c>
       <c r="D23" s="40" t="s">
-        <v>684</v>
+        <v>700</v>
       </c>
       <c r="E23" s="40" t="s">
         <v>64</v>
@@ -8717,14 +9361,14 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="40" t="s">
-        <v>686</v>
+        <v>702</v>
       </c>
       <c r="B24" s="40"/>
       <c r="C24" s="40" t="s">
-        <v>719</v>
+        <v>735</v>
       </c>
       <c r="D24" s="40" t="s">
-        <v>684</v>
+        <v>700</v>
       </c>
       <c r="E24" s="40" t="s">
         <v>64</v>
@@ -8745,14 +9389,14 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="40" t="s">
-        <v>687</v>
+        <v>703</v>
       </c>
       <c r="B25" s="40"/>
       <c r="C25" s="40" t="s">
-        <v>720</v>
+        <v>736</v>
       </c>
       <c r="D25" s="40" t="s">
-        <v>688</v>
+        <v>704</v>
       </c>
       <c r="E25" s="40" t="s">
         <v>64</v>
@@ -8773,14 +9417,14 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="40" t="s">
-        <v>655</v>
+        <v>668</v>
       </c>
       <c r="B26" s="40"/>
       <c r="C26" s="40" t="s">
-        <v>672</v>
+        <v>688</v>
       </c>
       <c r="D26" s="40" t="s">
-        <v>656</v>
+        <v>669</v>
       </c>
       <c r="E26" s="40" t="s">
         <v>64</v>
@@ -8801,14 +9445,14 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="40" t="s">
-        <v>657</v>
+        <v>670</v>
       </c>
       <c r="B27" s="40"/>
       <c r="C27" s="40" t="s">
-        <v>673</v>
+        <v>689</v>
       </c>
       <c r="D27" s="40" t="s">
-        <v>658</v>
+        <v>671</v>
       </c>
       <c r="E27" s="40" t="s">
         <v>64</v>
@@ -8829,14 +9473,14 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="40" t="s">
-        <v>679</v>
+        <v>695</v>
       </c>
       <c r="B28" s="40"/>
       <c r="C28" s="40" t="s">
-        <v>674</v>
+        <v>690</v>
       </c>
       <c r="D28" s="40" t="s">
-        <v>675</v>
+        <v>691</v>
       </c>
       <c r="E28" s="40" t="s">
         <v>64</v>
@@ -8859,14 +9503,14 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="40" t="s">
-        <v>680</v>
+        <v>696</v>
       </c>
       <c r="B29" s="40"/>
       <c r="C29" s="40" t="s">
-        <v>676</v>
+        <v>692</v>
       </c>
       <c r="D29" s="40" t="s">
-        <v>675</v>
+        <v>691</v>
       </c>
       <c r="E29" s="40" t="s">
         <v>64</v>
@@ -8889,14 +9533,14 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="40" t="s">
-        <v>681</v>
+        <v>697</v>
       </c>
       <c r="B30" s="40"/>
       <c r="C30" s="40" t="s">
-        <v>677</v>
+        <v>693</v>
       </c>
       <c r="D30" s="40" t="s">
-        <v>675</v>
+        <v>691</v>
       </c>
       <c r="E30" s="40" t="s">
         <v>64</v>
@@ -8919,14 +9563,14 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="40" t="s">
-        <v>682</v>
+        <v>698</v>
       </c>
       <c r="B31" s="40"/>
       <c r="C31" s="40" t="s">
-        <v>678</v>
+        <v>694</v>
       </c>
       <c r="D31" s="40" t="s">
-        <v>675</v>
+        <v>691</v>
       </c>
       <c r="E31" s="40" t="s">
         <v>64</v>
@@ -17622,7 +18266,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>650</v>
+        <v>663</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>557</v>

</xml_diff>

<commit_message>
removing structure ID from all but one measure
it is now saved as building name, in similar fashion to how hours of
operation are saved as a schedule set at the building level.
</commit_message>
<xml_diff>
--- a/projects/m0.xlsx
+++ b/projects/m0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="600" windowWidth="25125" windowHeight="15465" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="600" windowWidth="25125" windowHeight="12810" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$52</definedName>
     <definedName name="AnalysisType">Lookups!$A$17:$A$23</definedName>
     <definedName name="instance_defs">Lookups!$A$2:$D$9</definedName>
     <definedName name="instance_types">Lookups!$A$2:$A$9</definedName>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2363" uniqueCount="818">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2351" uniqueCount="818">
   <si>
     <t>type</t>
   </si>
@@ -4465,7 +4465,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -4564,7 +4564,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1801">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -7123,11 +7122,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y128"/>
+  <dimension ref="A1:Y125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C59" sqref="C59"/>
+      <pane ySplit="3" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8178,134 +8177,128 @@
       <c r="P46" s="39"/>
       <c r="Q46" s="2"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B47" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D47" s="50" t="s">
-        <v>754</v>
-      </c>
-      <c r="E47" s="31" t="s">
-        <v>754</v>
-      </c>
-      <c r="F47" s="31" t="s">
+    <row r="47" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B47" s="37" t="s">
+        <v>809</v>
+      </c>
+      <c r="C47" s="37" t="s">
+        <v>789</v>
+      </c>
+      <c r="D47" s="37" t="s">
+        <v>771</v>
+      </c>
+      <c r="E47" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G47" s="38"/>
+      <c r="H47" s="38"/>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B48" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" s="31" t="s">
+        <v>810</v>
+      </c>
+      <c r="E48" s="31" t="s">
+        <v>811</v>
+      </c>
+      <c r="F48" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="H47" s="31">
-        <v>999999</v>
-      </c>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
-      <c r="L47" s="3"/>
-      <c r="M47" s="3"/>
-      <c r="N47" s="3"/>
-      <c r="P47" s="39"/>
-      <c r="Q47" s="2"/>
-    </row>
-    <row r="48" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="37" t="b">
+      <c r="H48" s="31">
         <v>1</v>
       </c>
-      <c r="B48" s="37" t="s">
-        <v>809</v>
-      </c>
-      <c r="C48" s="37" t="s">
-        <v>789</v>
-      </c>
-      <c r="D48" s="37" t="s">
-        <v>771</v>
-      </c>
-      <c r="E48" s="37" t="s">
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+      <c r="M48" s="3"/>
+      <c r="N48" s="3"/>
+      <c r="P48" s="39"/>
+      <c r="Q48" s="2"/>
+    </row>
+    <row r="49" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B49" s="37" t="s">
+        <v>814</v>
+      </c>
+      <c r="C49" s="37" t="s">
+        <v>790</v>
+      </c>
+      <c r="D49" s="37" t="s">
+        <v>772</v>
+      </c>
+      <c r="E49" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G48" s="38"/>
-      <c r="H48" s="38"/>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B49" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D49" s="31" t="s">
-        <v>810</v>
-      </c>
-      <c r="E49" s="31" t="s">
-        <v>811</v>
-      </c>
-      <c r="F49" s="31" t="s">
+      <c r="G49" s="38"/>
+      <c r="H49" s="38"/>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B50" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D50" s="31" t="s">
+        <v>813</v>
+      </c>
+      <c r="E50" s="31" t="s">
+        <v>812</v>
+      </c>
+      <c r="F50" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="H49" s="31">
+      <c r="H50" s="31">
         <v>1</v>
       </c>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
-      <c r="L49" s="3"/>
-      <c r="M49" s="3"/>
-      <c r="N49" s="3"/>
-      <c r="P49" s="39"/>
-      <c r="Q49" s="2"/>
-    </row>
-    <row r="50" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="37" t="b">
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="3"/>
+      <c r="L50" s="3"/>
+      <c r="M50" s="3"/>
+      <c r="N50" s="3"/>
+      <c r="P50" s="39"/>
+      <c r="Q50" s="2"/>
+    </row>
+    <row r="51" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B50" s="37" t="s">
-        <v>814</v>
-      </c>
-      <c r="C50" s="37" t="s">
-        <v>790</v>
-      </c>
-      <c r="D50" s="37" t="s">
-        <v>772</v>
-      </c>
-      <c r="E50" s="37" t="s">
+      <c r="B51" s="37" t="s">
+        <v>815</v>
+      </c>
+      <c r="C51" s="37" t="s">
+        <v>791</v>
+      </c>
+      <c r="D51" s="37" t="s">
+        <v>773</v>
+      </c>
+      <c r="E51" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G50" s="38"/>
-      <c r="H50" s="38"/>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B51" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D51" s="31" t="s">
-        <v>813</v>
-      </c>
-      <c r="E51" s="31" t="s">
-        <v>812</v>
-      </c>
-      <c r="F51" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="H51" s="31">
-        <v>1</v>
-      </c>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
-      <c r="L51" s="3"/>
-      <c r="M51" s="3"/>
-      <c r="N51" s="3"/>
-      <c r="P51" s="39"/>
-      <c r="Q51" s="2"/>
+      <c r="G51" s="38"/>
+      <c r="H51" s="38"/>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B52" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="D52" s="50" t="s">
-        <v>754</v>
+      <c r="D52" s="31" t="s">
+        <v>817</v>
       </c>
       <c r="E52" s="31" t="s">
-        <v>754</v>
+        <v>816</v>
       </c>
       <c r="F52" s="31" t="s">
         <v>619</v>
       </c>
       <c r="H52" s="31">
-        <v>999999</v>
+        <v>1</v>
       </c>
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
@@ -8316,74 +8309,17 @@
       <c r="P52" s="39"/>
       <c r="Q52" s="2"/>
     </row>
-    <row r="53" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="B53" s="37" t="s">
-        <v>815</v>
-      </c>
-      <c r="C53" s="37" t="s">
-        <v>791</v>
-      </c>
-      <c r="D53" s="37" t="s">
-        <v>773</v>
-      </c>
-      <c r="E53" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G53" s="38"/>
-      <c r="H53" s="38"/>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H53" s="31"/>
+      <c r="I53" s="31"/>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B54" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D54" s="31" t="s">
-        <v>817</v>
-      </c>
-      <c r="E54" s="31" t="s">
-        <v>816</v>
-      </c>
-      <c r="F54" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="H54" s="31">
-        <v>1</v>
-      </c>
-      <c r="I54" s="3"/>
-      <c r="J54" s="3"/>
-      <c r="K54" s="3"/>
-      <c r="L54" s="3"/>
-      <c r="M54" s="3"/>
-      <c r="N54" s="3"/>
-      <c r="P54" s="39"/>
-      <c r="Q54" s="2"/>
+      <c r="H54" s="31"/>
+      <c r="I54" s="31"/>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B55" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D55" s="50" t="s">
-        <v>754</v>
-      </c>
-      <c r="E55" s="31" t="s">
-        <v>754</v>
-      </c>
-      <c r="F55" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="H55" s="31">
-        <v>999999</v>
-      </c>
-      <c r="I55" s="3"/>
-      <c r="J55" s="3"/>
-      <c r="K55" s="3"/>
-      <c r="L55" s="3"/>
-      <c r="M55" s="3"/>
-      <c r="N55" s="3"/>
-      <c r="P55" s="39"/>
-      <c r="Q55" s="2"/>
+      <c r="H55" s="31"/>
+      <c r="I55" s="31"/>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H56" s="31"/>
@@ -8665,20 +8601,8 @@
       <c r="H125" s="31"/>
       <c r="I125" s="31"/>
     </row>
-    <row r="126" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H126" s="31"/>
-      <c r="I126" s="31"/>
-    </row>
-    <row r="127" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H127" s="31"/>
-      <c r="I127" s="31"/>
-    </row>
-    <row r="128" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H128" s="31"/>
-      <c r="I128" s="31"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A2:Z55"/>
+  <autoFilter ref="A2:Z52"/>
   <mergeCells count="1">
     <mergeCell ref="T1:Y1"/>
   </mergeCells>

</xml_diff>

<commit_message>
Adding site loads (lighting) to spreadsheet
</commit_message>
<xml_diff>
--- a/projects/m0.xlsx
+++ b/projects/m0.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2351" uniqueCount="822">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2363" uniqueCount="829">
   <si>
     <t>type</t>
   </si>
@@ -2368,9 +2368,6 @@
     <t>Occupancy Multiplier</t>
   </si>
   <si>
-    <t>6 digit structure id</t>
-  </si>
-  <si>
     <t>multiplier_ventilation</t>
   </si>
   <si>
@@ -2507,6 +2504,30 @@
   </si>
   <si>
     <t>MidriseApartment</t>
+  </si>
+  <si>
+    <t>Six digit structure id</t>
+  </si>
+  <si>
+    <t>Add Site Loads to Building</t>
+  </si>
+  <si>
+    <t>AddSiteLoadsToBuilding</t>
+  </si>
+  <si>
+    <t>add_site_loads_to_building</t>
+  </si>
+  <si>
+    <t>multiplier_site_perim_lighting</t>
+  </si>
+  <si>
+    <t>multiplier_site_parking_lighting</t>
+  </si>
+  <si>
+    <t>Site Perimeter Lighting Multiplier</t>
+  </si>
+  <si>
+    <t>Site Parking Lighting Multiplier</t>
   </si>
 </sst>
 </file>
@@ -7136,9 +7157,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7349,7 +7370,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="C7" s="37" t="s">
         <v>739</v>
@@ -7416,7 +7437,7 @@
         <v>21</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E10" s="31" t="s">
         <v>742</v>
@@ -7434,7 +7455,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C11" s="37" t="s">
         <v>739</v>
@@ -7501,7 +7522,7 @@
         <v>21</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E14" s="31" t="s">
         <v>742</v>
@@ -7519,7 +7540,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="C15" s="37" t="s">
         <v>739</v>
@@ -7586,7 +7607,7 @@
         <v>21</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E18" s="31" t="s">
         <v>742</v>
@@ -7623,7 +7644,7 @@
         <v>21</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>775</v>
+        <v>821</v>
       </c>
       <c r="E20" s="31" t="s">
         <v>751</v>
@@ -7713,10 +7734,10 @@
         <v>21</v>
       </c>
       <c r="D24" s="48" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E24" s="48" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F24" s="31" t="s">
         <v>619</v>
@@ -7731,10 +7752,10 @@
         <v>21</v>
       </c>
       <c r="D25" s="48" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E25" s="48" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="F25" s="31" t="s">
         <v>619</v>
@@ -7793,10 +7814,10 @@
         <v>1</v>
       </c>
       <c r="B28" s="37" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="C28" s="37" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="D28" s="37" t="s">
         <v>762</v>
@@ -7812,10 +7833,10 @@
         <v>21</v>
       </c>
       <c r="D29" s="31" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="E29" s="31" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="F29" s="31" t="s">
         <v>619</v>
@@ -7837,10 +7858,10 @@
         <v>1</v>
       </c>
       <c r="B30" s="37" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="C30" s="37" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="D30" s="37" t="s">
         <v>763</v>
@@ -7856,10 +7877,10 @@
         <v>21</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E31" s="31" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="F31" s="31" t="s">
         <v>619</v>
@@ -7881,10 +7902,10 @@
         <v>1</v>
       </c>
       <c r="B32" s="37" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="C32" s="37" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="D32" s="37" t="s">
         <v>764</v>
@@ -7900,10 +7921,10 @@
         <v>21</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="E33" s="31" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F33" s="31" t="s">
         <v>619</v>
@@ -7953,7 +7974,7 @@
         <v>618</v>
       </c>
       <c r="H35" s="31" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
@@ -8046,7 +8067,7 @@
         <v>1</v>
       </c>
       <c r="B40" s="37" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="C40" s="37" t="s">
         <v>765</v>
@@ -8065,10 +8086,10 @@
         <v>1</v>
       </c>
       <c r="B41" s="37" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C41" s="37" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="D41" s="37" t="s">
         <v>766</v>
@@ -8112,7 +8133,7 @@
         <v>619</v>
       </c>
       <c r="G43" s="31" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="H43" s="31">
         <v>0</v>
@@ -8131,13 +8152,13 @@
         <v>1</v>
       </c>
       <c r="B44" s="37" t="s">
+        <v>800</v>
+      </c>
+      <c r="C44" s="37" t="s">
+        <v>783</v>
+      </c>
+      <c r="D44" s="37" t="s">
         <v>801</v>
-      </c>
-      <c r="C44" s="37" t="s">
-        <v>784</v>
-      </c>
-      <c r="D44" s="37" t="s">
-        <v>802</v>
       </c>
       <c r="E44" s="37" t="s">
         <v>68</v>
@@ -8150,10 +8171,10 @@
         <v>1</v>
       </c>
       <c r="B45" s="37" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C45" s="37" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="D45" s="37" t="s">
         <v>767</v>
@@ -8169,10 +8190,10 @@
         <v>21</v>
       </c>
       <c r="D46" s="31" t="s">
+        <v>803</v>
+      </c>
+      <c r="E46" s="31" t="s">
         <v>804</v>
-      </c>
-      <c r="E46" s="31" t="s">
-        <v>805</v>
       </c>
       <c r="F46" s="31" t="s">
         <v>619</v>
@@ -8194,10 +8215,10 @@
         <v>1</v>
       </c>
       <c r="B47" s="37" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="C47" s="37" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="D47" s="37" t="s">
         <v>768</v>
@@ -8213,10 +8234,10 @@
         <v>21</v>
       </c>
       <c r="D48" s="31" t="s">
+        <v>806</v>
+      </c>
+      <c r="E48" s="31" t="s">
         <v>807</v>
-      </c>
-      <c r="E48" s="31" t="s">
-        <v>808</v>
       </c>
       <c r="F48" s="31" t="s">
         <v>619</v>
@@ -8238,10 +8259,10 @@
         <v>1</v>
       </c>
       <c r="B49" s="37" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="C49" s="37" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="D49" s="37" t="s">
         <v>769</v>
@@ -8257,10 +8278,10 @@
         <v>21</v>
       </c>
       <c r="D50" s="31" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="E50" s="31" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="F50" s="31" t="s">
         <v>619</v>
@@ -8282,10 +8303,10 @@
         <v>1</v>
       </c>
       <c r="B51" s="37" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="C51" s="37" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="D51" s="37" t="s">
         <v>770</v>
@@ -8301,10 +8322,10 @@
         <v>21</v>
       </c>
       <c r="D52" s="31" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E52" s="31" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="F52" s="31" t="s">
         <v>619</v>
@@ -8321,17 +8342,74 @@
       <c r="P52" s="39"/>
       <c r="Q52" s="2"/>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H53" s="31"/>
-      <c r="I53" s="31"/>
+    <row r="53" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B53" s="37" t="s">
+        <v>822</v>
+      </c>
+      <c r="C53" s="37" t="s">
+        <v>824</v>
+      </c>
+      <c r="D53" s="37" t="s">
+        <v>823</v>
+      </c>
+      <c r="E53" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G53" s="38"/>
+      <c r="H53" s="38"/>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H54" s="31"/>
-      <c r="I54" s="31"/>
+      <c r="B54" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D54" s="31" t="s">
+        <v>827</v>
+      </c>
+      <c r="E54" s="31" t="s">
+        <v>825</v>
+      </c>
+      <c r="F54" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H54" s="31">
+        <v>1</v>
+      </c>
+      <c r="I54" s="3"/>
+      <c r="J54" s="3"/>
+      <c r="K54" s="3"/>
+      <c r="L54" s="3"/>
+      <c r="M54" s="3"/>
+      <c r="N54" s="3"/>
+      <c r="P54" s="39"/>
+      <c r="Q54" s="2"/>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H55" s="31"/>
-      <c r="I55" s="31"/>
+      <c r="B55" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D55" s="31" t="s">
+        <v>828</v>
+      </c>
+      <c r="E55" s="31" t="s">
+        <v>826</v>
+      </c>
+      <c r="F55" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H55" s="31">
+        <v>1</v>
+      </c>
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="3"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3"/>
+      <c r="N55" s="3"/>
+      <c r="P55" s="39"/>
+      <c r="Q55" s="2"/>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H56" s="31"/>

</xml_diff>

<commit_message>
Adding exhaust fan measure to workflow
tested locally and through spreadsheet.
</commit_message>
<xml_diff>
--- a/projects/m0.xlsx
+++ b/projects/m0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="600" windowWidth="25125" windowHeight="12810" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="660" windowWidth="25125" windowHeight="12165" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2363" uniqueCount="829">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2371" uniqueCount="834">
   <si>
     <t>type</t>
   </si>
@@ -2528,6 +2528,21 @@
   </si>
   <si>
     <t>Site Parking Lighting Multiplier</t>
+  </si>
+  <si>
+    <t>Add Exhaust to Zones by Space Type</t>
+  </si>
+  <si>
+    <t>AddExhaustToZonesBySpaceType</t>
+  </si>
+  <si>
+    <t>add_exhaust_to_zones_by_space_type</t>
+  </si>
+  <si>
+    <t>exhaust_fan_eff</t>
+  </si>
+  <si>
+    <t>Exhaust Efficiency Multiplier</t>
   </si>
 </sst>
 </file>
@@ -4498,7 +4513,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -4594,6 +4609,8 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7155,11 +7172,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y125"/>
+  <dimension ref="A1:Y127"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D59" sqref="D59"/>
+      <pane ySplit="3" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7213,14 +7230,14 @@
       <c r="Q1" s="5"/>
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
-      <c r="T1" s="49" t="s">
+      <c r="T1" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="U1" s="49"/>
-      <c r="V1" s="49"/>
-      <c r="W1" s="49"/>
-      <c r="X1" s="49"/>
-      <c r="Y1" s="49"/>
+      <c r="U1" s="51"/>
+      <c r="V1" s="51"/>
+      <c r="W1" s="51"/>
+      <c r="X1" s="51"/>
+      <c r="Y1" s="51"/>
     </row>
     <row r="2" spans="1:25" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -7973,7 +7990,7 @@
       <c r="F35" s="31" t="s">
         <v>618</v>
       </c>
-      <c r="H35" s="31" t="s">
+      <c r="H35" s="49" t="s">
         <v>820</v>
       </c>
       <c r="I35" s="3"/>
@@ -7998,7 +8015,7 @@
       <c r="F36" s="31" t="s">
         <v>618</v>
       </c>
-      <c r="H36" s="4" t="s">
+      <c r="H36" s="50" t="s">
         <v>686</v>
       </c>
       <c r="I36" s="3"/>
@@ -8021,7 +8038,7 @@
       <c r="F37" s="31" t="s">
         <v>618</v>
       </c>
-      <c r="H37" s="4" t="s">
+      <c r="H37" s="50" t="s">
         <v>657</v>
       </c>
       <c r="I37" s="31"/>
@@ -8147,24 +8164,24 @@
       <c r="P43" s="39"/>
       <c r="Q43" s="2"/>
     </row>
-    <row r="44" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="37" t="b">
+    <row r="44" spans="1:17" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="46" t="b">
         <v>1</v>
       </c>
-      <c r="B44" s="37" t="s">
+      <c r="B44" s="46" t="s">
         <v>800</v>
       </c>
-      <c r="C44" s="37" t="s">
+      <c r="C44" s="46" t="s">
         <v>783</v>
       </c>
-      <c r="D44" s="37" t="s">
+      <c r="D44" s="46" t="s">
         <v>801</v>
       </c>
-      <c r="E44" s="37" t="s">
+      <c r="E44" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="G44" s="38"/>
-      <c r="H44" s="38"/>
+      <c r="G44" s="47"/>
+      <c r="H44" s="47"/>
     </row>
     <row r="45" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="37" t="b">
@@ -8347,13 +8364,13 @@
         <v>1</v>
       </c>
       <c r="B53" s="37" t="s">
-        <v>822</v>
+        <v>829</v>
       </c>
       <c r="C53" s="37" t="s">
-        <v>824</v>
+        <v>831</v>
       </c>
       <c r="D53" s="37" t="s">
-        <v>823</v>
+        <v>830</v>
       </c>
       <c r="E53" s="37" t="s">
         <v>68</v>
@@ -8366,10 +8383,10 @@
         <v>21</v>
       </c>
       <c r="D54" s="31" t="s">
-        <v>827</v>
+        <v>833</v>
       </c>
       <c r="E54" s="31" t="s">
-        <v>825</v>
+        <v>832</v>
       </c>
       <c r="F54" s="31" t="s">
         <v>619</v>
@@ -8386,38 +8403,74 @@
       <c r="P54" s="39"/>
       <c r="Q54" s="2"/>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B55" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D55" s="31" t="s">
+    <row r="55" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B55" s="37" t="s">
+        <v>822</v>
+      </c>
+      <c r="C55" s="37" t="s">
+        <v>824</v>
+      </c>
+      <c r="D55" s="37" t="s">
+        <v>823</v>
+      </c>
+      <c r="E55" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G55" s="38"/>
+      <c r="H55" s="38"/>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B56" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D56" s="31" t="s">
+        <v>827</v>
+      </c>
+      <c r="E56" s="31" t="s">
+        <v>825</v>
+      </c>
+      <c r="F56" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H56" s="31">
+        <v>1</v>
+      </c>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
+      <c r="L56" s="3"/>
+      <c r="M56" s="3"/>
+      <c r="N56" s="3"/>
+      <c r="P56" s="39"/>
+      <c r="Q56" s="2"/>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B57" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D57" s="31" t="s">
         <v>828</v>
       </c>
-      <c r="E55" s="31" t="s">
+      <c r="E57" s="31" t="s">
         <v>826</v>
       </c>
-      <c r="F55" s="31" t="s">
+      <c r="F57" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="H55" s="31">
+      <c r="H57" s="31">
         <v>1</v>
       </c>
-      <c r="I55" s="3"/>
-      <c r="J55" s="3"/>
-      <c r="K55" s="3"/>
-      <c r="L55" s="3"/>
-      <c r="M55" s="3"/>
-      <c r="N55" s="3"/>
-      <c r="P55" s="39"/>
-      <c r="Q55" s="2"/>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H56" s="31"/>
-      <c r="I56" s="31"/>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H57" s="31"/>
-      <c r="I57" s="31"/>
+      <c r="I57" s="3"/>
+      <c r="J57" s="3"/>
+      <c r="K57" s="3"/>
+      <c r="L57" s="3"/>
+      <c r="M57" s="3"/>
+      <c r="N57" s="3"/>
+      <c r="P57" s="39"/>
+      <c r="Q57" s="2"/>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H58" s="31"/>
@@ -8690,6 +8743,14 @@
     <row r="125" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H125" s="31"/>
       <c r="I125" s="31"/>
+    </row>
+    <row r="126" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H126" s="31"/>
+      <c r="I126" s="31"/>
+    </row>
+    <row r="127" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H127" s="31"/>
+      <c r="I127" s="31"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:Z52"/>

</xml_diff>

<commit_message>
adding swh to spreadsheet
</commit_message>
<xml_diff>
--- a/projects/m0.xlsx
+++ b/projects/m0.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2371" uniqueCount="834">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2379" uniqueCount="839">
   <si>
     <t>type</t>
   </si>
@@ -2543,6 +2543,21 @@
   </si>
   <si>
     <t>Exhaust Efficiency Multiplier</t>
+  </si>
+  <si>
+    <t>AddWaterUseConnectionAndEquipment</t>
+  </si>
+  <si>
+    <t>Add Water Use Connection and Equipment</t>
+  </si>
+  <si>
+    <t>add_water_use_connection_and_equipment</t>
+  </si>
+  <si>
+    <t>multiplier_water_use</t>
+  </si>
+  <si>
+    <t>Water Use Multiplier</t>
   </si>
 </sst>
 </file>
@@ -7172,11 +7187,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y127"/>
+  <dimension ref="A1:Y129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
+      <pane ySplit="3" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8364,13 +8379,13 @@
         <v>1</v>
       </c>
       <c r="B53" s="37" t="s">
-        <v>829</v>
+        <v>835</v>
       </c>
       <c r="C53" s="37" t="s">
-        <v>831</v>
+        <v>836</v>
       </c>
       <c r="D53" s="37" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="E53" s="37" t="s">
         <v>68</v>
@@ -8383,10 +8398,10 @@
         <v>21</v>
       </c>
       <c r="D54" s="31" t="s">
-        <v>833</v>
+        <v>838</v>
       </c>
       <c r="E54" s="31" t="s">
-        <v>832</v>
+        <v>837</v>
       </c>
       <c r="F54" s="31" t="s">
         <v>619</v>
@@ -8408,13 +8423,13 @@
         <v>1</v>
       </c>
       <c r="B55" s="37" t="s">
-        <v>822</v>
+        <v>829</v>
       </c>
       <c r="C55" s="37" t="s">
-        <v>824</v>
+        <v>831</v>
       </c>
       <c r="D55" s="37" t="s">
-        <v>823</v>
+        <v>830</v>
       </c>
       <c r="E55" s="37" t="s">
         <v>68</v>
@@ -8427,10 +8442,10 @@
         <v>21</v>
       </c>
       <c r="D56" s="31" t="s">
-        <v>827</v>
+        <v>833</v>
       </c>
       <c r="E56" s="31" t="s">
-        <v>825</v>
+        <v>832</v>
       </c>
       <c r="F56" s="31" t="s">
         <v>619</v>
@@ -8447,38 +8462,74 @@
       <c r="P56" s="39"/>
       <c r="Q56" s="2"/>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B57" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D57" s="31" t="s">
+    <row r="57" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B57" s="37" t="s">
+        <v>822</v>
+      </c>
+      <c r="C57" s="37" t="s">
+        <v>824</v>
+      </c>
+      <c r="D57" s="37" t="s">
+        <v>823</v>
+      </c>
+      <c r="E57" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G57" s="38"/>
+      <c r="H57" s="38"/>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B58" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D58" s="31" t="s">
+        <v>827</v>
+      </c>
+      <c r="E58" s="31" t="s">
+        <v>825</v>
+      </c>
+      <c r="F58" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H58" s="31">
+        <v>1</v>
+      </c>
+      <c r="I58" s="3"/>
+      <c r="J58" s="3"/>
+      <c r="K58" s="3"/>
+      <c r="L58" s="3"/>
+      <c r="M58" s="3"/>
+      <c r="N58" s="3"/>
+      <c r="P58" s="39"/>
+      <c r="Q58" s="2"/>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B59" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D59" s="31" t="s">
         <v>828</v>
       </c>
-      <c r="E57" s="31" t="s">
+      <c r="E59" s="31" t="s">
         <v>826</v>
       </c>
-      <c r="F57" s="31" t="s">
+      <c r="F59" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="H57" s="31">
+      <c r="H59" s="31">
         <v>1</v>
       </c>
-      <c r="I57" s="3"/>
-      <c r="J57" s="3"/>
-      <c r="K57" s="3"/>
-      <c r="L57" s="3"/>
-      <c r="M57" s="3"/>
-      <c r="N57" s="3"/>
-      <c r="P57" s="39"/>
-      <c r="Q57" s="2"/>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H58" s="31"/>
-      <c r="I58" s="31"/>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H59" s="31"/>
-      <c r="I59" s="31"/>
+      <c r="I59" s="3"/>
+      <c r="J59" s="3"/>
+      <c r="K59" s="3"/>
+      <c r="L59" s="3"/>
+      <c r="M59" s="3"/>
+      <c r="N59" s="3"/>
+      <c r="P59" s="39"/>
+      <c r="Q59" s="2"/>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H60" s="31"/>
@@ -8751,6 +8802,14 @@
     <row r="127" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H127" s="31"/>
       <c r="I127" s="31"/>
+    </row>
+    <row r="128" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H128" s="31"/>
+      <c r="I128" s="31"/>
+    </row>
+    <row r="129" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H129" s="31"/>
+      <c r="I129" s="31"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:Z52"/>

</xml_diff>

<commit_message>
added updated construction and new adiabatic
Also removed surface matching. It isn't needed until we use basements.
The make envelope already does basic surface matching.
</commit_message>
<xml_diff>
--- a/projects/m0.xlsx
+++ b/projects/m0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="660" windowWidth="25125" windowHeight="12165" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="660" windowWidth="24720" windowHeight="12165" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$47</definedName>
     <definedName name="AnalysisType">Lookups!$A$17:$A$23</definedName>
     <definedName name="instance_defs">Lookups!$A$2:$D$9</definedName>
     <definedName name="instance_types">Lookups!$A$2:$A$9</definedName>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2379" uniqueCount="839">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2356" uniqueCount="828">
   <si>
     <t>type</t>
   </si>
@@ -1987,45 +1987,6 @@
     <t>Total Electricity Intensity</t>
   </si>
   <si>
-    <t>SpaceTypeAndConstructionSetWizard</t>
-  </si>
-  <si>
-    <t>buildingType</t>
-  </si>
-  <si>
-    <t>Building Type</t>
-  </si>
-  <si>
-    <t>Template</t>
-  </si>
-  <si>
-    <t>template</t>
-  </si>
-  <si>
-    <t>ASHRAE Climate Zone</t>
-  </si>
-  <si>
-    <t>climateZone</t>
-  </si>
-  <si>
-    <t>createSpaceTypes</t>
-  </si>
-  <si>
-    <t>createConstructionSet</t>
-  </si>
-  <si>
-    <t>ASHRAE 169-2006-5B</t>
-  </si>
-  <si>
-    <t>Create Space Types</t>
-  </si>
-  <si>
-    <t>Create Construction Set</t>
-  </si>
-  <si>
-    <t>Space Type And Construction Set Wizard</t>
-  </si>
-  <si>
     <t>OSM</t>
   </si>
   <si>
@@ -2101,9 +2062,6 @@
     <t>Rotate Building</t>
   </si>
   <si>
-    <t>DOE Ref 1980-2004</t>
-  </si>
-  <si>
     <t>calibration_reports.electric_bill_consumption_modeled</t>
   </si>
   <si>
@@ -2338,9 +2296,6 @@
     <t>AddInternalMassToSpaceTypes</t>
   </si>
   <si>
-    <t>SurfaceMatching</t>
-  </si>
-  <si>
     <t>AddThermostats</t>
   </si>
   <si>
@@ -2422,9 +2377,6 @@
     <t>Internal Mass Multiplier</t>
   </si>
   <si>
-    <t>Surface Matching</t>
-  </si>
-  <si>
     <t>Add Thermostats</t>
   </si>
   <si>
@@ -2503,9 +2455,6 @@
     <t>Primary space type-c</t>
   </si>
   <si>
-    <t>MidriseApartment</t>
-  </si>
-  <si>
     <t>Six digit structure id</t>
   </si>
   <si>
@@ -2558,6 +2507,24 @@
   </si>
   <si>
     <t>Water Use Multiplier</t>
+  </si>
+  <si>
+    <t>AddInteriorConstructionsToAdiabaticSurfaces</t>
+  </si>
+  <si>
+    <t>add_interior_constructions_to_adiabatic_surfaces</t>
+  </si>
+  <si>
+    <t>add_constructions_to_space_types</t>
+  </si>
+  <si>
+    <t>AddConstructionsToSpaceTypes</t>
+  </si>
+  <si>
+    <t>Add Constructions to Space Types</t>
+  </si>
+  <si>
+    <t>Add Interior Constructions to Adiabatic Surfaces</t>
   </si>
 </sst>
 </file>
@@ -4624,11 +4591,11 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1801">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -6733,7 +6700,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6814,7 +6781,7 @@
         <v>456</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>662</v>
+        <v>649</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>457</v>
@@ -6825,7 +6792,7 @@
         <v>469</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>736</v>
+        <v>722</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>614</v>
@@ -6907,7 +6874,7 @@
         <v>39</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>683</v>
+        <v>670</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>471</v>
@@ -6918,10 +6885,10 @@
         <v>25</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>737</v>
+        <v>723</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>678</v>
+        <v>665</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -6929,10 +6896,10 @@
         <v>26</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>684</v>
+        <v>671</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>678</v>
+        <v>665</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -6997,7 +6964,7 @@
         <v>451</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>664</v>
+        <v>651</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -7086,7 +7053,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>677</v>
+        <v>664</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>31</v>
@@ -7099,7 +7066,7 @@
         <v>29</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>667</v>
+        <v>654</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -7113,7 +7080,7 @@
         <v>38</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>677</v>
+        <v>664</v>
       </c>
       <c r="E39" s="13" t="s">
         <v>449</v>
@@ -7124,10 +7091,10 @@
         <v>32</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>661</v>
+        <v>648</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>665</v>
+        <v>652</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>620</v>
@@ -7141,7 +7108,7 @@
         <v>34</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>682</v>
+        <v>669</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="13" t="s">
@@ -7150,13 +7117,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
-        <v>666</v>
+        <v>653</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>760</v>
+        <v>746</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>759</v>
+        <v>745</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -7187,11 +7154,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y129"/>
+  <dimension ref="A1:Y124"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B49" sqref="B49"/>
+      <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7245,14 +7212,14 @@
       <c r="Q1" s="5"/>
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
-      <c r="T1" s="51" t="s">
+      <c r="T1" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="U1" s="51"/>
-      <c r="V1" s="51"/>
-      <c r="W1" s="51"/>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="51"/>
+      <c r="U1" s="49"/>
+      <c r="V1" s="49"/>
+      <c r="W1" s="49"/>
+      <c r="X1" s="49"/>
+      <c r="Y1" s="49"/>
     </row>
     <row r="2" spans="1:25" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -7349,13 +7316,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>672</v>
+        <v>659</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>673</v>
+        <v>660</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>673</v>
+        <v>660</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>68</v>
@@ -7368,16 +7335,16 @@
         <v>21</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>679</v>
+        <v>666</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>680</v>
+        <v>667</v>
       </c>
       <c r="F5" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>681</v>
+        <v>668</v>
       </c>
     </row>
     <row r="6" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -7385,16 +7352,16 @@
         <v>21</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>675</v>
+        <v>662</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>674</v>
+        <v>661</v>
       </c>
       <c r="F6" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H6" s="31" t="s">
-        <v>758</v>
+        <v>744</v>
       </c>
     </row>
     <row r="7" spans="1:25" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -7402,13 +7369,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>814</v>
+        <v>798</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>739</v>
+        <v>725</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>738</v>
+        <v>724</v>
       </c>
       <c r="E7" s="37" t="s">
         <v>68</v>
@@ -7421,16 +7388,16 @@
         <v>21</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>743</v>
+        <v>729</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>740</v>
+        <v>726</v>
       </c>
       <c r="F8" s="31" t="s">
         <v>618</v>
       </c>
       <c r="H8" s="31" t="s">
-        <v>747</v>
+        <v>733</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
@@ -7446,10 +7413,10 @@
         <v>21</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>744</v>
+        <v>730</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>741</v>
+        <v>727</v>
       </c>
       <c r="F9" s="31" t="s">
         <v>619</v>
@@ -7469,10 +7436,10 @@
         <v>21</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>817</v>
+        <v>801</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>742</v>
+        <v>728</v>
       </c>
       <c r="F10" s="31" t="s">
         <v>622</v>
@@ -7487,13 +7454,13 @@
         <v>1</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>815</v>
+        <v>799</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>739</v>
+        <v>725</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>738</v>
+        <v>724</v>
       </c>
       <c r="E11" s="37" t="s">
         <v>68</v>
@@ -7506,16 +7473,16 @@
         <v>21</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>743</v>
+        <v>729</v>
       </c>
       <c r="E12" s="31" t="s">
-        <v>740</v>
+        <v>726</v>
       </c>
       <c r="F12" s="31" t="s">
         <v>618</v>
       </c>
       <c r="H12" s="31" t="s">
-        <v>745</v>
+        <v>731</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -7531,10 +7498,10 @@
         <v>21</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>744</v>
+        <v>730</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>741</v>
+        <v>727</v>
       </c>
       <c r="F13" s="31" t="s">
         <v>619</v>
@@ -7554,10 +7521,10 @@
         <v>21</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>818</v>
+        <v>802</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>742</v>
+        <v>728</v>
       </c>
       <c r="F14" s="31" t="s">
         <v>622</v>
@@ -7572,13 +7539,13 @@
         <v>1</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>816</v>
+        <v>800</v>
       </c>
       <c r="C15" s="37" t="s">
-        <v>739</v>
+        <v>725</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>738</v>
+        <v>724</v>
       </c>
       <c r="E15" s="37" t="s">
         <v>68</v>
@@ -7591,16 +7558,16 @@
         <v>21</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>743</v>
+        <v>729</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>740</v>
+        <v>726</v>
       </c>
       <c r="F16" s="31" t="s">
         <v>618</v>
       </c>
       <c r="H16" s="31" t="s">
-        <v>746</v>
+        <v>732</v>
       </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
@@ -7616,10 +7583,10 @@
         <v>21</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>744</v>
+        <v>730</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>741</v>
+        <v>727</v>
       </c>
       <c r="F17" s="31" t="s">
         <v>619</v>
@@ -7639,10 +7606,10 @@
         <v>21</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>819</v>
+        <v>803</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>742</v>
+        <v>728</v>
       </c>
       <c r="F18" s="31" t="s">
         <v>622</v>
@@ -7657,13 +7624,13 @@
         <v>1</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>750</v>
+        <v>736</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>748</v>
+        <v>734</v>
       </c>
       <c r="D19" s="37" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="E19" s="37" t="s">
         <v>68</v>
@@ -7676,10 +7643,10 @@
         <v>21</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>821</v>
+        <v>804</v>
       </c>
       <c r="E20" s="31" t="s">
-        <v>751</v>
+        <v>737</v>
       </c>
       <c r="F20" s="31" t="s">
         <v>631</v>
@@ -7701,16 +7668,16 @@
         <v>21</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>753</v>
+        <v>739</v>
       </c>
       <c r="E21" s="31" t="s">
-        <v>752</v>
+        <v>738</v>
       </c>
       <c r="F21" s="31" t="s">
         <v>619</v>
       </c>
       <c r="G21" s="31" t="s">
-        <v>676</v>
+        <v>663</v>
       </c>
       <c r="H21" s="4">
         <v>10</v>
@@ -7727,16 +7694,16 @@
         <v>21</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>755</v>
+        <v>741</v>
       </c>
       <c r="E22" s="31" t="s">
-        <v>754</v>
+        <v>740</v>
       </c>
       <c r="F22" s="31" t="s">
         <v>619</v>
       </c>
       <c r="G22" s="31" t="s">
-        <v>676</v>
+        <v>663</v>
       </c>
       <c r="H22" s="4">
         <v>10</v>
@@ -7748,10 +7715,10 @@
         <v>21</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>757</v>
+        <v>743</v>
       </c>
       <c r="E23" s="31" t="s">
-        <v>756</v>
+        <v>742</v>
       </c>
       <c r="F23" s="31" t="s">
         <v>619</v>
@@ -7766,10 +7733,10 @@
         <v>21</v>
       </c>
       <c r="D24" s="48" t="s">
-        <v>795</v>
+        <v>779</v>
       </c>
       <c r="E24" s="48" t="s">
-        <v>797</v>
+        <v>781</v>
       </c>
       <c r="F24" s="31" t="s">
         <v>619</v>
@@ -7784,10 +7751,10 @@
         <v>21</v>
       </c>
       <c r="D25" s="48" t="s">
-        <v>796</v>
+        <v>780</v>
       </c>
       <c r="E25" s="48" t="s">
-        <v>798</v>
+        <v>782</v>
       </c>
       <c r="F25" s="31" t="s">
         <v>619</v>
@@ -7802,13 +7769,13 @@
         <v>1</v>
       </c>
       <c r="B26" s="37" t="s">
-        <v>772</v>
+        <v>757</v>
       </c>
       <c r="C26" s="37" t="s">
-        <v>771</v>
+        <v>756</v>
       </c>
       <c r="D26" s="37" t="s">
-        <v>761</v>
+        <v>747</v>
       </c>
       <c r="E26" s="37" t="s">
         <v>68</v>
@@ -7821,10 +7788,10 @@
         <v>21</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>774</v>
+        <v>759</v>
       </c>
       <c r="E27" s="31" t="s">
-        <v>773</v>
+        <v>758</v>
       </c>
       <c r="F27" s="31" t="s">
         <v>619</v>
@@ -7846,13 +7813,13 @@
         <v>1</v>
       </c>
       <c r="B28" s="37" t="s">
-        <v>778</v>
+        <v>763</v>
       </c>
       <c r="C28" s="37" t="s">
-        <v>780</v>
+        <v>765</v>
       </c>
       <c r="D28" s="37" t="s">
-        <v>762</v>
+        <v>748</v>
       </c>
       <c r="E28" s="37" t="s">
         <v>68</v>
@@ -7865,10 +7832,10 @@
         <v>21</v>
       </c>
       <c r="D29" s="31" t="s">
-        <v>776</v>
+        <v>761</v>
       </c>
       <c r="E29" s="31" t="s">
-        <v>775</v>
+        <v>760</v>
       </c>
       <c r="F29" s="31" t="s">
         <v>619</v>
@@ -7890,13 +7857,13 @@
         <v>1</v>
       </c>
       <c r="B30" s="37" t="s">
-        <v>777</v>
+        <v>762</v>
       </c>
       <c r="C30" s="37" t="s">
-        <v>779</v>
+        <v>764</v>
       </c>
       <c r="D30" s="37" t="s">
-        <v>763</v>
+        <v>749</v>
       </c>
       <c r="E30" s="37" t="s">
         <v>68</v>
@@ -7909,10 +7876,10 @@
         <v>21</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>789</v>
+        <v>774</v>
       </c>
       <c r="E31" s="31" t="s">
-        <v>788</v>
+        <v>773</v>
       </c>
       <c r="F31" s="31" t="s">
         <v>619</v>
@@ -7934,13 +7901,13 @@
         <v>1</v>
       </c>
       <c r="B32" s="37" t="s">
-        <v>790</v>
+        <v>775</v>
       </c>
       <c r="C32" s="37" t="s">
-        <v>781</v>
+        <v>766</v>
       </c>
       <c r="D32" s="37" t="s">
-        <v>764</v>
+        <v>750</v>
       </c>
       <c r="E32" s="37" t="s">
         <v>68</v>
@@ -7953,10 +7920,10 @@
         <v>21</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>792</v>
+        <v>777</v>
       </c>
       <c r="E33" s="31" t="s">
-        <v>791</v>
+        <v>776</v>
       </c>
       <c r="F33" s="31" t="s">
         <v>619</v>
@@ -7973,139 +7940,141 @@
       <c r="P33" s="39"/>
       <c r="Q33" s="2"/>
     </row>
-    <row r="34" spans="1:17" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="46" t="b">
+    <row r="34" spans="1:17" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="50" t="b">
         <v>1</v>
       </c>
-      <c r="B34" s="46" t="s">
-        <v>660</v>
-      </c>
-      <c r="C34" s="46" t="s">
-        <v>648</v>
-      </c>
-      <c r="D34" s="46" t="s">
-        <v>648</v>
-      </c>
-      <c r="E34" s="46" t="s">
+      <c r="B34" s="50" t="s">
+        <v>826</v>
+      </c>
+      <c r="C34" s="50" t="s">
+        <v>824</v>
+      </c>
+      <c r="D34" s="50" t="s">
+        <v>825</v>
+      </c>
+      <c r="E34" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="G34" s="47"/>
-      <c r="H34" s="47"/>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B35" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D35" s="31" t="s">
-        <v>650</v>
-      </c>
-      <c r="E35" s="31" t="s">
-        <v>649</v>
-      </c>
-      <c r="F35" s="31" t="s">
-        <v>618</v>
-      </c>
-      <c r="H35" s="49" t="s">
-        <v>820</v>
-      </c>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="3"/>
-      <c r="N35" s="3"/>
-      <c r="P35" s="39"/>
-      <c r="Q35" s="2"/>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B36" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D36" s="31" t="s">
-        <v>651</v>
-      </c>
-      <c r="E36" s="31" t="s">
-        <v>652</v>
-      </c>
-      <c r="F36" s="31" t="s">
-        <v>618</v>
-      </c>
-      <c r="H36" s="50" t="s">
-        <v>686</v>
-      </c>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="3"/>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B37" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D37" s="31" t="s">
-        <v>653</v>
-      </c>
-      <c r="E37" s="31" t="s">
-        <v>654</v>
-      </c>
-      <c r="F37" s="31" t="s">
-        <v>618</v>
-      </c>
-      <c r="H37" s="50" t="s">
-        <v>657</v>
-      </c>
-      <c r="I37" s="31"/>
+      <c r="G34" s="51"/>
+      <c r="H34" s="51"/>
+    </row>
+    <row r="35" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B35" s="37" t="s">
+        <v>827</v>
+      </c>
+      <c r="C35" s="37" t="s">
+        <v>823</v>
+      </c>
+      <c r="D35" s="37" t="s">
+        <v>822</v>
+      </c>
+      <c r="E35" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38"/>
+    </row>
+    <row r="36" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B36" s="37" t="s">
+        <v>778</v>
+      </c>
+      <c r="C36" s="37" t="s">
+        <v>767</v>
+      </c>
+      <c r="D36" s="37" t="s">
+        <v>751</v>
+      </c>
+      <c r="E36" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
+    </row>
+    <row r="37" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B37" s="37" t="s">
+        <v>672</v>
+      </c>
+      <c r="C37" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="E37" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B38" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D38" s="31" t="s">
-        <v>658</v>
+        <v>341</v>
       </c>
       <c r="E38" s="31" t="s">
-        <v>655</v>
+        <v>75</v>
       </c>
       <c r="F38" s="31" t="s">
-        <v>622</v>
-      </c>
-      <c r="H38" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I38" s="31"/>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B39" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D39" s="31" t="s">
-        <v>659</v>
-      </c>
-      <c r="E39" s="31" t="s">
-        <v>656</v>
-      </c>
-      <c r="F39" s="31" t="s">
-        <v>622</v>
-      </c>
-      <c r="H39" s="4" t="b">
+        <v>619</v>
+      </c>
+      <c r="G38" s="31" t="s">
+        <v>783</v>
+      </c>
+      <c r="H38" s="31">
+        <v>0</v>
+      </c>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="P38" s="39"/>
+      <c r="Q38" s="2"/>
+    </row>
+    <row r="39" spans="1:17" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="46" t="b">
         <v>1</v>
       </c>
-      <c r="I39" s="31"/>
+      <c r="B39" s="46" t="s">
+        <v>784</v>
+      </c>
+      <c r="C39" s="46" t="s">
+        <v>768</v>
+      </c>
+      <c r="D39" s="46" t="s">
+        <v>785</v>
+      </c>
+      <c r="E39" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="G39" s="47"/>
+      <c r="H39" s="47"/>
     </row>
     <row r="40" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="37" t="b">
         <v>1</v>
       </c>
       <c r="B40" s="37" t="s">
-        <v>793</v>
+        <v>786</v>
       </c>
       <c r="C40" s="37" t="s">
-        <v>765</v>
+        <v>769</v>
       </c>
       <c r="D40" s="37" t="s">
-        <v>765</v>
+        <v>752</v>
       </c>
       <c r="E40" s="37" t="s">
         <v>68</v>
@@ -8113,37 +8082,43 @@
       <c r="G40" s="38"/>
       <c r="H40" s="38"/>
     </row>
-    <row r="41" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="37" t="b">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B41" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" s="31" t="s">
+        <v>787</v>
+      </c>
+      <c r="E41" s="31" t="s">
+        <v>788</v>
+      </c>
+      <c r="F41" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H41" s="31">
         <v>1</v>
       </c>
-      <c r="B41" s="37" t="s">
-        <v>794</v>
-      </c>
-      <c r="C41" s="37" t="s">
-        <v>782</v>
-      </c>
-      <c r="D41" s="37" t="s">
-        <v>766</v>
-      </c>
-      <c r="E41" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G41" s="38"/>
-      <c r="H41" s="38"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="P41" s="39"/>
+      <c r="Q41" s="2"/>
     </row>
     <row r="42" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="37" t="b">
         <v>1</v>
       </c>
       <c r="B42" s="37" t="s">
-        <v>685</v>
+        <v>789</v>
       </c>
       <c r="C42" s="37" t="s">
-        <v>74</v>
+        <v>770</v>
       </c>
       <c r="D42" s="37" t="s">
-        <v>74</v>
+        <v>753</v>
       </c>
       <c r="E42" s="37" t="s">
         <v>68</v>
@@ -8156,19 +8131,16 @@
         <v>21</v>
       </c>
       <c r="D43" s="31" t="s">
-        <v>341</v>
+        <v>790</v>
       </c>
       <c r="E43" s="31" t="s">
-        <v>75</v>
+        <v>791</v>
       </c>
       <c r="F43" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="G43" s="31" t="s">
-        <v>799</v>
-      </c>
       <c r="H43" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
@@ -8179,229 +8151,235 @@
       <c r="P43" s="39"/>
       <c r="Q43" s="2"/>
     </row>
-    <row r="44" spans="1:17" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="46" t="b">
+    <row r="44" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B44" s="46" t="s">
-        <v>800</v>
-      </c>
-      <c r="C44" s="46" t="s">
-        <v>783</v>
-      </c>
-      <c r="D44" s="46" t="s">
-        <v>801</v>
-      </c>
-      <c r="E44" s="46" t="s">
+      <c r="B44" s="37" t="s">
+        <v>794</v>
+      </c>
+      <c r="C44" s="37" t="s">
+        <v>771</v>
+      </c>
+      <c r="D44" s="37" t="s">
+        <v>754</v>
+      </c>
+      <c r="E44" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G44" s="47"/>
-      <c r="H44" s="47"/>
-    </row>
-    <row r="45" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="37" t="b">
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B45" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" s="31" t="s">
+        <v>793</v>
+      </c>
+      <c r="E45" s="31" t="s">
+        <v>792</v>
+      </c>
+      <c r="F45" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H45" s="31">
         <v>1</v>
       </c>
-      <c r="B45" s="37" t="s">
-        <v>802</v>
-      </c>
-      <c r="C45" s="37" t="s">
-        <v>784</v>
-      </c>
-      <c r="D45" s="37" t="s">
-        <v>767</v>
-      </c>
-      <c r="E45" s="37" t="s">
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="3"/>
+      <c r="P45" s="39"/>
+      <c r="Q45" s="2"/>
+    </row>
+    <row r="46" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B46" s="37" t="s">
+        <v>795</v>
+      </c>
+      <c r="C46" s="37" t="s">
+        <v>772</v>
+      </c>
+      <c r="D46" s="37" t="s">
+        <v>755</v>
+      </c>
+      <c r="E46" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G45" s="38"/>
-      <c r="H45" s="38"/>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B46" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D46" s="31" t="s">
-        <v>803</v>
-      </c>
-      <c r="E46" s="31" t="s">
-        <v>804</v>
-      </c>
-      <c r="F46" s="31" t="s">
+      <c r="G46" s="38"/>
+      <c r="H46" s="38"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B47" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D47" s="31" t="s">
+        <v>797</v>
+      </c>
+      <c r="E47" s="31" t="s">
+        <v>796</v>
+      </c>
+      <c r="F47" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="H46" s="31">
+      <c r="H47" s="31">
         <v>1</v>
       </c>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
-      <c r="L46" s="3"/>
-      <c r="M46" s="3"/>
-      <c r="N46" s="3"/>
-      <c r="P46" s="39"/>
-      <c r="Q46" s="2"/>
-    </row>
-    <row r="47" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="37" t="b">
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
+      <c r="P47" s="39"/>
+      <c r="Q47" s="2"/>
+    </row>
+    <row r="48" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B47" s="37" t="s">
+      <c r="B48" s="37" t="s">
+        <v>818</v>
+      </c>
+      <c r="C48" s="37" t="s">
+        <v>819</v>
+      </c>
+      <c r="D48" s="37" t="s">
+        <v>817</v>
+      </c>
+      <c r="E48" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G48" s="38"/>
+      <c r="H48" s="38"/>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B49" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D49" s="31" t="s">
+        <v>821</v>
+      </c>
+      <c r="E49" s="31" t="s">
+        <v>820</v>
+      </c>
+      <c r="F49" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H49" s="31">
+        <v>1</v>
+      </c>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
+      <c r="N49" s="3"/>
+      <c r="P49" s="39"/>
+      <c r="Q49" s="2"/>
+    </row>
+    <row r="50" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B50" s="37" t="s">
+        <v>812</v>
+      </c>
+      <c r="C50" s="37" t="s">
+        <v>814</v>
+      </c>
+      <c r="D50" s="37" t="s">
+        <v>813</v>
+      </c>
+      <c r="E50" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G50" s="38"/>
+      <c r="H50" s="38"/>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B51" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D51" s="31" t="s">
+        <v>816</v>
+      </c>
+      <c r="E51" s="31" t="s">
+        <v>815</v>
+      </c>
+      <c r="F51" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H51" s="31">
+        <v>1</v>
+      </c>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="3"/>
+      <c r="P51" s="39"/>
+      <c r="Q51" s="2"/>
+    </row>
+    <row r="52" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B52" s="37" t="s">
         <v>805</v>
       </c>
-      <c r="C47" s="37" t="s">
-        <v>785</v>
-      </c>
-      <c r="D47" s="37" t="s">
-        <v>768</v>
-      </c>
-      <c r="E47" s="37" t="s">
+      <c r="C52" s="37" t="s">
+        <v>807</v>
+      </c>
+      <c r="D52" s="37" t="s">
+        <v>806</v>
+      </c>
+      <c r="E52" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G47" s="38"/>
-      <c r="H47" s="38"/>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B48" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D48" s="31" t="s">
-        <v>806</v>
-      </c>
-      <c r="E48" s="31" t="s">
-        <v>807</v>
-      </c>
-      <c r="F48" s="31" t="s">
+      <c r="G52" s="38"/>
+      <c r="H52" s="38"/>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B53" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D53" s="31" t="s">
+        <v>810</v>
+      </c>
+      <c r="E53" s="31" t="s">
+        <v>808</v>
+      </c>
+      <c r="F53" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="H48" s="31">
+      <c r="H53" s="31">
         <v>1</v>
       </c>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
-      <c r="L48" s="3"/>
-      <c r="M48" s="3"/>
-      <c r="N48" s="3"/>
-      <c r="P48" s="39"/>
-      <c r="Q48" s="2"/>
-    </row>
-    <row r="49" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="B49" s="37" t="s">
-        <v>810</v>
-      </c>
-      <c r="C49" s="37" t="s">
-        <v>786</v>
-      </c>
-      <c r="D49" s="37" t="s">
-        <v>769</v>
-      </c>
-      <c r="E49" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G49" s="38"/>
-      <c r="H49" s="38"/>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B50" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D50" s="31" t="s">
-        <v>809</v>
-      </c>
-      <c r="E50" s="31" t="s">
-        <v>808</v>
-      </c>
-      <c r="F50" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="H50" s="31">
-        <v>1</v>
-      </c>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
-      <c r="K50" s="3"/>
-      <c r="L50" s="3"/>
-      <c r="M50" s="3"/>
-      <c r="N50" s="3"/>
-      <c r="P50" s="39"/>
-      <c r="Q50" s="2"/>
-    </row>
-    <row r="51" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="B51" s="37" t="s">
-        <v>811</v>
-      </c>
-      <c r="C51" s="37" t="s">
-        <v>787</v>
-      </c>
-      <c r="D51" s="37" t="s">
-        <v>770</v>
-      </c>
-      <c r="E51" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G51" s="38"/>
-      <c r="H51" s="38"/>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B52" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D52" s="31" t="s">
-        <v>813</v>
-      </c>
-      <c r="E52" s="31" t="s">
-        <v>812</v>
-      </c>
-      <c r="F52" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="H52" s="31">
-        <v>1</v>
-      </c>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
-      <c r="K52" s="3"/>
-      <c r="L52" s="3"/>
-      <c r="M52" s="3"/>
-      <c r="N52" s="3"/>
-      <c r="P52" s="39"/>
-      <c r="Q52" s="2"/>
-    </row>
-    <row r="53" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="B53" s="37" t="s">
-        <v>835</v>
-      </c>
-      <c r="C53" s="37" t="s">
-        <v>836</v>
-      </c>
-      <c r="D53" s="37" t="s">
-        <v>834</v>
-      </c>
-      <c r="E53" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G53" s="38"/>
-      <c r="H53" s="38"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="3"/>
+      <c r="L53" s="3"/>
+      <c r="M53" s="3"/>
+      <c r="N53" s="3"/>
+      <c r="P53" s="39"/>
+      <c r="Q53" s="2"/>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B54" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D54" s="31" t="s">
-        <v>838</v>
+        <v>811</v>
       </c>
       <c r="E54" s="31" t="s">
-        <v>837</v>
+        <v>809</v>
       </c>
       <c r="F54" s="31" t="s">
         <v>619</v>
@@ -8418,118 +8396,25 @@
       <c r="P54" s="39"/>
       <c r="Q54" s="2"/>
     </row>
-    <row r="55" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="B55" s="37" t="s">
-        <v>829</v>
-      </c>
-      <c r="C55" s="37" t="s">
-        <v>831</v>
-      </c>
-      <c r="D55" s="37" t="s">
-        <v>830</v>
-      </c>
-      <c r="E55" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G55" s="38"/>
-      <c r="H55" s="38"/>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H55" s="31"/>
+      <c r="I55" s="31"/>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B56" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D56" s="31" t="s">
-        <v>833</v>
-      </c>
-      <c r="E56" s="31" t="s">
-        <v>832</v>
-      </c>
-      <c r="F56" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="H56" s="31">
-        <v>1</v>
-      </c>
-      <c r="I56" s="3"/>
-      <c r="J56" s="3"/>
-      <c r="K56" s="3"/>
-      <c r="L56" s="3"/>
-      <c r="M56" s="3"/>
-      <c r="N56" s="3"/>
-      <c r="P56" s="39"/>
-      <c r="Q56" s="2"/>
-    </row>
-    <row r="57" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="B57" s="37" t="s">
-        <v>822</v>
-      </c>
-      <c r="C57" s="37" t="s">
-        <v>824</v>
-      </c>
-      <c r="D57" s="37" t="s">
-        <v>823</v>
-      </c>
-      <c r="E57" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G57" s="38"/>
-      <c r="H57" s="38"/>
+      <c r="H56" s="31"/>
+      <c r="I56" s="31"/>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H57" s="31"/>
+      <c r="I57" s="31"/>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B58" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D58" s="31" t="s">
-        <v>827</v>
-      </c>
-      <c r="E58" s="31" t="s">
-        <v>825</v>
-      </c>
-      <c r="F58" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="H58" s="31">
-        <v>1</v>
-      </c>
-      <c r="I58" s="3"/>
-      <c r="J58" s="3"/>
-      <c r="K58" s="3"/>
-      <c r="L58" s="3"/>
-      <c r="M58" s="3"/>
-      <c r="N58" s="3"/>
-      <c r="P58" s="39"/>
-      <c r="Q58" s="2"/>
+      <c r="H58" s="31"/>
+      <c r="I58" s="31"/>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B59" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D59" s="31" t="s">
-        <v>828</v>
-      </c>
-      <c r="E59" s="31" t="s">
-        <v>826</v>
-      </c>
-      <c r="F59" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="H59" s="31">
-        <v>1</v>
-      </c>
-      <c r="I59" s="3"/>
-      <c r="J59" s="3"/>
-      <c r="K59" s="3"/>
-      <c r="L59" s="3"/>
-      <c r="M59" s="3"/>
-      <c r="N59" s="3"/>
-      <c r="P59" s="39"/>
-      <c r="Q59" s="2"/>
+      <c r="H59" s="31"/>
+      <c r="I59" s="31"/>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H60" s="31"/>
@@ -8791,28 +8676,8 @@
       <c r="H124" s="31"/>
       <c r="I124" s="31"/>
     </row>
-    <row r="125" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H125" s="31"/>
-      <c r="I125" s="31"/>
-    </row>
-    <row r="126" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H126" s="31"/>
-      <c r="I126" s="31"/>
-    </row>
-    <row r="127" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H127" s="31"/>
-      <c r="I127" s="31"/>
-    </row>
-    <row r="128" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H128" s="31"/>
-      <c r="I128" s="31"/>
-    </row>
-    <row r="129" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H129" s="31"/>
-      <c r="I129" s="31"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A2:Z52"/>
+  <autoFilter ref="A2:Z47"/>
   <mergeCells count="1">
     <mergeCell ref="T1:Y1"/>
   </mergeCells>
@@ -9058,11 +8923,11 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="40" t="s">
-        <v>704</v>
+        <v>690</v>
       </c>
       <c r="B8" s="40"/>
       <c r="C8" s="40" t="s">
-        <v>705</v>
+        <v>691</v>
       </c>
       <c r="D8" s="40" t="s">
         <v>468</v>
@@ -9086,11 +8951,11 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="40" t="s">
-        <v>706</v>
+        <v>692</v>
       </c>
       <c r="B9" s="40"/>
       <c r="C9" s="40" t="s">
-        <v>707</v>
+        <v>693</v>
       </c>
       <c r="D9" s="40" t="s">
         <v>468</v>
@@ -9114,11 +8979,11 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="40" t="s">
-        <v>708</v>
+        <v>694</v>
       </c>
       <c r="B10" s="40"/>
       <c r="C10" s="40" t="s">
-        <v>709</v>
+        <v>695</v>
       </c>
       <c r="D10" s="40" t="s">
         <v>468</v>
@@ -9142,11 +9007,11 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
-        <v>710</v>
+        <v>696</v>
       </c>
       <c r="B11" s="40"/>
       <c r="C11" s="40" t="s">
-        <v>711</v>
+        <v>697</v>
       </c>
       <c r="D11" s="40" t="s">
         <v>468</v>
@@ -9170,11 +9035,11 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="B12" s="40"/>
       <c r="C12" s="40" t="s">
-        <v>713</v>
+        <v>699</v>
       </c>
       <c r="D12" s="40" t="s">
         <v>468</v>
@@ -9198,11 +9063,11 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="40" t="s">
-        <v>714</v>
+        <v>700</v>
       </c>
       <c r="B13" s="40"/>
       <c r="C13" s="40" t="s">
-        <v>715</v>
+        <v>701</v>
       </c>
       <c r="D13" s="40" t="s">
         <v>468</v>
@@ -9226,11 +9091,11 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="40" t="s">
-        <v>716</v>
+        <v>702</v>
       </c>
       <c r="B14" s="40"/>
       <c r="C14" s="40" t="s">
-        <v>717</v>
+        <v>703</v>
       </c>
       <c r="D14" s="40" t="s">
         <v>468</v>
@@ -9254,11 +9119,11 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="40" t="s">
-        <v>718</v>
+        <v>704</v>
       </c>
       <c r="B15" s="40"/>
       <c r="C15" s="40" t="s">
-        <v>719</v>
+        <v>705</v>
       </c>
       <c r="D15" s="40" t="s">
         <v>468</v>
@@ -9282,11 +9147,11 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="40" t="s">
-        <v>720</v>
+        <v>706</v>
       </c>
       <c r="B16" s="40"/>
       <c r="C16" s="40" t="s">
-        <v>721</v>
+        <v>707</v>
       </c>
       <c r="D16" s="40" t="s">
         <v>468</v>
@@ -9310,11 +9175,11 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="40" t="s">
-        <v>722</v>
+        <v>708</v>
       </c>
       <c r="B17" s="40"/>
       <c r="C17" s="40" t="s">
-        <v>723</v>
+        <v>709</v>
       </c>
       <c r="D17" s="40" t="s">
         <v>468</v>
@@ -9338,11 +9203,11 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="40" t="s">
-        <v>724</v>
+        <v>710</v>
       </c>
       <c r="B18" s="40"/>
       <c r="C18" s="40" t="s">
-        <v>725</v>
+        <v>711</v>
       </c>
       <c r="D18" s="40" t="s">
         <v>468</v>
@@ -9366,11 +9231,11 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="40" t="s">
-        <v>726</v>
+        <v>712</v>
       </c>
       <c r="B19" s="40"/>
       <c r="C19" s="40" t="s">
-        <v>727</v>
+        <v>713</v>
       </c>
       <c r="D19" s="40" t="s">
         <v>468</v>
@@ -9394,11 +9259,11 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="40" t="s">
-        <v>728</v>
+        <v>714</v>
       </c>
       <c r="B20" s="40"/>
       <c r="C20" s="40" t="s">
-        <v>729</v>
+        <v>715</v>
       </c>
       <c r="D20" s="40" t="s">
         <v>468</v>
@@ -9422,11 +9287,11 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="40" t="s">
-        <v>730</v>
+        <v>716</v>
       </c>
       <c r="B21" s="40"/>
       <c r="C21" s="40" t="s">
-        <v>731</v>
+        <v>717</v>
       </c>
       <c r="D21" s="40" t="s">
         <v>468</v>
@@ -9450,14 +9315,14 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="40" t="s">
-        <v>698</v>
+        <v>684</v>
       </c>
       <c r="B22" s="40"/>
       <c r="C22" s="40" t="s">
-        <v>732</v>
+        <v>718</v>
       </c>
       <c r="D22" s="40" t="s">
-        <v>699</v>
+        <v>685</v>
       </c>
       <c r="E22" s="40" t="s">
         <v>64</v>
@@ -9478,14 +9343,14 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="40" t="s">
-        <v>700</v>
+        <v>686</v>
       </c>
       <c r="B23" s="40"/>
       <c r="C23" s="40" t="s">
-        <v>733</v>
+        <v>719</v>
       </c>
       <c r="D23" s="40" t="s">
-        <v>699</v>
+        <v>685</v>
       </c>
       <c r="E23" s="40" t="s">
         <v>64</v>
@@ -9506,14 +9371,14 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="40" t="s">
-        <v>701</v>
+        <v>687</v>
       </c>
       <c r="B24" s="40"/>
       <c r="C24" s="40" t="s">
-        <v>734</v>
+        <v>720</v>
       </c>
       <c r="D24" s="40" t="s">
-        <v>699</v>
+        <v>685</v>
       </c>
       <c r="E24" s="40" t="s">
         <v>64</v>
@@ -9534,14 +9399,14 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="40" t="s">
-        <v>702</v>
+        <v>688</v>
       </c>
       <c r="B25" s="40"/>
       <c r="C25" s="40" t="s">
-        <v>735</v>
+        <v>721</v>
       </c>
       <c r="D25" s="40" t="s">
-        <v>703</v>
+        <v>689</v>
       </c>
       <c r="E25" s="40" t="s">
         <v>64</v>
@@ -9562,14 +9427,14 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="40" t="s">
-        <v>668</v>
+        <v>655</v>
       </c>
       <c r="B26" s="40"/>
       <c r="C26" s="40" t="s">
-        <v>687</v>
+        <v>673</v>
       </c>
       <c r="D26" s="40" t="s">
-        <v>669</v>
+        <v>656</v>
       </c>
       <c r="E26" s="40" t="s">
         <v>64</v>
@@ -9590,14 +9455,14 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="40" t="s">
-        <v>670</v>
+        <v>657</v>
       </c>
       <c r="B27" s="40"/>
       <c r="C27" s="40" t="s">
-        <v>688</v>
+        <v>674</v>
       </c>
       <c r="D27" s="40" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="E27" s="40" t="s">
         <v>64</v>
@@ -9618,14 +9483,14 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="40" t="s">
-        <v>694</v>
+        <v>680</v>
       </c>
       <c r="B28" s="40"/>
       <c r="C28" s="40" t="s">
-        <v>689</v>
+        <v>675</v>
       </c>
       <c r="D28" s="40" t="s">
-        <v>690</v>
+        <v>676</v>
       </c>
       <c r="E28" s="40" t="s">
         <v>64</v>
@@ -9648,14 +9513,14 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="40" t="s">
-        <v>695</v>
+        <v>681</v>
       </c>
       <c r="B29" s="40"/>
       <c r="C29" s="40" t="s">
-        <v>691</v>
+        <v>677</v>
       </c>
       <c r="D29" s="40" t="s">
-        <v>690</v>
+        <v>676</v>
       </c>
       <c r="E29" s="40" t="s">
         <v>64</v>
@@ -9678,14 +9543,14 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="40" t="s">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="B30" s="40"/>
       <c r="C30" s="40" t="s">
-        <v>692</v>
+        <v>678</v>
       </c>
       <c r="D30" s="40" t="s">
-        <v>690</v>
+        <v>676</v>
       </c>
       <c r="E30" s="40" t="s">
         <v>64</v>
@@ -9708,14 +9573,14 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="40" t="s">
-        <v>697</v>
+        <v>683</v>
       </c>
       <c r="B31" s="40"/>
       <c r="C31" s="40" t="s">
-        <v>693</v>
+        <v>679</v>
       </c>
       <c r="D31" s="40" t="s">
-        <v>690</v>
+        <v>676</v>
       </c>
       <c r="E31" s="40" t="s">
         <v>64</v>
@@ -18411,7 +18276,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>663</v>
+        <v>650</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>557</v>

</xml_diff>

<commit_message>
re-order internal mass measure
Needed to move it down so it occurs after the constructions are added to
the model.
</commit_message>
<xml_diff>
--- a/projects/m0.xlsx
+++ b/projects/m0.xlsx
@@ -7158,7 +7158,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
+      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7896,87 +7896,87 @@
       <c r="P31" s="39"/>
       <c r="Q31" s="2"/>
     </row>
-    <row r="32" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="37" t="b">
+    <row r="32" spans="1:17" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="50" t="b">
         <v>1</v>
       </c>
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="50" t="s">
+        <v>826</v>
+      </c>
+      <c r="C32" s="50" t="s">
+        <v>824</v>
+      </c>
+      <c r="D32" s="50" t="s">
+        <v>825</v>
+      </c>
+      <c r="E32" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="G32" s="51"/>
+      <c r="H32" s="51"/>
+    </row>
+    <row r="33" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B33" s="37" t="s">
+        <v>827</v>
+      </c>
+      <c r="C33" s="37" t="s">
+        <v>823</v>
+      </c>
+      <c r="D33" s="37" t="s">
+        <v>822</v>
+      </c>
+      <c r="E33" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+    </row>
+    <row r="34" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B34" s="37" t="s">
         <v>775</v>
       </c>
-      <c r="C32" s="37" t="s">
+      <c r="C34" s="37" t="s">
         <v>766</v>
       </c>
-      <c r="D32" s="37" t="s">
+      <c r="D34" s="37" t="s">
         <v>750</v>
       </c>
-      <c r="E32" s="37" t="s">
+      <c r="E34" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G32" s="38"/>
-      <c r="H32" s="38"/>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B33" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D33" s="31" t="s">
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B35" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="31" t="s">
         <v>777</v>
       </c>
-      <c r="E33" s="31" t="s">
+      <c r="E35" s="31" t="s">
         <v>776</v>
       </c>
-      <c r="F33" s="31" t="s">
+      <c r="F35" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="H33" s="31">
+      <c r="H35" s="31">
         <v>1</v>
       </c>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
-      <c r="P33" s="39"/>
-      <c r="Q33" s="2"/>
-    </row>
-    <row r="34" spans="1:17" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="50" t="b">
-        <v>1</v>
-      </c>
-      <c r="B34" s="50" t="s">
-        <v>826</v>
-      </c>
-      <c r="C34" s="50" t="s">
-        <v>824</v>
-      </c>
-      <c r="D34" s="50" t="s">
-        <v>825</v>
-      </c>
-      <c r="E34" s="50" t="s">
-        <v>68</v>
-      </c>
-      <c r="G34" s="51"/>
-      <c r="H34" s="51"/>
-    </row>
-    <row r="35" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="B35" s="37" t="s">
-        <v>827</v>
-      </c>
-      <c r="C35" s="37" t="s">
-        <v>823</v>
-      </c>
-      <c r="D35" s="37" t="s">
-        <v>822</v>
-      </c>
-      <c r="E35" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G35" s="38"/>
-      <c r="H35" s="38"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="P35" s="39"/>
+      <c r="Q35" s="2"/>
     </row>
     <row r="36" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="37" t="b">

</xml_diff>

<commit_message>
adding new args to gather space type measures
also added place holder for hvac measrues that will pull system types
for each space type from the gather space type data.
</commit_message>
<xml_diff>
--- a/projects/m0.xlsx
+++ b/projects/m0.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$50</definedName>
     <definedName name="AnalysisType">Lookups!$A$17:$A$23</definedName>
     <definedName name="instance_defs">Lookups!$A$2:$D$9</definedName>
     <definedName name="instance_types">Lookups!$A$2:$A$9</definedName>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2356" uniqueCount="828">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2415" uniqueCount="864">
   <si>
     <t>type</t>
   </si>
@@ -2525,6 +2525,114 @@
   </si>
   <si>
     <t>Add Interior Constructions to Adiabatic Surfaces</t>
+  </si>
+  <si>
+    <t>HVAC System Type</t>
+  </si>
+  <si>
+    <t>hvac_system_type</t>
+  </si>
+  <si>
+    <t>add_system_03</t>
+  </si>
+  <si>
+    <t>AddSystem03</t>
+  </si>
+  <si>
+    <t>Add System 03</t>
+  </si>
+  <si>
+    <t>Add System 01</t>
+  </si>
+  <si>
+    <t>add_system_01</t>
+  </si>
+  <si>
+    <t>AddSystem01</t>
+  </si>
+  <si>
+    <t>Add System 02</t>
+  </si>
+  <si>
+    <t>add_system_02</t>
+  </si>
+  <si>
+    <t>AddSystem02</t>
+  </si>
+  <si>
+    <t>Add System 04</t>
+  </si>
+  <si>
+    <t>add_system_04</t>
+  </si>
+  <si>
+    <t>AddSystem04</t>
+  </si>
+  <si>
+    <t>Add System 05</t>
+  </si>
+  <si>
+    <t>add_system_05</t>
+  </si>
+  <si>
+    <t>AddSystem05</t>
+  </si>
+  <si>
+    <t>Add System 06</t>
+  </si>
+  <si>
+    <t>add_system_06</t>
+  </si>
+  <si>
+    <t>AddSystem06</t>
+  </si>
+  <si>
+    <t>Add System 07</t>
+  </si>
+  <si>
+    <t>add_system_07</t>
+  </si>
+  <si>
+    <t>AddSystem07</t>
+  </si>
+  <si>
+    <t>Add System 08</t>
+  </si>
+  <si>
+    <t>add_system_08</t>
+  </si>
+  <si>
+    <t>AddSystem08</t>
+  </si>
+  <si>
+    <t>Add System 09</t>
+  </si>
+  <si>
+    <t>add_system_09</t>
+  </si>
+  <si>
+    <t>AddSystem09</t>
+  </si>
+  <si>
+    <t>Add System 10</t>
+  </si>
+  <si>
+    <t>add_system_10</t>
+  </si>
+  <si>
+    <t>AddSystem10</t>
+  </si>
+  <si>
+    <t>Add Service Water Heating Supply</t>
+  </si>
+  <si>
+    <t>add_service_water_heating_supply</t>
+  </si>
+  <si>
+    <t>AddServiceWaterHeatingSupply</t>
+  </si>
+  <si>
+    <t>SysType 3</t>
   </si>
 </sst>
 </file>
@@ -7157,8 +7265,8 @@
   <dimension ref="A1:Y124"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7449,484 +7557,475 @@
       </c>
       <c r="I10" s="31"/>
     </row>
-    <row r="11" spans="1:25" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="b">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B11" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>828</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>829</v>
+      </c>
+      <c r="F11" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>863</v>
+      </c>
+      <c r="I11" s="31"/>
+    </row>
+    <row r="12" spans="1:25" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B12" s="37" t="s">
         <v>799</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C12" s="37" t="s">
         <v>725</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D12" s="37" t="s">
         <v>724</v>
       </c>
-      <c r="E11" s="37" t="s">
+      <c r="E12" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B12" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>729</v>
-      </c>
-      <c r="E12" s="31" t="s">
-        <v>726</v>
-      </c>
-      <c r="F12" s="31" t="s">
-        <v>618</v>
-      </c>
-      <c r="H12" s="31" t="s">
-        <v>731</v>
-      </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="P12" s="39"/>
-      <c r="Q12" s="2"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B13" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="F13" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="H13" s="4">
-        <v>2.8000000000000001E-2</v>
+        <v>618</v>
+      </c>
+      <c r="H13" s="31" t="s">
+        <v>731</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="P13" s="39"/>
+      <c r="Q13" s="2"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B14" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D14" s="31" t="s">
+        <v>730</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>727</v>
+      </c>
+      <c r="F14" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H14" s="4">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="3"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B15" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="31" t="s">
         <v>802</v>
       </c>
-      <c r="E14" s="31" t="s">
+      <c r="E15" s="31" t="s">
         <v>728</v>
       </c>
-      <c r="F14" s="31" t="s">
+      <c r="F15" s="31" t="s">
         <v>622</v>
       </c>
-      <c r="H14" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="I14" s="31"/>
-    </row>
-    <row r="15" spans="1:25" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="B15" s="37" t="s">
-        <v>800</v>
-      </c>
-      <c r="C15" s="37" t="s">
-        <v>725</v>
-      </c>
-      <c r="D15" s="37" t="s">
-        <v>724</v>
-      </c>
-      <c r="E15" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
+      <c r="H15" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="31"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>729</v>
+        <v>828</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>726</v>
-      </c>
-      <c r="F16" s="31" t="s">
-        <v>618</v>
+        <v>829</v>
+      </c>
+      <c r="F16" s="30" t="s">
+        <v>104</v>
       </c>
       <c r="H16" s="31" t="s">
-        <v>732</v>
-      </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="P16" s="39"/>
-      <c r="Q16" s="2"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="31" t="s">
-        <v>730</v>
-      </c>
-      <c r="E17" s="31" t="s">
-        <v>727</v>
-      </c>
-      <c r="F17" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="H17" s="4">
-        <v>9.9000000000000005E-2</v>
-      </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="3"/>
+        <v>863</v>
+      </c>
+      <c r="I16" s="31"/>
+    </row>
+    <row r="17" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B17" s="37" t="s">
+        <v>800</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>725</v>
+      </c>
+      <c r="D17" s="37" t="s">
+        <v>724</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B18" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>803</v>
+        <v>729</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="F18" s="31" t="s">
-        <v>622</v>
-      </c>
-      <c r="H18" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="I18" s="31"/>
-    </row>
-    <row r="19" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="B19" s="37" t="s">
-        <v>736</v>
-      </c>
-      <c r="C19" s="37" t="s">
-        <v>734</v>
-      </c>
-      <c r="D19" s="37" t="s">
-        <v>735</v>
-      </c>
-      <c r="E19" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
+        <v>618</v>
+      </c>
+      <c r="H18" s="31" t="s">
+        <v>732</v>
+      </c>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="P18" s="39"/>
+      <c r="Q18" s="2"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B19" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>730</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>727</v>
+      </c>
+      <c r="F19" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H19" s="4">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="3"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B20" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E20" s="31" t="s">
-        <v>737</v>
+        <v>728</v>
       </c>
       <c r="F20" s="31" t="s">
-        <v>631</v>
-      </c>
-      <c r="H20" s="31">
-        <v>999999</v>
-      </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="P20" s="39"/>
-      <c r="Q20" s="2"/>
+        <v>622</v>
+      </c>
+      <c r="H20" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" s="31"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B21" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>739</v>
+        <v>828</v>
       </c>
       <c r="E21" s="31" t="s">
-        <v>738</v>
-      </c>
-      <c r="F21" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="G21" s="31" t="s">
-        <v>663</v>
-      </c>
-      <c r="H21" s="4">
-        <v>10</v>
-      </c>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="3"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B22" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22" s="31" t="s">
-        <v>741</v>
-      </c>
-      <c r="E22" s="31" t="s">
-        <v>740</v>
-      </c>
-      <c r="F22" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="G22" s="31" t="s">
-        <v>663</v>
-      </c>
-      <c r="H22" s="4">
-        <v>10</v>
-      </c>
-      <c r="I22" s="31"/>
+        <v>829</v>
+      </c>
+      <c r="F21" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="H21" s="31" t="s">
+        <v>863</v>
+      </c>
+      <c r="I21" s="31"/>
+    </row>
+    <row r="22" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B22" s="37" t="s">
+        <v>736</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>734</v>
+      </c>
+      <c r="D22" s="37" t="s">
+        <v>735</v>
+      </c>
+      <c r="E22" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B23" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>743</v>
+        <v>804</v>
       </c>
       <c r="E23" s="31" t="s">
-        <v>742</v>
+        <v>737</v>
       </c>
       <c r="F23" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="H23" s="4">
-        <v>2</v>
-      </c>
-      <c r="I23" s="31"/>
+        <v>631</v>
+      </c>
+      <c r="H23" s="31">
+        <v>999999</v>
+      </c>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="P23" s="39"/>
+      <c r="Q23" s="2"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B24" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="48" t="s">
-        <v>779</v>
-      </c>
-      <c r="E24" s="48" t="s">
-        <v>781</v>
+      <c r="D24" s="31" t="s">
+        <v>739</v>
+      </c>
+      <c r="E24" s="31" t="s">
+        <v>738</v>
       </c>
       <c r="F24" s="31" t="s">
         <v>619</v>
       </c>
+      <c r="G24" s="31" t="s">
+        <v>663</v>
+      </c>
       <c r="H24" s="4">
-        <v>8</v>
-      </c>
-      <c r="I24" s="31"/>
+        <v>10</v>
+      </c>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="3"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B25" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="48" t="s">
-        <v>780</v>
-      </c>
-      <c r="E25" s="48" t="s">
-        <v>782</v>
+      <c r="D25" s="31" t="s">
+        <v>741</v>
+      </c>
+      <c r="E25" s="31" t="s">
+        <v>740</v>
       </c>
       <c r="F25" s="31" t="s">
         <v>619</v>
       </c>
+      <c r="G25" s="31" t="s">
+        <v>663</v>
+      </c>
       <c r="H25" s="4">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I25" s="31"/>
     </row>
-    <row r="26" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="B26" s="37" t="s">
-        <v>757</v>
-      </c>
-      <c r="C26" s="37" t="s">
-        <v>756</v>
-      </c>
-      <c r="D26" s="37" t="s">
-        <v>747</v>
-      </c>
-      <c r="E26" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B26" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="31" t="s">
+        <v>743</v>
+      </c>
+      <c r="E26" s="31" t="s">
+        <v>742</v>
+      </c>
+      <c r="F26" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H26" s="4">
+        <v>2</v>
+      </c>
+      <c r="I26" s="31"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B27" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="31" t="s">
-        <v>759</v>
-      </c>
-      <c r="E27" s="31" t="s">
-        <v>758</v>
+      <c r="D27" s="48" t="s">
+        <v>779</v>
+      </c>
+      <c r="E27" s="48" t="s">
+        <v>781</v>
       </c>
       <c r="F27" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="H27" s="31">
+      <c r="H27" s="4">
+        <v>8</v>
+      </c>
+      <c r="I27" s="31"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B28" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="48" t="s">
+        <v>780</v>
+      </c>
+      <c r="E28" s="48" t="s">
+        <v>782</v>
+      </c>
+      <c r="F28" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H28" s="4">
+        <v>17</v>
+      </c>
+      <c r="I28" s="31"/>
+    </row>
+    <row r="29" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="P27" s="39"/>
-      <c r="Q27" s="2"/>
-    </row>
-    <row r="28" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="37" t="b">
+      <c r="B29" s="37" t="s">
+        <v>757</v>
+      </c>
+      <c r="C29" s="37" t="s">
+        <v>756</v>
+      </c>
+      <c r="D29" s="37" t="s">
+        <v>747</v>
+      </c>
+      <c r="E29" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B30" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="31" t="s">
+        <v>759</v>
+      </c>
+      <c r="E30" s="31" t="s">
+        <v>758</v>
+      </c>
+      <c r="F30" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H30" s="31">
         <v>1</v>
       </c>
-      <c r="B28" s="37" t="s">
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="P30" s="39"/>
+      <c r="Q30" s="2"/>
+    </row>
+    <row r="31" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B31" s="37" t="s">
         <v>763</v>
       </c>
-      <c r="C28" s="37" t="s">
+      <c r="C31" s="37" t="s">
         <v>765</v>
       </c>
-      <c r="D28" s="37" t="s">
+      <c r="D31" s="37" t="s">
         <v>748</v>
       </c>
-      <c r="E28" s="37" t="s">
+      <c r="E31" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B29" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D29" s="31" t="s">
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B32" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="31" t="s">
         <v>761</v>
       </c>
-      <c r="E29" s="31" t="s">
+      <c r="E32" s="31" t="s">
         <v>760</v>
       </c>
-      <c r="F29" s="31" t="s">
+      <c r="F32" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="H29" s="31">
+      <c r="H32" s="31">
         <v>1</v>
       </c>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="P29" s="39"/>
-      <c r="Q29" s="2"/>
-    </row>
-    <row r="30" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="B30" s="37" t="s">
-        <v>762</v>
-      </c>
-      <c r="C30" s="37" t="s">
-        <v>764</v>
-      </c>
-      <c r="D30" s="37" t="s">
-        <v>749</v>
-      </c>
-      <c r="E30" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B31" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D31" s="31" t="s">
-        <v>774</v>
-      </c>
-      <c r="E31" s="31" t="s">
-        <v>773</v>
-      </c>
-      <c r="F31" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="H31" s="31">
-        <v>1</v>
-      </c>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-      <c r="P31" s="39"/>
-      <c r="Q31" s="2"/>
-    </row>
-    <row r="32" spans="1:17" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="50" t="b">
-        <v>1</v>
-      </c>
-      <c r="B32" s="50" t="s">
-        <v>826</v>
-      </c>
-      <c r="C32" s="50" t="s">
-        <v>824</v>
-      </c>
-      <c r="D32" s="50" t="s">
-        <v>825</v>
-      </c>
-      <c r="E32" s="50" t="s">
-        <v>68</v>
-      </c>
-      <c r="G32" s="51"/>
-      <c r="H32" s="51"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="P32" s="39"/>
+      <c r="Q32" s="2"/>
     </row>
     <row r="33" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="37" t="b">
         <v>1</v>
       </c>
       <c r="B33" s="37" t="s">
-        <v>827</v>
+        <v>762</v>
       </c>
       <c r="C33" s="37" t="s">
-        <v>823</v>
+        <v>764</v>
       </c>
       <c r="D33" s="37" t="s">
-        <v>822</v>
+        <v>749</v>
       </c>
       <c r="E33" s="37" t="s">
         <v>68</v>
@@ -7934,62 +8033,62 @@
       <c r="G33" s="38"/>
       <c r="H33" s="38"/>
     </row>
-    <row r="34" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="37" t="b">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B34" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="31" t="s">
+        <v>774</v>
+      </c>
+      <c r="E34" s="31" t="s">
+        <v>773</v>
+      </c>
+      <c r="F34" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H34" s="31">
         <v>1</v>
       </c>
-      <c r="B34" s="37" t="s">
-        <v>775</v>
-      </c>
-      <c r="C34" s="37" t="s">
-        <v>766</v>
-      </c>
-      <c r="D34" s="37" t="s">
-        <v>750</v>
-      </c>
-      <c r="E34" s="37" t="s">
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="P34" s="39"/>
+      <c r="Q34" s="2"/>
+    </row>
+    <row r="35" spans="1:17" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="B35" s="50" t="s">
+        <v>826</v>
+      </c>
+      <c r="C35" s="50" t="s">
+        <v>824</v>
+      </c>
+      <c r="D35" s="50" t="s">
+        <v>825</v>
+      </c>
+      <c r="E35" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="G34" s="38"/>
-      <c r="H34" s="38"/>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B35" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D35" s="31" t="s">
-        <v>777</v>
-      </c>
-      <c r="E35" s="31" t="s">
-        <v>776</v>
-      </c>
-      <c r="F35" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="H35" s="31">
-        <v>1</v>
-      </c>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="3"/>
-      <c r="N35" s="3"/>
-      <c r="P35" s="39"/>
-      <c r="Q35" s="2"/>
+      <c r="G35" s="51"/>
+      <c r="H35" s="51"/>
     </row>
     <row r="36" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="37" t="b">
         <v>1</v>
       </c>
       <c r="B36" s="37" t="s">
-        <v>778</v>
+        <v>827</v>
       </c>
       <c r="C36" s="37" t="s">
-        <v>767</v>
+        <v>823</v>
       </c>
       <c r="D36" s="37" t="s">
-        <v>751</v>
+        <v>822</v>
       </c>
       <c r="E36" s="37" t="s">
         <v>68</v>
@@ -8002,13 +8101,13 @@
         <v>1</v>
       </c>
       <c r="B37" s="37" t="s">
-        <v>672</v>
+        <v>775</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>74</v>
+        <v>766</v>
       </c>
       <c r="D37" s="37" t="s">
-        <v>74</v>
+        <v>750</v>
       </c>
       <c r="E37" s="37" t="s">
         <v>68</v>
@@ -8021,19 +8120,16 @@
         <v>21</v>
       </c>
       <c r="D38" s="31" t="s">
-        <v>341</v>
+        <v>777</v>
       </c>
       <c r="E38" s="31" t="s">
-        <v>75</v>
+        <v>776</v>
       </c>
       <c r="F38" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="G38" s="31" t="s">
-        <v>783</v>
-      </c>
       <c r="H38" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
@@ -8044,37 +8140,37 @@
       <c r="P38" s="39"/>
       <c r="Q38" s="2"/>
     </row>
-    <row r="39" spans="1:17" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="46" t="b">
+    <row r="39" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B39" s="46" t="s">
-        <v>784</v>
-      </c>
-      <c r="C39" s="46" t="s">
-        <v>768</v>
-      </c>
-      <c r="D39" s="46" t="s">
-        <v>785</v>
-      </c>
-      <c r="E39" s="46" t="s">
+      <c r="B39" s="37" t="s">
+        <v>778</v>
+      </c>
+      <c r="C39" s="37" t="s">
+        <v>767</v>
+      </c>
+      <c r="D39" s="37" t="s">
+        <v>751</v>
+      </c>
+      <c r="E39" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G39" s="47"/>
-      <c r="H39" s="47"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
     </row>
     <row r="40" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="37" t="b">
         <v>1</v>
       </c>
       <c r="B40" s="37" t="s">
-        <v>786</v>
+        <v>672</v>
       </c>
       <c r="C40" s="37" t="s">
-        <v>769</v>
+        <v>74</v>
       </c>
       <c r="D40" s="37" t="s">
-        <v>752</v>
+        <v>74</v>
       </c>
       <c r="E40" s="37" t="s">
         <v>68</v>
@@ -8087,16 +8183,19 @@
         <v>21</v>
       </c>
       <c r="D41" s="31" t="s">
-        <v>787</v>
+        <v>341</v>
       </c>
       <c r="E41" s="31" t="s">
-        <v>788</v>
+        <v>75</v>
       </c>
       <c r="F41" s="31" t="s">
         <v>619</v>
       </c>
+      <c r="G41" s="31" t="s">
+        <v>783</v>
+      </c>
       <c r="H41" s="31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
@@ -8107,279 +8206,273 @@
       <c r="P41" s="39"/>
       <c r="Q41" s="2"/>
     </row>
-    <row r="42" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="37" t="b">
+    <row r="42" spans="1:17" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="46" t="b">
         <v>1</v>
       </c>
-      <c r="B42" s="37" t="s">
+      <c r="B42" s="46" t="s">
+        <v>784</v>
+      </c>
+      <c r="C42" s="46" t="s">
+        <v>768</v>
+      </c>
+      <c r="D42" s="46" t="s">
+        <v>785</v>
+      </c>
+      <c r="E42" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="G42" s="47"/>
+      <c r="H42" s="47"/>
+    </row>
+    <row r="43" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B43" s="37" t="s">
+        <v>786</v>
+      </c>
+      <c r="C43" s="37" t="s">
+        <v>769</v>
+      </c>
+      <c r="D43" s="37" t="s">
+        <v>752</v>
+      </c>
+      <c r="E43" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G43" s="38"/>
+      <c r="H43" s="38"/>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B44" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" s="31" t="s">
+        <v>787</v>
+      </c>
+      <c r="E44" s="31" t="s">
+        <v>788</v>
+      </c>
+      <c r="F44" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H44" s="31">
+        <v>1</v>
+      </c>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="3"/>
+      <c r="P44" s="39"/>
+      <c r="Q44" s="2"/>
+    </row>
+    <row r="45" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B45" s="37" t="s">
         <v>789</v>
       </c>
-      <c r="C42" s="37" t="s">
+      <c r="C45" s="37" t="s">
         <v>770</v>
       </c>
-      <c r="D42" s="37" t="s">
+      <c r="D45" s="37" t="s">
         <v>753</v>
       </c>
-      <c r="E42" s="37" t="s">
+      <c r="E45" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G42" s="38"/>
-      <c r="H42" s="38"/>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B43" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D43" s="31" t="s">
+      <c r="G45" s="38"/>
+      <c r="H45" s="38"/>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B46" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" s="31" t="s">
         <v>790</v>
       </c>
-      <c r="E43" s="31" t="s">
+      <c r="E46" s="31" t="s">
         <v>791</v>
       </c>
-      <c r="F43" s="31" t="s">
+      <c r="F46" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="H43" s="31">
+      <c r="H46" s="31">
         <v>1</v>
       </c>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="3"/>
-      <c r="P43" s="39"/>
-      <c r="Q43" s="2"/>
-    </row>
-    <row r="44" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="37" t="b">
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="3"/>
+      <c r="N46" s="3"/>
+      <c r="P46" s="39"/>
+      <c r="Q46" s="2"/>
+    </row>
+    <row r="47" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B44" s="37" t="s">
+      <c r="B47" s="37" t="s">
         <v>794</v>
       </c>
-      <c r="C44" s="37" t="s">
+      <c r="C47" s="37" t="s">
         <v>771</v>
       </c>
-      <c r="D44" s="37" t="s">
+      <c r="D47" s="37" t="s">
         <v>754</v>
       </c>
-      <c r="E44" s="37" t="s">
+      <c r="E47" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G44" s="38"/>
-      <c r="H44" s="38"/>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B45" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D45" s="31" t="s">
+      <c r="G47" s="38"/>
+      <c r="H47" s="38"/>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B48" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" s="31" t="s">
         <v>793</v>
       </c>
-      <c r="E45" s="31" t="s">
+      <c r="E48" s="31" t="s">
         <v>792</v>
       </c>
-      <c r="F45" s="31" t="s">
+      <c r="F48" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="H45" s="31">
+      <c r="H48" s="31">
         <v>1</v>
       </c>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
-      <c r="L45" s="3"/>
-      <c r="M45" s="3"/>
-      <c r="N45" s="3"/>
-      <c r="P45" s="39"/>
-      <c r="Q45" s="2"/>
-    </row>
-    <row r="46" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="37" t="b">
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+      <c r="M48" s="3"/>
+      <c r="N48" s="3"/>
+      <c r="P48" s="39"/>
+      <c r="Q48" s="2"/>
+    </row>
+    <row r="49" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B46" s="37" t="s">
+      <c r="B49" s="37" t="s">
         <v>795</v>
       </c>
-      <c r="C46" s="37" t="s">
+      <c r="C49" s="37" t="s">
         <v>772</v>
       </c>
-      <c r="D46" s="37" t="s">
+      <c r="D49" s="37" t="s">
         <v>755</v>
       </c>
-      <c r="E46" s="37" t="s">
+      <c r="E49" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G46" s="38"/>
-      <c r="H46" s="38"/>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B47" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D47" s="31" t="s">
+      <c r="G49" s="38"/>
+      <c r="H49" s="38"/>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B50" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D50" s="31" t="s">
         <v>797</v>
       </c>
-      <c r="E47" s="31" t="s">
+      <c r="E50" s="31" t="s">
         <v>796</v>
       </c>
-      <c r="F47" s="31" t="s">
+      <c r="F50" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="H47" s="31">
+      <c r="H50" s="31">
         <v>1</v>
       </c>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
-      <c r="L47" s="3"/>
-      <c r="M47" s="3"/>
-      <c r="N47" s="3"/>
-      <c r="P47" s="39"/>
-      <c r="Q47" s="2"/>
-    </row>
-    <row r="48" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="37" t="b">
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="3"/>
+      <c r="L50" s="3"/>
+      <c r="M50" s="3"/>
+      <c r="N50" s="3"/>
+      <c r="P50" s="39"/>
+      <c r="Q50" s="2"/>
+    </row>
+    <row r="51" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B48" s="37" t="s">
+      <c r="B51" s="37" t="s">
         <v>818</v>
       </c>
-      <c r="C48" s="37" t="s">
+      <c r="C51" s="37" t="s">
         <v>819</v>
       </c>
-      <c r="D48" s="37" t="s">
+      <c r="D51" s="37" t="s">
         <v>817</v>
       </c>
-      <c r="E48" s="37" t="s">
+      <c r="E51" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G48" s="38"/>
-      <c r="H48" s="38"/>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B49" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D49" s="31" t="s">
+      <c r="G51" s="38"/>
+      <c r="H51" s="38"/>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B52" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D52" s="31" t="s">
         <v>821</v>
       </c>
-      <c r="E49" s="31" t="s">
+      <c r="E52" s="31" t="s">
         <v>820</v>
       </c>
-      <c r="F49" s="31" t="s">
+      <c r="F52" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="H49" s="31">
+      <c r="H52" s="31">
         <v>1</v>
       </c>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
-      <c r="L49" s="3"/>
-      <c r="M49" s="3"/>
-      <c r="N49" s="3"/>
-      <c r="P49" s="39"/>
-      <c r="Q49" s="2"/>
-    </row>
-    <row r="50" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="37" t="b">
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
+      <c r="N52" s="3"/>
+      <c r="P52" s="39"/>
+      <c r="Q52" s="2"/>
+    </row>
+    <row r="53" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B50" s="37" t="s">
+      <c r="B53" s="37" t="s">
         <v>812</v>
       </c>
-      <c r="C50" s="37" t="s">
+      <c r="C53" s="37" t="s">
         <v>814</v>
       </c>
-      <c r="D50" s="37" t="s">
+      <c r="D53" s="37" t="s">
         <v>813</v>
       </c>
-      <c r="E50" s="37" t="s">
+      <c r="E53" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G50" s="38"/>
-      <c r="H50" s="38"/>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B51" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D51" s="31" t="s">
-        <v>816</v>
-      </c>
-      <c r="E51" s="31" t="s">
-        <v>815</v>
-      </c>
-      <c r="F51" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="H51" s="31">
-        <v>1</v>
-      </c>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
-      <c r="L51" s="3"/>
-      <c r="M51" s="3"/>
-      <c r="N51" s="3"/>
-      <c r="P51" s="39"/>
-      <c r="Q51" s="2"/>
-    </row>
-    <row r="52" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="B52" s="37" t="s">
-        <v>805</v>
-      </c>
-      <c r="C52" s="37" t="s">
-        <v>807</v>
-      </c>
-      <c r="D52" s="37" t="s">
-        <v>806</v>
-      </c>
-      <c r="E52" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G52" s="38"/>
-      <c r="H52" s="38"/>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B53" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D53" s="31" t="s">
-        <v>810</v>
-      </c>
-      <c r="E53" s="31" t="s">
-        <v>808</v>
-      </c>
-      <c r="F53" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="H53" s="31">
-        <v>1</v>
-      </c>
-      <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
-      <c r="K53" s="3"/>
-      <c r="L53" s="3"/>
-      <c r="M53" s="3"/>
-      <c r="N53" s="3"/>
-      <c r="P53" s="39"/>
-      <c r="Q53" s="2"/>
+      <c r="G53" s="38"/>
+      <c r="H53" s="38"/>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B54" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D54" s="31" t="s">
-        <v>811</v>
+        <v>816</v>
       </c>
       <c r="E54" s="31" t="s">
-        <v>809</v>
+        <v>815</v>
       </c>
       <c r="F54" s="31" t="s">
         <v>619</v>
@@ -8396,107 +8489,329 @@
       <c r="P54" s="39"/>
       <c r="Q54" s="2"/>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H55" s="31"/>
-      <c r="I55" s="31"/>
+    <row r="55" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B55" s="37" t="s">
+        <v>805</v>
+      </c>
+      <c r="C55" s="37" t="s">
+        <v>807</v>
+      </c>
+      <c r="D55" s="37" t="s">
+        <v>806</v>
+      </c>
+      <c r="E55" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G55" s="38"/>
+      <c r="H55" s="38"/>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H56" s="31"/>
-      <c r="I56" s="31"/>
+      <c r="B56" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D56" s="31" t="s">
+        <v>810</v>
+      </c>
+      <c r="E56" s="31" t="s">
+        <v>808</v>
+      </c>
+      <c r="F56" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H56" s="31">
+        <v>1</v>
+      </c>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
+      <c r="L56" s="3"/>
+      <c r="M56" s="3"/>
+      <c r="N56" s="3"/>
+      <c r="P56" s="39"/>
+      <c r="Q56" s="2"/>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H57" s="31"/>
-      <c r="I57" s="31"/>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H58" s="31"/>
-      <c r="I58" s="31"/>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H59" s="31"/>
-      <c r="I59" s="31"/>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H60" s="31"/>
-      <c r="I60" s="31"/>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H61" s="31"/>
-      <c r="I61" s="31"/>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H62" s="31"/>
-      <c r="I62" s="31"/>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H63" s="31"/>
-      <c r="I63" s="31"/>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H64" s="31"/>
-      <c r="I64" s="31"/>
-    </row>
-    <row r="65" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H65" s="31"/>
-      <c r="I65" s="31"/>
-    </row>
-    <row r="66" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H66" s="31"/>
-      <c r="I66" s="31"/>
-    </row>
-    <row r="67" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H67" s="31"/>
-      <c r="I67" s="31"/>
-    </row>
-    <row r="68" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H68" s="31"/>
-      <c r="I68" s="31"/>
-    </row>
-    <row r="69" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="B57" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D57" s="31" t="s">
+        <v>811</v>
+      </c>
+      <c r="E57" s="31" t="s">
+        <v>809</v>
+      </c>
+      <c r="F57" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H57" s="31">
+        <v>1</v>
+      </c>
+      <c r="I57" s="3"/>
+      <c r="J57" s="3"/>
+      <c r="K57" s="3"/>
+      <c r="L57" s="3"/>
+      <c r="M57" s="3"/>
+      <c r="N57" s="3"/>
+      <c r="P57" s="39"/>
+      <c r="Q57" s="2"/>
+    </row>
+    <row r="58" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="37" t="b">
+        <v>0</v>
+      </c>
+      <c r="B58" s="37" t="s">
+        <v>833</v>
+      </c>
+      <c r="C58" s="37" t="s">
+        <v>834</v>
+      </c>
+      <c r="D58" s="37" t="s">
+        <v>835</v>
+      </c>
+      <c r="E58" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G58" s="38"/>
+      <c r="H58" s="38"/>
+    </row>
+    <row r="59" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="37" t="b">
+        <v>0</v>
+      </c>
+      <c r="B59" s="37" t="s">
+        <v>836</v>
+      </c>
+      <c r="C59" s="37" t="s">
+        <v>837</v>
+      </c>
+      <c r="D59" s="37" t="s">
+        <v>838</v>
+      </c>
+      <c r="E59" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G59" s="38"/>
+      <c r="H59" s="38"/>
+    </row>
+    <row r="60" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="37" t="b">
+        <v>0</v>
+      </c>
+      <c r="B60" s="37" t="s">
+        <v>832</v>
+      </c>
+      <c r="C60" s="37" t="s">
+        <v>830</v>
+      </c>
+      <c r="D60" s="37" t="s">
+        <v>831</v>
+      </c>
+      <c r="E60" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G60" s="38"/>
+      <c r="H60" s="38"/>
+    </row>
+    <row r="61" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="37" t="b">
+        <v>0</v>
+      </c>
+      <c r="B61" s="37" t="s">
+        <v>839</v>
+      </c>
+      <c r="C61" s="37" t="s">
+        <v>840</v>
+      </c>
+      <c r="D61" s="37" t="s">
+        <v>841</v>
+      </c>
+      <c r="E61" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G61" s="38"/>
+      <c r="H61" s="38"/>
+    </row>
+    <row r="62" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="37" t="b">
+        <v>0</v>
+      </c>
+      <c r="B62" s="37" t="s">
+        <v>842</v>
+      </c>
+      <c r="C62" s="37" t="s">
+        <v>843</v>
+      </c>
+      <c r="D62" s="37" t="s">
+        <v>844</v>
+      </c>
+      <c r="E62" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G62" s="38"/>
+      <c r="H62" s="38"/>
+    </row>
+    <row r="63" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="37" t="b">
+        <v>0</v>
+      </c>
+      <c r="B63" s="37" t="s">
+        <v>845</v>
+      </c>
+      <c r="C63" s="37" t="s">
+        <v>846</v>
+      </c>
+      <c r="D63" s="37" t="s">
+        <v>847</v>
+      </c>
+      <c r="E63" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G63" s="38"/>
+      <c r="H63" s="38"/>
+    </row>
+    <row r="64" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="37" t="b">
+        <v>0</v>
+      </c>
+      <c r="B64" s="37" t="s">
+        <v>848</v>
+      </c>
+      <c r="C64" s="37" t="s">
+        <v>849</v>
+      </c>
+      <c r="D64" s="37" t="s">
+        <v>850</v>
+      </c>
+      <c r="E64" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G64" s="38"/>
+      <c r="H64" s="38"/>
+    </row>
+    <row r="65" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="37" t="b">
+        <v>0</v>
+      </c>
+      <c r="B65" s="37" t="s">
+        <v>851</v>
+      </c>
+      <c r="C65" s="37" t="s">
+        <v>852</v>
+      </c>
+      <c r="D65" s="37" t="s">
+        <v>853</v>
+      </c>
+      <c r="E65" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G65" s="38"/>
+      <c r="H65" s="38"/>
+    </row>
+    <row r="66" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="37" t="b">
+        <v>0</v>
+      </c>
+      <c r="B66" s="37" t="s">
+        <v>854</v>
+      </c>
+      <c r="C66" s="37" t="s">
+        <v>855</v>
+      </c>
+      <c r="D66" s="37" t="s">
+        <v>856</v>
+      </c>
+      <c r="E66" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G66" s="38"/>
+      <c r="H66" s="38"/>
+    </row>
+    <row r="67" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="37" t="b">
+        <v>0</v>
+      </c>
+      <c r="B67" s="37" t="s">
+        <v>857</v>
+      </c>
+      <c r="C67" s="37" t="s">
+        <v>858</v>
+      </c>
+      <c r="D67" s="37" t="s">
+        <v>859</v>
+      </c>
+      <c r="E67" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G67" s="38"/>
+      <c r="H67" s="38"/>
+    </row>
+    <row r="68" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="37" t="b">
+        <v>0</v>
+      </c>
+      <c r="B68" s="37" t="s">
+        <v>860</v>
+      </c>
+      <c r="C68" s="37" t="s">
+        <v>861</v>
+      </c>
+      <c r="D68" s="37" t="s">
+        <v>862</v>
+      </c>
+      <c r="E68" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G68" s="38"/>
+      <c r="H68" s="38"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H69" s="31"/>
       <c r="I69" s="31"/>
     </row>
-    <row r="70" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H70" s="31"/>
       <c r="I70" s="31"/>
     </row>
-    <row r="71" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H71" s="31"/>
       <c r="I71" s="31"/>
     </row>
-    <row r="72" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H72" s="31"/>
       <c r="I72" s="31"/>
     </row>
-    <row r="73" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H73" s="31"/>
       <c r="I73" s="31"/>
     </row>
-    <row r="74" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H74" s="31"/>
       <c r="I74" s="31"/>
     </row>
-    <row r="75" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H75" s="31"/>
       <c r="I75" s="31"/>
     </row>
-    <row r="76" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H76" s="31"/>
       <c r="I76" s="31"/>
     </row>
-    <row r="77" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H77" s="31"/>
       <c r="I77" s="31"/>
     </row>
-    <row r="78" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H78" s="31"/>
       <c r="I78" s="31"/>
     </row>
-    <row r="79" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H79" s="31"/>
       <c r="I79" s="31"/>
     </row>
-    <row r="80" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H80" s="31"/>
       <c r="I80" s="31"/>
     </row>
@@ -8677,7 +8992,7 @@
       <c r="I124" s="31"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:Z47"/>
+  <autoFilter ref="A2:Z50"/>
   <mergeCells count="1">
     <mergeCell ref="T1:Y1"/>
   </mergeCells>

</xml_diff>

<commit_message>
needed to add gas schedule
used copy of elec equip schedule
</commit_message>
<xml_diff>
--- a/projects/m0.xlsx
+++ b/projects/m0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="660" windowWidth="24720" windowHeight="12165" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="660" windowWidth="24720" windowHeight="12165" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -1903,9 +1903,6 @@
     <t>double</t>
   </si>
   <si>
-    <t>retail</t>
-  </si>
-  <si>
     <t>0.3.0</t>
   </si>
   <si>
@@ -1999,9 +1996,6 @@
     <t>single_run</t>
   </si>
   <si>
-    <t>../seeds/EmptySeedModel.osm</t>
-  </si>
-  <si>
     <t>Directory</t>
   </si>
   <si>
@@ -2633,6 +2627,12 @@
   </si>
   <si>
     <t>SysType 3</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>../seeds/ScheduleSetSeedModel_temp.osm</t>
   </si>
 </sst>
 </file>
@@ -4699,11 +4699,11 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1801">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -6841,8 +6841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6878,7 +6878,7 @@
         <v>436</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>437</v>
@@ -6889,7 +6889,7 @@
         <v>456</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>457</v>
@@ -6900,7 +6900,7 @@
         <v>469</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>614</v>
@@ -6982,7 +6982,7 @@
         <v>39</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>471</v>
@@ -6993,10 +6993,10 @@
         <v>25</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -7004,10 +7004,10 @@
         <v>26</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -7072,7 +7072,7 @@
         <v>451</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -7161,7 +7161,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>31</v>
@@ -7174,7 +7174,7 @@
         <v>29</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -7188,7 +7188,7 @@
         <v>38</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="E39" s="13" t="s">
         <v>449</v>
@@ -7199,13 +7199,13 @@
         <v>32</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>652</v>
+        <v>863</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>620</v>
+        <v>862</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -7216,7 +7216,7 @@
         <v>34</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="13" t="s">
@@ -7225,13 +7225,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -7264,7 +7264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
@@ -7320,14 +7320,14 @@
       <c r="Q1" s="5"/>
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
-      <c r="T1" s="49" t="s">
+      <c r="T1" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="U1" s="49"/>
-      <c r="V1" s="49"/>
-      <c r="W1" s="49"/>
-      <c r="X1" s="49"/>
-      <c r="Y1" s="49"/>
+      <c r="U1" s="51"/>
+      <c r="V1" s="51"/>
+      <c r="W1" s="51"/>
+      <c r="X1" s="51"/>
+      <c r="Y1" s="51"/>
     </row>
     <row r="2" spans="1:25" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -7424,13 +7424,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>68</v>
@@ -7443,16 +7443,16 @@
         <v>21</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="F5" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="6" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -7460,16 +7460,16 @@
         <v>21</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="F6" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H6" s="31" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
     </row>
     <row r="7" spans="1:25" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -7477,13 +7477,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="E7" s="37" t="s">
         <v>68</v>
@@ -7496,16 +7496,16 @@
         <v>21</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="F8" s="31" t="s">
         <v>618</v>
       </c>
       <c r="H8" s="31" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
@@ -7521,10 +7521,10 @@
         <v>21</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="F9" s="31" t="s">
         <v>619</v>
@@ -7544,13 +7544,13 @@
         <v>21</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="F10" s="31" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="H10" s="31" t="b">
         <v>1</v>
@@ -7562,16 +7562,16 @@
         <v>21</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="E11" s="31" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="F11" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H11" s="31" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="I11" s="31"/>
     </row>
@@ -7580,13 +7580,13 @@
         <v>1</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="E12" s="37" t="s">
         <v>68</v>
@@ -7599,16 +7599,16 @@
         <v>21</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="F13" s="31" t="s">
         <v>618</v>
       </c>
       <c r="H13" s="31" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
@@ -7624,10 +7624,10 @@
         <v>21</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="F14" s="31" t="s">
         <v>619</v>
@@ -7647,13 +7647,13 @@
         <v>21</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="F15" s="31" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="H15" s="31" t="b">
         <v>0</v>
@@ -7665,16 +7665,16 @@
         <v>21</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="F16" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H16" s="31" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="I16" s="31"/>
     </row>
@@ -7683,13 +7683,13 @@
         <v>1</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="D17" s="37" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="E17" s="37" t="s">
         <v>68</v>
@@ -7702,16 +7702,16 @@
         <v>21</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="F18" s="31" t="s">
         <v>618</v>
       </c>
       <c r="H18" s="31" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
@@ -7727,10 +7727,10 @@
         <v>21</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="E19" s="31" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="F19" s="31" t="s">
         <v>619</v>
@@ -7750,13 +7750,13 @@
         <v>21</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="E20" s="31" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="F20" s="31" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="H20" s="31" t="b">
         <v>0</v>
@@ -7768,16 +7768,16 @@
         <v>21</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="E21" s="31" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="F21" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H21" s="31" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="I21" s="31"/>
     </row>
@@ -7786,13 +7786,13 @@
         <v>1</v>
       </c>
       <c r="B22" s="37" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="C22" s="37" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="D22" s="37" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="E22" s="37" t="s">
         <v>68</v>
@@ -7805,13 +7805,13 @@
         <v>21</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="E23" s="31" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="F23" s="31" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="H23" s="31">
         <v>999999</v>
@@ -7830,16 +7830,16 @@
         <v>21</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="E24" s="31" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="F24" s="31" t="s">
         <v>619</v>
       </c>
       <c r="G24" s="31" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="H24" s="4">
         <v>10</v>
@@ -7856,16 +7856,16 @@
         <v>21</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="E25" s="31" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="F25" s="31" t="s">
         <v>619</v>
       </c>
       <c r="G25" s="31" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="H25" s="4">
         <v>10</v>
@@ -7877,10 +7877,10 @@
         <v>21</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="E26" s="31" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="F26" s="31" t="s">
         <v>619</v>
@@ -7895,10 +7895,10 @@
         <v>21</v>
       </c>
       <c r="D27" s="48" t="s">
+        <v>777</v>
+      </c>
+      <c r="E27" s="48" t="s">
         <v>779</v>
-      </c>
-      <c r="E27" s="48" t="s">
-        <v>781</v>
       </c>
       <c r="F27" s="31" t="s">
         <v>619</v>
@@ -7913,10 +7913,10 @@
         <v>21</v>
       </c>
       <c r="D28" s="48" t="s">
+        <v>778</v>
+      </c>
+      <c r="E28" s="48" t="s">
         <v>780</v>
-      </c>
-      <c r="E28" s="48" t="s">
-        <v>782</v>
       </c>
       <c r="F28" s="31" t="s">
         <v>619</v>
@@ -7931,13 +7931,13 @@
         <v>1</v>
       </c>
       <c r="B29" s="37" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="D29" s="37" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="E29" s="37" t="s">
         <v>68</v>
@@ -7950,10 +7950,10 @@
         <v>21</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E30" s="31" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="F30" s="31" t="s">
         <v>619</v>
@@ -7975,13 +7975,13 @@
         <v>1</v>
       </c>
       <c r="B31" s="37" t="s">
+        <v>761</v>
+      </c>
+      <c r="C31" s="37" t="s">
         <v>763</v>
       </c>
-      <c r="C31" s="37" t="s">
-        <v>765</v>
-      </c>
       <c r="D31" s="37" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="E31" s="37" t="s">
         <v>68</v>
@@ -7994,10 +7994,10 @@
         <v>21</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="E32" s="31" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F32" s="31" t="s">
         <v>619</v>
@@ -8019,13 +8019,13 @@
         <v>1</v>
       </c>
       <c r="B33" s="37" t="s">
+        <v>760</v>
+      </c>
+      <c r="C33" s="37" t="s">
         <v>762</v>
       </c>
-      <c r="C33" s="37" t="s">
-        <v>764</v>
-      </c>
       <c r="D33" s="37" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E33" s="37" t="s">
         <v>68</v>
@@ -8038,10 +8038,10 @@
         <v>21</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="E34" s="31" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="F34" s="31" t="s">
         <v>619</v>
@@ -8058,37 +8058,37 @@
       <c r="P34" s="39"/>
       <c r="Q34" s="2"/>
     </row>
-    <row r="35" spans="1:17" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="50" t="b">
+    <row r="35" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="49" t="b">
         <v>1</v>
       </c>
-      <c r="B35" s="50" t="s">
-        <v>826</v>
-      </c>
-      <c r="C35" s="50" t="s">
+      <c r="B35" s="49" t="s">
         <v>824</v>
       </c>
-      <c r="D35" s="50" t="s">
-        <v>825</v>
-      </c>
-      <c r="E35" s="50" t="s">
+      <c r="C35" s="49" t="s">
+        <v>822</v>
+      </c>
+      <c r="D35" s="49" t="s">
+        <v>823</v>
+      </c>
+      <c r="E35" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="G35" s="51"/>
-      <c r="H35" s="51"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="50"/>
     </row>
     <row r="36" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="37" t="b">
         <v>1</v>
       </c>
       <c r="B36" s="37" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="C36" s="37" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="D36" s="37" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="E36" s="37" t="s">
         <v>68</v>
@@ -8101,13 +8101,13 @@
         <v>1</v>
       </c>
       <c r="B37" s="37" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D37" s="37" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="E37" s="37" t="s">
         <v>68</v>
@@ -8120,10 +8120,10 @@
         <v>21</v>
       </c>
       <c r="D38" s="31" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="E38" s="31" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="F38" s="31" t="s">
         <v>619</v>
@@ -8145,13 +8145,13 @@
         <v>1</v>
       </c>
       <c r="B39" s="37" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="C39" s="37" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="D39" s="37" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="E39" s="37" t="s">
         <v>68</v>
@@ -8164,7 +8164,7 @@
         <v>1</v>
       </c>
       <c r="B40" s="37" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="C40" s="37" t="s">
         <v>74</v>
@@ -8192,7 +8192,7 @@
         <v>619</v>
       </c>
       <c r="G41" s="31" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="H41" s="31">
         <v>0</v>
@@ -8211,13 +8211,13 @@
         <v>1</v>
       </c>
       <c r="B42" s="46" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="C42" s="46" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D42" s="46" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="E42" s="46" t="s">
         <v>68</v>
@@ -8230,13 +8230,13 @@
         <v>1</v>
       </c>
       <c r="B43" s="37" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="C43" s="37" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="D43" s="37" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="E43" s="37" t="s">
         <v>68</v>
@@ -8249,10 +8249,10 @@
         <v>21</v>
       </c>
       <c r="D44" s="31" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="E44" s="31" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="F44" s="31" t="s">
         <v>619</v>
@@ -8274,13 +8274,13 @@
         <v>1</v>
       </c>
       <c r="B45" s="37" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="C45" s="37" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="D45" s="37" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="E45" s="37" t="s">
         <v>68</v>
@@ -8293,10 +8293,10 @@
         <v>21</v>
       </c>
       <c r="D46" s="31" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="E46" s="31" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="F46" s="31" t="s">
         <v>619</v>
@@ -8318,13 +8318,13 @@
         <v>1</v>
       </c>
       <c r="B47" s="37" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C47" s="37" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="D47" s="37" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="E47" s="37" t="s">
         <v>68</v>
@@ -8337,10 +8337,10 @@
         <v>21</v>
       </c>
       <c r="D48" s="31" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="E48" s="31" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="F48" s="31" t="s">
         <v>619</v>
@@ -8362,13 +8362,13 @@
         <v>1</v>
       </c>
       <c r="B49" s="37" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="C49" s="37" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="D49" s="37" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="E49" s="37" t="s">
         <v>68</v>
@@ -8381,10 +8381,10 @@
         <v>21</v>
       </c>
       <c r="D50" s="31" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="E50" s="31" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="F50" s="31" t="s">
         <v>619</v>
@@ -8406,13 +8406,13 @@
         <v>1</v>
       </c>
       <c r="B51" s="37" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="C51" s="37" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="D51" s="37" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="E51" s="37" t="s">
         <v>68</v>
@@ -8425,10 +8425,10 @@
         <v>21</v>
       </c>
       <c r="D52" s="31" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E52" s="31" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="F52" s="31" t="s">
         <v>619</v>
@@ -8450,13 +8450,13 @@
         <v>1</v>
       </c>
       <c r="B53" s="37" t="s">
+        <v>810</v>
+      </c>
+      <c r="C53" s="37" t="s">
         <v>812</v>
       </c>
-      <c r="C53" s="37" t="s">
-        <v>814</v>
-      </c>
       <c r="D53" s="37" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="E53" s="37" t="s">
         <v>68</v>
@@ -8469,10 +8469,10 @@
         <v>21</v>
       </c>
       <c r="D54" s="31" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="E54" s="31" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="F54" s="31" t="s">
         <v>619</v>
@@ -8494,13 +8494,13 @@
         <v>1</v>
       </c>
       <c r="B55" s="37" t="s">
+        <v>803</v>
+      </c>
+      <c r="C55" s="37" t="s">
         <v>805</v>
       </c>
-      <c r="C55" s="37" t="s">
-        <v>807</v>
-      </c>
       <c r="D55" s="37" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="E55" s="37" t="s">
         <v>68</v>
@@ -8513,10 +8513,10 @@
         <v>21</v>
       </c>
       <c r="D56" s="31" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="E56" s="31" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="F56" s="31" t="s">
         <v>619</v>
@@ -8538,10 +8538,10 @@
         <v>21</v>
       </c>
       <c r="D57" s="31" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="E57" s="31" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="F57" s="31" t="s">
         <v>619</v>
@@ -8563,13 +8563,13 @@
         <v>0</v>
       </c>
       <c r="B58" s="37" t="s">
+        <v>831</v>
+      </c>
+      <c r="C58" s="37" t="s">
+        <v>832</v>
+      </c>
+      <c r="D58" s="37" t="s">
         <v>833</v>
-      </c>
-      <c r="C58" s="37" t="s">
-        <v>834</v>
-      </c>
-      <c r="D58" s="37" t="s">
-        <v>835</v>
       </c>
       <c r="E58" s="37" t="s">
         <v>68</v>
@@ -8582,13 +8582,13 @@
         <v>0</v>
       </c>
       <c r="B59" s="37" t="s">
+        <v>834</v>
+      </c>
+      <c r="C59" s="37" t="s">
+        <v>835</v>
+      </c>
+      <c r="D59" s="37" t="s">
         <v>836</v>
-      </c>
-      <c r="C59" s="37" t="s">
-        <v>837</v>
-      </c>
-      <c r="D59" s="37" t="s">
-        <v>838</v>
       </c>
       <c r="E59" s="37" t="s">
         <v>68</v>
@@ -8601,13 +8601,13 @@
         <v>0</v>
       </c>
       <c r="B60" s="37" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="C60" s="37" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="D60" s="37" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="E60" s="37" t="s">
         <v>68</v>
@@ -8620,13 +8620,13 @@
         <v>0</v>
       </c>
       <c r="B61" s="37" t="s">
+        <v>837</v>
+      </c>
+      <c r="C61" s="37" t="s">
+        <v>838</v>
+      </c>
+      <c r="D61" s="37" t="s">
         <v>839</v>
-      </c>
-      <c r="C61" s="37" t="s">
-        <v>840</v>
-      </c>
-      <c r="D61" s="37" t="s">
-        <v>841</v>
       </c>
       <c r="E61" s="37" t="s">
         <v>68</v>
@@ -8639,13 +8639,13 @@
         <v>0</v>
       </c>
       <c r="B62" s="37" t="s">
+        <v>840</v>
+      </c>
+      <c r="C62" s="37" t="s">
+        <v>841</v>
+      </c>
+      <c r="D62" s="37" t="s">
         <v>842</v>
-      </c>
-      <c r="C62" s="37" t="s">
-        <v>843</v>
-      </c>
-      <c r="D62" s="37" t="s">
-        <v>844</v>
       </c>
       <c r="E62" s="37" t="s">
         <v>68</v>
@@ -8658,13 +8658,13 @@
         <v>0</v>
       </c>
       <c r="B63" s="37" t="s">
+        <v>843</v>
+      </c>
+      <c r="C63" s="37" t="s">
+        <v>844</v>
+      </c>
+      <c r="D63" s="37" t="s">
         <v>845</v>
-      </c>
-      <c r="C63" s="37" t="s">
-        <v>846</v>
-      </c>
-      <c r="D63" s="37" t="s">
-        <v>847</v>
       </c>
       <c r="E63" s="37" t="s">
         <v>68</v>
@@ -8677,13 +8677,13 @@
         <v>0</v>
       </c>
       <c r="B64" s="37" t="s">
+        <v>846</v>
+      </c>
+      <c r="C64" s="37" t="s">
+        <v>847</v>
+      </c>
+      <c r="D64" s="37" t="s">
         <v>848</v>
-      </c>
-      <c r="C64" s="37" t="s">
-        <v>849</v>
-      </c>
-      <c r="D64" s="37" t="s">
-        <v>850</v>
       </c>
       <c r="E64" s="37" t="s">
         <v>68</v>
@@ -8696,13 +8696,13 @@
         <v>0</v>
       </c>
       <c r="B65" s="37" t="s">
+        <v>849</v>
+      </c>
+      <c r="C65" s="37" t="s">
+        <v>850</v>
+      </c>
+      <c r="D65" s="37" t="s">
         <v>851</v>
-      </c>
-      <c r="C65" s="37" t="s">
-        <v>852</v>
-      </c>
-      <c r="D65" s="37" t="s">
-        <v>853</v>
       </c>
       <c r="E65" s="37" t="s">
         <v>68</v>
@@ -8715,13 +8715,13 @@
         <v>0</v>
       </c>
       <c r="B66" s="37" t="s">
+        <v>852</v>
+      </c>
+      <c r="C66" s="37" t="s">
+        <v>853</v>
+      </c>
+      <c r="D66" s="37" t="s">
         <v>854</v>
-      </c>
-      <c r="C66" s="37" t="s">
-        <v>855</v>
-      </c>
-      <c r="D66" s="37" t="s">
-        <v>856</v>
       </c>
       <c r="E66" s="37" t="s">
         <v>68</v>
@@ -8734,13 +8734,13 @@
         <v>0</v>
       </c>
       <c r="B67" s="37" t="s">
+        <v>855</v>
+      </c>
+      <c r="C67" s="37" t="s">
+        <v>856</v>
+      </c>
+      <c r="D67" s="37" t="s">
         <v>857</v>
-      </c>
-      <c r="C67" s="37" t="s">
-        <v>858</v>
-      </c>
-      <c r="D67" s="37" t="s">
-        <v>859</v>
       </c>
       <c r="E67" s="37" t="s">
         <v>68</v>
@@ -8753,13 +8753,13 @@
         <v>0</v>
       </c>
       <c r="B68" s="37" t="s">
+        <v>858</v>
+      </c>
+      <c r="C68" s="37" t="s">
+        <v>859</v>
+      </c>
+      <c r="D68" s="37" t="s">
         <v>860</v>
-      </c>
-      <c r="C68" s="37" t="s">
-        <v>861</v>
-      </c>
-      <c r="D68" s="37" t="s">
-        <v>862</v>
       </c>
       <c r="E68" s="37" t="s">
         <v>68</v>
@@ -9049,7 +9049,7 @@
         <v>459</v>
       </c>
       <c r="B2" s="44" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C2" s="43" t="s">
         <v>460</v>
@@ -9061,38 +9061,38 @@
         <v>11</v>
       </c>
       <c r="F2" s="43" t="s">
+        <v>622</v>
+      </c>
+      <c r="G2" s="43" t="s">
         <v>623</v>
       </c>
-      <c r="G2" s="43" t="s">
+      <c r="H2" s="43" t="s">
         <v>624</v>
       </c>
-      <c r="H2" s="43" t="s">
+      <c r="I2" s="43" t="s">
         <v>625</v>
       </c>
-      <c r="I2" s="43" t="s">
+      <c r="J2" s="43" t="s">
         <v>626</v>
       </c>
-      <c r="J2" s="43" t="s">
+      <c r="K2" s="43" t="s">
         <v>627</v>
-      </c>
-      <c r="K2" s="43" t="s">
-        <v>628</v>
       </c>
       <c r="L2" s="43"/>
     </row>
     <row r="3" spans="1:12" s="14" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="44" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D3" s="44"/>
       <c r="E3" s="44" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="F3" s="44" t="s">
         <v>461</v>
@@ -9110,21 +9110,21 @@
         <v>619</v>
       </c>
       <c r="K3" s="44" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="L3" s="44" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="40" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D4" s="40" t="s">
         <v>468</v>
@@ -9148,13 +9148,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="40" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D5" s="40" t="s">
         <v>468</v>
@@ -9178,13 +9178,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="40" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D6" s="40" t="s">
         <v>468</v>
@@ -9208,13 +9208,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="40" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D7" s="40" t="s">
         <v>468</v>
@@ -9238,11 +9238,11 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="40" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B8" s="40"/>
       <c r="C8" s="40" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="D8" s="40" t="s">
         <v>468</v>
@@ -9266,11 +9266,11 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="40" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B9" s="40"/>
       <c r="C9" s="40" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="D9" s="40" t="s">
         <v>468</v>
@@ -9294,11 +9294,11 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="40" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="B10" s="40"/>
       <c r="C10" s="40" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="D10" s="40" t="s">
         <v>468</v>
@@ -9322,11 +9322,11 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="B11" s="40"/>
       <c r="C11" s="40" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="D11" s="40" t="s">
         <v>468</v>
@@ -9350,11 +9350,11 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="B12" s="40"/>
       <c r="C12" s="40" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="D12" s="40" t="s">
         <v>468</v>
@@ -9378,11 +9378,11 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="40" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="B13" s="40"/>
       <c r="C13" s="40" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="D13" s="40" t="s">
         <v>468</v>
@@ -9406,11 +9406,11 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="40" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="B14" s="40"/>
       <c r="C14" s="40" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="D14" s="40" t="s">
         <v>468</v>
@@ -9434,11 +9434,11 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="40" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="B15" s="40"/>
       <c r="C15" s="40" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="D15" s="40" t="s">
         <v>468</v>
@@ -9462,11 +9462,11 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="40" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="B16" s="40"/>
       <c r="C16" s="40" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="D16" s="40" t="s">
         <v>468</v>
@@ -9490,11 +9490,11 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="40" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="B17" s="40"/>
       <c r="C17" s="40" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="D17" s="40" t="s">
         <v>468</v>
@@ -9518,11 +9518,11 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="40" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="B18" s="40"/>
       <c r="C18" s="40" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="D18" s="40" t="s">
         <v>468</v>
@@ -9546,11 +9546,11 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="40" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="B19" s="40"/>
       <c r="C19" s="40" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="D19" s="40" t="s">
         <v>468</v>
@@ -9574,11 +9574,11 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="40" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="B20" s="40"/>
       <c r="C20" s="40" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="D20" s="40" t="s">
         <v>468</v>
@@ -9602,11 +9602,11 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="40" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="B21" s="40"/>
       <c r="C21" s="40" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="D21" s="40" t="s">
         <v>468</v>
@@ -9630,14 +9630,14 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="40" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="B22" s="40"/>
       <c r="C22" s="40" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="D22" s="40" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="E22" s="40" t="s">
         <v>64</v>
@@ -9658,14 +9658,14 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="40" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="B23" s="40"/>
       <c r="C23" s="40" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="D23" s="40" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="E23" s="40" t="s">
         <v>64</v>
@@ -9686,14 +9686,14 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="40" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="B24" s="40"/>
       <c r="C24" s="40" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="D24" s="40" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="E24" s="40" t="s">
         <v>64</v>
@@ -9714,14 +9714,14 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="40" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="B25" s="40"/>
       <c r="C25" s="40" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="D25" s="40" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="E25" s="40" t="s">
         <v>64</v>
@@ -9742,14 +9742,14 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="40" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B26" s="40"/>
       <c r="C26" s="40" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="D26" s="40" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="E26" s="40" t="s">
         <v>64</v>
@@ -9770,14 +9770,14 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="40" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B27" s="40"/>
       <c r="C27" s="40" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="D27" s="40" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="E27" s="40" t="s">
         <v>64</v>
@@ -9798,14 +9798,14 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="40" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B28" s="40"/>
       <c r="C28" s="40" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="D28" s="40" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="E28" s="40" t="s">
         <v>64</v>
@@ -9828,14 +9828,14 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="40" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="B29" s="40"/>
       <c r="C29" s="40" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="D29" s="40" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="E29" s="40" t="s">
         <v>64</v>
@@ -9858,14 +9858,14 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="40" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="B30" s="40"/>
       <c r="C30" s="40" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="D30" s="40" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="E30" s="40" t="s">
         <v>64</v>
@@ -9888,14 +9888,14 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="40" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="B31" s="40"/>
       <c r="C31" s="40" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="D31" s="40" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="E31" s="40" t="s">
         <v>64</v>
@@ -18591,7 +18591,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>557</v>

</xml_diff>

<commit_message>
turning on system 01 measure
</commit_message>
<xml_diff>
--- a/projects/m0.xlsx
+++ b/projects/m0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="660" windowWidth="24720" windowHeight="12165" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="660" windowWidth="24720" windowHeight="12165" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -2527,96 +2527,6 @@
     <t>hvac_system_type</t>
   </si>
   <si>
-    <t>add_system_03</t>
-  </si>
-  <si>
-    <t>AddSystem03</t>
-  </si>
-  <si>
-    <t>Add System 03</t>
-  </si>
-  <si>
-    <t>Add System 01</t>
-  </si>
-  <si>
-    <t>add_system_01</t>
-  </si>
-  <si>
-    <t>AddSystem01</t>
-  </si>
-  <si>
-    <t>Add System 02</t>
-  </si>
-  <si>
-    <t>add_system_02</t>
-  </si>
-  <si>
-    <t>AddSystem02</t>
-  </si>
-  <si>
-    <t>Add System 04</t>
-  </si>
-  <si>
-    <t>add_system_04</t>
-  </si>
-  <si>
-    <t>AddSystem04</t>
-  </si>
-  <si>
-    <t>Add System 05</t>
-  </si>
-  <si>
-    <t>add_system_05</t>
-  </si>
-  <si>
-    <t>AddSystem05</t>
-  </si>
-  <si>
-    <t>Add System 06</t>
-  </si>
-  <si>
-    <t>add_system_06</t>
-  </si>
-  <si>
-    <t>AddSystem06</t>
-  </si>
-  <si>
-    <t>Add System 07</t>
-  </si>
-  <si>
-    <t>add_system_07</t>
-  </si>
-  <si>
-    <t>AddSystem07</t>
-  </si>
-  <si>
-    <t>Add System 08</t>
-  </si>
-  <si>
-    <t>add_system_08</t>
-  </si>
-  <si>
-    <t>AddSystem08</t>
-  </si>
-  <si>
-    <t>Add System 09</t>
-  </si>
-  <si>
-    <t>add_system_09</t>
-  </si>
-  <si>
-    <t>AddSystem09</t>
-  </si>
-  <si>
-    <t>Add System 10</t>
-  </si>
-  <si>
-    <t>add_system_10</t>
-  </si>
-  <si>
-    <t>AddSystem10</t>
-  </si>
-  <si>
     <t>Add Service Water Heating Supply</t>
   </si>
   <si>
@@ -2626,13 +2536,103 @@
     <t>AddServiceWaterHeatingSupply</t>
   </si>
   <si>
-    <t>SysType 3</t>
-  </si>
-  <si>
     <t>na</t>
   </si>
   <si>
     <t>../seeds/ScheduleSetSeedModel_temp.osm</t>
+  </si>
+  <si>
+    <t>AddSystem01BySpaceType</t>
+  </si>
+  <si>
+    <t>AddSystem02BySpaceType</t>
+  </si>
+  <si>
+    <t>AddSystem03BySpaceType</t>
+  </si>
+  <si>
+    <t>AddSystem04BySpaceType</t>
+  </si>
+  <si>
+    <t>AddSystem05BySpaceType</t>
+  </si>
+  <si>
+    <t>AddSystem06BySpaceType</t>
+  </si>
+  <si>
+    <t>AddSystem07BySpaceType</t>
+  </si>
+  <si>
+    <t>AddSystem08BySpaceType</t>
+  </si>
+  <si>
+    <t>AddSystem09BySpaceType</t>
+  </si>
+  <si>
+    <t>AddSystem10BySpaceType</t>
+  </si>
+  <si>
+    <t>Add System 01 By Space Type</t>
+  </si>
+  <si>
+    <t>Add System 02 By Space Type</t>
+  </si>
+  <si>
+    <t>Add System 03 By Space Type</t>
+  </si>
+  <si>
+    <t>Add System 04 By Space Type</t>
+  </si>
+  <si>
+    <t>Add System 05 By Space Type</t>
+  </si>
+  <si>
+    <t>Add System 06 By Space Type</t>
+  </si>
+  <si>
+    <t>Add System 07 By Space Type</t>
+  </si>
+  <si>
+    <t>Add System 08 By Space Type</t>
+  </si>
+  <si>
+    <t>Add System 09 By Space Type</t>
+  </si>
+  <si>
+    <t>Add System 10 By Space Type</t>
+  </si>
+  <si>
+    <t>SysType 1</t>
+  </si>
+  <si>
+    <t>add_system01_by_space_type</t>
+  </si>
+  <si>
+    <t>add_system02_by_space_type</t>
+  </si>
+  <si>
+    <t>add_system03_by_space_type</t>
+  </si>
+  <si>
+    <t>add_system04_by_space_type</t>
+  </si>
+  <si>
+    <t>add_system05_by_space_type</t>
+  </si>
+  <si>
+    <t>add_system06_by_space_type</t>
+  </si>
+  <si>
+    <t>add_system07_by_space_type</t>
+  </si>
+  <si>
+    <t>add_system08_by_space_type</t>
+  </si>
+  <si>
+    <t>add_system09_by_space_type</t>
+  </si>
+  <si>
+    <t>add_system10_by_space_type</t>
   </si>
 </sst>
 </file>
@@ -6841,8 +6841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7202,10 +7202,10 @@
         <v>647</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>863</v>
+        <v>832</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>862</v>
+        <v>831</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -7262,11 +7262,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y124"/>
+  <dimension ref="A1:Y123"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7571,7 +7571,7 @@
         <v>104</v>
       </c>
       <c r="H11" s="31" t="s">
-        <v>861</v>
+        <v>853</v>
       </c>
       <c r="I11" s="31"/>
     </row>
@@ -7674,7 +7674,7 @@
         <v>104</v>
       </c>
       <c r="H16" s="31" t="s">
-        <v>861</v>
+        <v>853</v>
       </c>
       <c r="I16" s="31"/>
     </row>
@@ -7777,7 +7777,7 @@
         <v>104</v>
       </c>
       <c r="H21" s="31" t="s">
-        <v>861</v>
+        <v>853</v>
       </c>
       <c r="I21" s="31"/>
     </row>
@@ -8560,13 +8560,13 @@
     </row>
     <row r="58" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B58" s="37" t="s">
-        <v>831</v>
+        <v>843</v>
       </c>
       <c r="C58" s="37" t="s">
-        <v>832</v>
+        <v>854</v>
       </c>
       <c r="D58" s="37" t="s">
         <v>833</v>
@@ -8582,13 +8582,13 @@
         <v>0</v>
       </c>
       <c r="B59" s="37" t="s">
+        <v>844</v>
+      </c>
+      <c r="C59" s="37" t="s">
+        <v>855</v>
+      </c>
+      <c r="D59" s="37" t="s">
         <v>834</v>
-      </c>
-      <c r="C59" s="37" t="s">
-        <v>835</v>
-      </c>
-      <c r="D59" s="37" t="s">
-        <v>836</v>
       </c>
       <c r="E59" s="37" t="s">
         <v>68</v>
@@ -8601,13 +8601,13 @@
         <v>0</v>
       </c>
       <c r="B60" s="37" t="s">
-        <v>830</v>
+        <v>845</v>
       </c>
       <c r="C60" s="37" t="s">
-        <v>828</v>
+        <v>856</v>
       </c>
       <c r="D60" s="37" t="s">
-        <v>829</v>
+        <v>835</v>
       </c>
       <c r="E60" s="37" t="s">
         <v>68</v>
@@ -8620,13 +8620,13 @@
         <v>0</v>
       </c>
       <c r="B61" s="37" t="s">
-        <v>837</v>
+        <v>846</v>
       </c>
       <c r="C61" s="37" t="s">
-        <v>838</v>
+        <v>857</v>
       </c>
       <c r="D61" s="37" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
       <c r="E61" s="37" t="s">
         <v>68</v>
@@ -8639,13 +8639,13 @@
         <v>0</v>
       </c>
       <c r="B62" s="37" t="s">
-        <v>840</v>
+        <v>847</v>
       </c>
       <c r="C62" s="37" t="s">
-        <v>841</v>
+        <v>858</v>
       </c>
       <c r="D62" s="37" t="s">
-        <v>842</v>
+        <v>837</v>
       </c>
       <c r="E62" s="37" t="s">
         <v>68</v>
@@ -8658,13 +8658,13 @@
         <v>0</v>
       </c>
       <c r="B63" s="37" t="s">
-        <v>843</v>
+        <v>848</v>
       </c>
       <c r="C63" s="37" t="s">
-        <v>844</v>
+        <v>859</v>
       </c>
       <c r="D63" s="37" t="s">
-        <v>845</v>
+        <v>838</v>
       </c>
       <c r="E63" s="37" t="s">
         <v>68</v>
@@ -8677,13 +8677,13 @@
         <v>0</v>
       </c>
       <c r="B64" s="37" t="s">
-        <v>846</v>
+        <v>849</v>
       </c>
       <c r="C64" s="37" t="s">
-        <v>847</v>
+        <v>860</v>
       </c>
       <c r="D64" s="37" t="s">
-        <v>848</v>
+        <v>839</v>
       </c>
       <c r="E64" s="37" t="s">
         <v>68</v>
@@ -8696,13 +8696,13 @@
         <v>0</v>
       </c>
       <c r="B65" s="37" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="C65" s="37" t="s">
-        <v>850</v>
+        <v>861</v>
       </c>
       <c r="D65" s="37" t="s">
-        <v>851</v>
+        <v>840</v>
       </c>
       <c r="E65" s="37" t="s">
         <v>68</v>
@@ -8715,13 +8715,13 @@
         <v>0</v>
       </c>
       <c r="B66" s="37" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="C66" s="37" t="s">
-        <v>853</v>
+        <v>862</v>
       </c>
       <c r="D66" s="37" t="s">
-        <v>854</v>
+        <v>841</v>
       </c>
       <c r="E66" s="37" t="s">
         <v>68</v>
@@ -8734,13 +8734,13 @@
         <v>0</v>
       </c>
       <c r="B67" s="37" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
       <c r="C67" s="37" t="s">
-        <v>856</v>
+        <v>863</v>
       </c>
       <c r="D67" s="37" t="s">
-        <v>857</v>
+        <v>842</v>
       </c>
       <c r="E67" s="37" t="s">
         <v>68</v>
@@ -8753,13 +8753,13 @@
         <v>0</v>
       </c>
       <c r="B68" s="37" t="s">
-        <v>858</v>
+        <v>828</v>
       </c>
       <c r="C68" s="37" t="s">
-        <v>859</v>
+        <v>829</v>
       </c>
       <c r="D68" s="37" t="s">
-        <v>860</v>
+        <v>830</v>
       </c>
       <c r="E68" s="37" t="s">
         <v>68</v>
@@ -8986,10 +8986,6 @@
     <row r="123" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H123" s="31"/>
       <c r="I123" s="31"/>
-    </row>
-    <row r="124" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H124" s="31"/>
-      <c r="I124" s="31"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:Z50"/>

</xml_diff>

<commit_message>
updating spreadsheet and server version in settings
</commit_message>
<xml_diff>
--- a/projects/m0.xlsx
+++ b/projects/m0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="660" windowWidth="24720" windowHeight="12165" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="660" windowWidth="24720" windowHeight="12165" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -2203,9 +2203,6 @@
     <t>standard_reports.total_building_area</t>
   </si>
   <si>
-    <t>1.8.0-pre12</t>
-  </si>
-  <si>
     <t>../../../GitHub/cofee-measures/model0</t>
   </si>
   <si>
@@ -2633,6 +2630,9 @@
   </si>
   <si>
     <t>add_system10_by_space_type</t>
+  </si>
+  <si>
+    <t>1.8.0</t>
   </si>
 </sst>
 </file>
@@ -6841,8 +6841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6900,7 +6900,7 @@
         <v>469</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>720</v>
+        <v>863</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>614</v>
@@ -6993,7 +6993,7 @@
         <v>25</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>663</v>
@@ -7026,7 +7026,7 @@
         <v>463</v>
       </c>
       <c r="B16" s="24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>608</v>
@@ -7202,10 +7202,10 @@
         <v>647</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -7228,10 +7228,10 @@
         <v>651</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -7264,9 +7264,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C71" sqref="C71"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7469,7 +7469,7 @@
         <v>104</v>
       </c>
       <c r="H6" s="31" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="7" spans="1:25" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -7477,13 +7477,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="E7" s="37" t="s">
         <v>68</v>
@@ -7496,16 +7496,16 @@
         <v>21</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F8" s="31" t="s">
         <v>618</v>
       </c>
       <c r="H8" s="31" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
@@ -7521,10 +7521,10 @@
         <v>21</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="F9" s="31" t="s">
         <v>619</v>
@@ -7544,10 +7544,10 @@
         <v>21</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="F10" s="31" t="s">
         <v>621</v>
@@ -7562,16 +7562,16 @@
         <v>21</v>
       </c>
       <c r="D11" s="31" t="s">
+        <v>825</v>
+      </c>
+      <c r="E11" s="31" t="s">
         <v>826</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>827</v>
       </c>
       <c r="F11" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H11" s="31" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="I11" s="31"/>
     </row>
@@ -7580,13 +7580,13 @@
         <v>1</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="E12" s="37" t="s">
         <v>68</v>
@@ -7599,16 +7599,16 @@
         <v>21</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F13" s="31" t="s">
         <v>618</v>
       </c>
       <c r="H13" s="31" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
@@ -7624,10 +7624,10 @@
         <v>21</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="F14" s="31" t="s">
         <v>619</v>
@@ -7647,10 +7647,10 @@
         <v>21</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="F15" s="31" t="s">
         <v>621</v>
@@ -7665,16 +7665,16 @@
         <v>21</v>
       </c>
       <c r="D16" s="31" t="s">
+        <v>825</v>
+      </c>
+      <c r="E16" s="31" t="s">
         <v>826</v>
-      </c>
-      <c r="E16" s="31" t="s">
-        <v>827</v>
       </c>
       <c r="F16" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H16" s="31" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="I16" s="31"/>
     </row>
@@ -7683,13 +7683,13 @@
         <v>1</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D17" s="37" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="E17" s="37" t="s">
         <v>68</v>
@@ -7702,16 +7702,16 @@
         <v>21</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F18" s="31" t="s">
         <v>618</v>
       </c>
       <c r="H18" s="31" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
@@ -7727,10 +7727,10 @@
         <v>21</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="E19" s="31" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="F19" s="31" t="s">
         <v>619</v>
@@ -7750,10 +7750,10 @@
         <v>21</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E20" s="31" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="F20" s="31" t="s">
         <v>621</v>
@@ -7768,16 +7768,16 @@
         <v>21</v>
       </c>
       <c r="D21" s="31" t="s">
+        <v>825</v>
+      </c>
+      <c r="E21" s="31" t="s">
         <v>826</v>
-      </c>
-      <c r="E21" s="31" t="s">
-        <v>827</v>
       </c>
       <c r="F21" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H21" s="31" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="I21" s="31"/>
     </row>
@@ -7786,13 +7786,13 @@
         <v>1</v>
       </c>
       <c r="B22" s="37" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C22" s="37" t="s">
+        <v>731</v>
+      </c>
+      <c r="D22" s="37" t="s">
         <v>732</v>
-      </c>
-      <c r="D22" s="37" t="s">
-        <v>733</v>
       </c>
       <c r="E22" s="37" t="s">
         <v>68</v>
@@ -7805,10 +7805,10 @@
         <v>21</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E23" s="31" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="F23" s="31" t="s">
         <v>630</v>
@@ -7830,10 +7830,10 @@
         <v>21</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E24" s="31" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="F24" s="31" t="s">
         <v>619</v>
@@ -7856,10 +7856,10 @@
         <v>21</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E25" s="31" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="F25" s="31" t="s">
         <v>619</v>
@@ -7877,10 +7877,10 @@
         <v>21</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E26" s="31" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="F26" s="31" t="s">
         <v>619</v>
@@ -7895,10 +7895,10 @@
         <v>21</v>
       </c>
       <c r="D27" s="48" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="E27" s="48" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="F27" s="31" t="s">
         <v>619</v>
@@ -7913,10 +7913,10 @@
         <v>21</v>
       </c>
       <c r="D28" s="48" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="E28" s="48" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="F28" s="31" t="s">
         <v>619</v>
@@ -7931,13 +7931,13 @@
         <v>1</v>
       </c>
       <c r="B29" s="37" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="D29" s="37" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E29" s="37" t="s">
         <v>68</v>
@@ -7950,10 +7950,10 @@
         <v>21</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="E30" s="31" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="F30" s="31" t="s">
         <v>619</v>
@@ -7975,13 +7975,13 @@
         <v>1</v>
       </c>
       <c r="B31" s="37" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C31" s="37" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="D31" s="37" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E31" s="37" t="s">
         <v>68</v>
@@ -7994,10 +7994,10 @@
         <v>21</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E32" s="31" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="F32" s="31" t="s">
         <v>619</v>
@@ -8019,13 +8019,13 @@
         <v>1</v>
       </c>
       <c r="B33" s="37" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C33" s="37" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="D33" s="37" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="E33" s="37" t="s">
         <v>68</v>
@@ -8038,10 +8038,10 @@
         <v>21</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="E34" s="31" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="F34" s="31" t="s">
         <v>619</v>
@@ -8063,13 +8063,13 @@
         <v>1</v>
       </c>
       <c r="B35" s="49" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="C35" s="49" t="s">
+        <v>821</v>
+      </c>
+      <c r="D35" s="49" t="s">
         <v>822</v>
-      </c>
-      <c r="D35" s="49" t="s">
-        <v>823</v>
       </c>
       <c r="E35" s="49" t="s">
         <v>68</v>
@@ -8082,13 +8082,13 @@
         <v>1</v>
       </c>
       <c r="B36" s="37" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C36" s="37" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="D36" s="37" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E36" s="37" t="s">
         <v>68</v>
@@ -8101,13 +8101,13 @@
         <v>1</v>
       </c>
       <c r="B37" s="37" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="D37" s="37" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="E37" s="37" t="s">
         <v>68</v>
@@ -8120,10 +8120,10 @@
         <v>21</v>
       </c>
       <c r="D38" s="31" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="E38" s="31" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="F38" s="31" t="s">
         <v>619</v>
@@ -8145,13 +8145,13 @@
         <v>1</v>
       </c>
       <c r="B39" s="37" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="C39" s="37" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="D39" s="37" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E39" s="37" t="s">
         <v>68</v>
@@ -8192,7 +8192,7 @@
         <v>619</v>
       </c>
       <c r="G41" s="31" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="H41" s="31">
         <v>0</v>
@@ -8211,13 +8211,13 @@
         <v>1</v>
       </c>
       <c r="B42" s="46" t="s">
+        <v>781</v>
+      </c>
+      <c r="C42" s="46" t="s">
+        <v>765</v>
+      </c>
+      <c r="D42" s="46" t="s">
         <v>782</v>
-      </c>
-      <c r="C42" s="46" t="s">
-        <v>766</v>
-      </c>
-      <c r="D42" s="46" t="s">
-        <v>783</v>
       </c>
       <c r="E42" s="46" t="s">
         <v>68</v>
@@ -8230,13 +8230,13 @@
         <v>1</v>
       </c>
       <c r="B43" s="37" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="C43" s="37" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="D43" s="37" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="E43" s="37" t="s">
         <v>68</v>
@@ -8249,10 +8249,10 @@
         <v>21</v>
       </c>
       <c r="D44" s="31" t="s">
+        <v>784</v>
+      </c>
+      <c r="E44" s="31" t="s">
         <v>785</v>
-      </c>
-      <c r="E44" s="31" t="s">
-        <v>786</v>
       </c>
       <c r="F44" s="31" t="s">
         <v>619</v>
@@ -8274,13 +8274,13 @@
         <v>1</v>
       </c>
       <c r="B45" s="37" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="C45" s="37" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="D45" s="37" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="E45" s="37" t="s">
         <v>68</v>
@@ -8293,10 +8293,10 @@
         <v>21</v>
       </c>
       <c r="D46" s="31" t="s">
+        <v>787</v>
+      </c>
+      <c r="E46" s="31" t="s">
         <v>788</v>
-      </c>
-      <c r="E46" s="31" t="s">
-        <v>789</v>
       </c>
       <c r="F46" s="31" t="s">
         <v>619</v>
@@ -8318,13 +8318,13 @@
         <v>1</v>
       </c>
       <c r="B47" s="37" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="C47" s="37" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="D47" s="37" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="E47" s="37" t="s">
         <v>68</v>
@@ -8337,10 +8337,10 @@
         <v>21</v>
       </c>
       <c r="D48" s="31" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="E48" s="31" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="F48" s="31" t="s">
         <v>619</v>
@@ -8362,13 +8362,13 @@
         <v>1</v>
       </c>
       <c r="B49" s="37" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="C49" s="37" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="D49" s="37" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="E49" s="37" t="s">
         <v>68</v>
@@ -8381,10 +8381,10 @@
         <v>21</v>
       </c>
       <c r="D50" s="31" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E50" s="31" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F50" s="31" t="s">
         <v>619</v>
@@ -8406,13 +8406,13 @@
         <v>1</v>
       </c>
       <c r="B51" s="37" t="s">
+        <v>815</v>
+      </c>
+      <c r="C51" s="37" t="s">
         <v>816</v>
       </c>
-      <c r="C51" s="37" t="s">
-        <v>817</v>
-      </c>
       <c r="D51" s="37" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="E51" s="37" t="s">
         <v>68</v>
@@ -8425,10 +8425,10 @@
         <v>21</v>
       </c>
       <c r="D52" s="31" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E52" s="31" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="F52" s="31" t="s">
         <v>619</v>
@@ -8450,13 +8450,13 @@
         <v>1</v>
       </c>
       <c r="B53" s="37" t="s">
+        <v>809</v>
+      </c>
+      <c r="C53" s="37" t="s">
+        <v>811</v>
+      </c>
+      <c r="D53" s="37" t="s">
         <v>810</v>
-      </c>
-      <c r="C53" s="37" t="s">
-        <v>812</v>
-      </c>
-      <c r="D53" s="37" t="s">
-        <v>811</v>
       </c>
       <c r="E53" s="37" t="s">
         <v>68</v>
@@ -8469,10 +8469,10 @@
         <v>21</v>
       </c>
       <c r="D54" s="31" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E54" s="31" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="F54" s="31" t="s">
         <v>619</v>
@@ -8494,13 +8494,13 @@
         <v>1</v>
       </c>
       <c r="B55" s="37" t="s">
+        <v>802</v>
+      </c>
+      <c r="C55" s="37" t="s">
+        <v>804</v>
+      </c>
+      <c r="D55" s="37" t="s">
         <v>803</v>
-      </c>
-      <c r="C55" s="37" t="s">
-        <v>805</v>
-      </c>
-      <c r="D55" s="37" t="s">
-        <v>804</v>
       </c>
       <c r="E55" s="37" t="s">
         <v>68</v>
@@ -8513,10 +8513,10 @@
         <v>21</v>
       </c>
       <c r="D56" s="31" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E56" s="31" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="F56" s="31" t="s">
         <v>619</v>
@@ -8538,10 +8538,10 @@
         <v>21</v>
       </c>
       <c r="D57" s="31" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="E57" s="31" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="F57" s="31" t="s">
         <v>619</v>
@@ -8563,13 +8563,13 @@
         <v>1</v>
       </c>
       <c r="B58" s="37" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="C58" s="37" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="D58" s="37" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="E58" s="37" t="s">
         <v>68</v>
@@ -8582,13 +8582,13 @@
         <v>0</v>
       </c>
       <c r="B59" s="37" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C59" s="37" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="D59" s="37" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="E59" s="37" t="s">
         <v>68</v>
@@ -8601,13 +8601,13 @@
         <v>0</v>
       </c>
       <c r="B60" s="37" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C60" s="37" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="D60" s="37" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="E60" s="37" t="s">
         <v>68</v>
@@ -8620,13 +8620,13 @@
         <v>0</v>
       </c>
       <c r="B61" s="37" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="C61" s="37" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="D61" s="37" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="E61" s="37" t="s">
         <v>68</v>
@@ -8639,13 +8639,13 @@
         <v>0</v>
       </c>
       <c r="B62" s="37" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="C62" s="37" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="D62" s="37" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="E62" s="37" t="s">
         <v>68</v>
@@ -8658,13 +8658,13 @@
         <v>0</v>
       </c>
       <c r="B63" s="37" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="C63" s="37" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="D63" s="37" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="E63" s="37" t="s">
         <v>68</v>
@@ -8677,13 +8677,13 @@
         <v>0</v>
       </c>
       <c r="B64" s="37" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C64" s="37" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="D64" s="37" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="E64" s="37" t="s">
         <v>68</v>
@@ -8696,13 +8696,13 @@
         <v>0</v>
       </c>
       <c r="B65" s="37" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C65" s="37" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D65" s="37" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="E65" s="37" t="s">
         <v>68</v>
@@ -8715,13 +8715,13 @@
         <v>0</v>
       </c>
       <c r="B66" s="37" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="C66" s="37" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="D66" s="37" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="E66" s="37" t="s">
         <v>68</v>
@@ -8734,13 +8734,13 @@
         <v>0</v>
       </c>
       <c r="B67" s="37" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="C67" s="37" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="D67" s="37" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="E67" s="37" t="s">
         <v>68</v>
@@ -8753,13 +8753,13 @@
         <v>0</v>
       </c>
       <c r="B68" s="37" t="s">
+        <v>827</v>
+      </c>
+      <c r="C68" s="37" t="s">
         <v>828</v>
       </c>
-      <c r="C68" s="37" t="s">
+      <c r="D68" s="37" t="s">
         <v>829</v>
-      </c>
-      <c r="D68" s="37" t="s">
-        <v>830</v>
       </c>
       <c r="E68" s="37" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
adding system 2 and 3 to workflow
Each of the three space types now make system 1, 2 , and 3. To test more
hvac systems I'll have to try out different combinations of systems for
the space types.
</commit_message>
<xml_diff>
--- a/projects/m0.xlsx
+++ b/projects/m0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="660" windowWidth="24720" windowHeight="12165" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="720" windowWidth="14880" windowHeight="7425" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2415" uniqueCount="864">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2415" uniqueCount="866">
   <si>
     <t>type</t>
   </si>
@@ -2533,6 +2533,9 @@
     <t>AddServiceWaterHeatingSupply</t>
   </si>
   <si>
+    <t>SysType 3</t>
+  </si>
+  <si>
     <t>na</t>
   </si>
   <si>
@@ -2633,6 +2636,9 @@
   </si>
   <si>
     <t>1.8.0</t>
+  </si>
+  <si>
+    <t>SysType 2</t>
   </si>
 </sst>
 </file>
@@ -6841,8 +6847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6900,7 +6906,7 @@
         <v>469</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>614</v>
@@ -7202,10 +7208,10 @@
         <v>647</v>
       </c>
       <c r="D40" s="31" t="s">
+        <v>832</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>831</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>830</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -7264,9 +7270,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y123"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7571,7 +7577,7 @@
         <v>104</v>
       </c>
       <c r="H11" s="31" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="I11" s="31"/>
     </row>
@@ -7674,7 +7680,7 @@
         <v>104</v>
       </c>
       <c r="H16" s="31" t="s">
-        <v>852</v>
+        <v>830</v>
       </c>
       <c r="I16" s="31"/>
     </row>
@@ -7777,7 +7783,7 @@
         <v>104</v>
       </c>
       <c r="H21" s="31" t="s">
-        <v>852</v>
+        <v>865</v>
       </c>
       <c r="I21" s="31"/>
     </row>
@@ -8563,13 +8569,13 @@
         <v>1</v>
       </c>
       <c r="B58" s="37" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="C58" s="37" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="D58" s="37" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="E58" s="37" t="s">
         <v>68</v>
@@ -8579,16 +8585,16 @@
     </row>
     <row r="59" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B59" s="37" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="C59" s="37" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="D59" s="37" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="E59" s="37" t="s">
         <v>68</v>
@@ -8598,16 +8604,16 @@
     </row>
     <row r="60" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B60" s="37" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="C60" s="37" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="D60" s="37" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="E60" s="37" t="s">
         <v>68</v>
@@ -8620,13 +8626,13 @@
         <v>0</v>
       </c>
       <c r="B61" s="37" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="C61" s="37" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="D61" s="37" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="E61" s="37" t="s">
         <v>68</v>
@@ -8639,13 +8645,13 @@
         <v>0</v>
       </c>
       <c r="B62" s="37" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="C62" s="37" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="D62" s="37" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="E62" s="37" t="s">
         <v>68</v>
@@ -8658,13 +8664,13 @@
         <v>0</v>
       </c>
       <c r="B63" s="37" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="C63" s="37" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D63" s="37" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="E63" s="37" t="s">
         <v>68</v>
@@ -8677,13 +8683,13 @@
         <v>0</v>
       </c>
       <c r="B64" s="37" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C64" s="37" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="D64" s="37" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="E64" s="37" t="s">
         <v>68</v>
@@ -8696,13 +8702,13 @@
         <v>0</v>
       </c>
       <c r="B65" s="37" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="C65" s="37" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="D65" s="37" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="E65" s="37" t="s">
         <v>68</v>
@@ -8715,13 +8721,13 @@
         <v>0</v>
       </c>
       <c r="B66" s="37" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="C66" s="37" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="D66" s="37" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="E66" s="37" t="s">
         <v>68</v>
@@ -8734,13 +8740,13 @@
         <v>0</v>
       </c>
       <c r="B67" s="37" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="C67" s="37" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="D67" s="37" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="E67" s="37" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
turning on service water heating supply measure
I have hard coded logic for now to make this NaturalGas, but if it is in
analytic record I can pull from there.
</commit_message>
<xml_diff>
--- a/projects/m0.xlsx
+++ b/projects/m0.xlsx
@@ -7271,8 +7271,8 @@
   <dimension ref="A1:Y123"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B76" sqref="B76"/>
+      <pane ySplit="3" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8756,7 +8756,7 @@
     </row>
     <row r="68" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B68" s="37" t="s">
         <v>827</v>

</xml_diff>

<commit_message>
adding place holder to make schedules
I only want to go through OSM file once vs. each time I need the
schedules. When this is ready hoo arguments will move to this from space
type ratios.
</commit_message>
<xml_diff>
--- a/projects/m0.xlsx
+++ b/projects/m0.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$53</definedName>
     <definedName name="AnalysisType">Lookups!$A$17:$A$23</definedName>
     <definedName name="instance_defs">Lookups!$A$2:$D$9</definedName>
     <definedName name="instance_types">Lookups!$A$2:$A$9</definedName>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2415" uniqueCount="866">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2427" uniqueCount="869">
   <si>
     <t>type</t>
   </si>
@@ -2639,13 +2639,22 @@
   </si>
   <si>
     <t>SysType 2</t>
+  </si>
+  <si>
+    <t>Add Schedules to Model</t>
+  </si>
+  <si>
+    <t>add_schedules_to_model</t>
+  </si>
+  <si>
+    <t>AddSchedulesToModel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2724,6 +2733,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -4609,7 +4625,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -4710,6 +4726,8 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1801">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -7268,11 +7286,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y123"/>
+  <dimension ref="A1:Y126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B68" sqref="B68"/>
+      <pane ySplit="3" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7896,54 +7914,52 @@
       </c>
       <c r="I26" s="31"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B27" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" s="48" t="s">
+    <row r="27" spans="1:17" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="52" t="s">
         <v>776</v>
       </c>
-      <c r="E27" s="48" t="s">
+      <c r="E27" s="52" t="s">
         <v>778</v>
       </c>
-      <c r="F27" s="31" t="s">
+      <c r="F27" s="52" t="s">
         <v>619</v>
       </c>
-      <c r="H27" s="4">
+      <c r="H27" s="53">
         <v>8</v>
       </c>
-      <c r="I27" s="31"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B28" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="48" t="s">
+    </row>
+    <row r="28" spans="1:17" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="52" t="s">
         <v>777</v>
       </c>
-      <c r="E28" s="48" t="s">
+      <c r="E28" s="52" t="s">
         <v>779</v>
       </c>
-      <c r="F28" s="31" t="s">
+      <c r="F28" s="52" t="s">
         <v>619</v>
       </c>
-      <c r="H28" s="4">
+      <c r="H28" s="53">
         <v>17</v>
       </c>
-      <c r="I28" s="31"/>
     </row>
     <row r="29" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B29" s="37" t="s">
-        <v>754</v>
+        <v>866</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>753</v>
+        <v>867</v>
       </c>
       <c r="D29" s="37" t="s">
-        <v>744</v>
+        <v>868</v>
       </c>
       <c r="E29" s="37" t="s">
         <v>68</v>
@@ -7955,146 +7971,138 @@
       <c r="B30" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="D30" s="31" t="s">
-        <v>756</v>
-      </c>
-      <c r="E30" s="31" t="s">
-        <v>755</v>
+      <c r="D30" s="48" t="s">
+        <v>776</v>
+      </c>
+      <c r="E30" s="48" t="s">
+        <v>778</v>
       </c>
       <c r="F30" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="H30" s="31">
+      <c r="H30" s="4">
+        <v>8</v>
+      </c>
+      <c r="I30" s="31"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B31" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="48" t="s">
+        <v>777</v>
+      </c>
+      <c r="E31" s="48" t="s">
+        <v>779</v>
+      </c>
+      <c r="F31" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H31" s="4">
+        <v>17</v>
+      </c>
+      <c r="I31" s="31"/>
+    </row>
+    <row r="32" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="P30" s="39"/>
-      <c r="Q30" s="2"/>
-    </row>
-    <row r="31" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="37" t="b">
+      <c r="B32" s="37" t="s">
+        <v>754</v>
+      </c>
+      <c r="C32" s="37" t="s">
+        <v>753</v>
+      </c>
+      <c r="D32" s="37" t="s">
+        <v>744</v>
+      </c>
+      <c r="E32" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B33" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="31" t="s">
+        <v>756</v>
+      </c>
+      <c r="E33" s="31" t="s">
+        <v>755</v>
+      </c>
+      <c r="F33" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H33" s="31">
         <v>1</v>
       </c>
-      <c r="B31" s="37" t="s">
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="P33" s="39"/>
+      <c r="Q33" s="2"/>
+    </row>
+    <row r="34" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B34" s="37" t="s">
         <v>760</v>
       </c>
-      <c r="C31" s="37" t="s">
+      <c r="C34" s="37" t="s">
         <v>762</v>
       </c>
-      <c r="D31" s="37" t="s">
+      <c r="D34" s="37" t="s">
         <v>745</v>
       </c>
-      <c r="E31" s="37" t="s">
+      <c r="E34" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B32" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D32" s="31" t="s">
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B35" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="31" t="s">
         <v>758</v>
       </c>
-      <c r="E32" s="31" t="s">
+      <c r="E35" s="31" t="s">
         <v>757</v>
       </c>
-      <c r="F32" s="31" t="s">
+      <c r="F35" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="H32" s="31">
+      <c r="H35" s="31">
         <v>1</v>
       </c>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
-      <c r="P32" s="39"/>
-      <c r="Q32" s="2"/>
-    </row>
-    <row r="33" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="B33" s="37" t="s">
-        <v>759</v>
-      </c>
-      <c r="C33" s="37" t="s">
-        <v>761</v>
-      </c>
-      <c r="D33" s="37" t="s">
-        <v>746</v>
-      </c>
-      <c r="E33" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G33" s="38"/>
-      <c r="H33" s="38"/>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B34" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" s="31" t="s">
-        <v>771</v>
-      </c>
-      <c r="E34" s="31" t="s">
-        <v>770</v>
-      </c>
-      <c r="F34" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="H34" s="31">
-        <v>1</v>
-      </c>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
-      <c r="N34" s="3"/>
-      <c r="P34" s="39"/>
-      <c r="Q34" s="2"/>
-    </row>
-    <row r="35" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B35" s="49" t="s">
-        <v>823</v>
-      </c>
-      <c r="C35" s="49" t="s">
-        <v>821</v>
-      </c>
-      <c r="D35" s="49" t="s">
-        <v>822</v>
-      </c>
-      <c r="E35" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="G35" s="50"/>
-      <c r="H35" s="50"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="P35" s="39"/>
+      <c r="Q35" s="2"/>
     </row>
     <row r="36" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="37" t="b">
         <v>1</v>
       </c>
       <c r="B36" s="37" t="s">
-        <v>824</v>
+        <v>759</v>
       </c>
       <c r="C36" s="37" t="s">
-        <v>820</v>
+        <v>761</v>
       </c>
       <c r="D36" s="37" t="s">
-        <v>819</v>
+        <v>746</v>
       </c>
       <c r="E36" s="37" t="s">
         <v>68</v>
@@ -8102,62 +8110,62 @@
       <c r="G36" s="38"/>
       <c r="H36" s="38"/>
     </row>
-    <row r="37" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="37" t="b">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B37" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="31" t="s">
+        <v>771</v>
+      </c>
+      <c r="E37" s="31" t="s">
+        <v>770</v>
+      </c>
+      <c r="F37" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H37" s="31">
         <v>1</v>
       </c>
-      <c r="B37" s="37" t="s">
-        <v>772</v>
-      </c>
-      <c r="C37" s="37" t="s">
-        <v>763</v>
-      </c>
-      <c r="D37" s="37" t="s">
-        <v>747</v>
-      </c>
-      <c r="E37" s="37" t="s">
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="P37" s="39"/>
+      <c r="Q37" s="2"/>
+    </row>
+    <row r="38" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B38" s="49" t="s">
+        <v>823</v>
+      </c>
+      <c r="C38" s="49" t="s">
+        <v>821</v>
+      </c>
+      <c r="D38" s="49" t="s">
+        <v>822</v>
+      </c>
+      <c r="E38" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="G37" s="38"/>
-      <c r="H37" s="38"/>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B38" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D38" s="31" t="s">
-        <v>774</v>
-      </c>
-      <c r="E38" s="31" t="s">
-        <v>773</v>
-      </c>
-      <c r="F38" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="H38" s="31">
-        <v>1</v>
-      </c>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
-      <c r="P38" s="39"/>
-      <c r="Q38" s="2"/>
+      <c r="G38" s="50"/>
+      <c r="H38" s="50"/>
     </row>
     <row r="39" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="37" t="b">
         <v>1</v>
       </c>
       <c r="B39" s="37" t="s">
-        <v>775</v>
+        <v>824</v>
       </c>
       <c r="C39" s="37" t="s">
-        <v>764</v>
+        <v>820</v>
       </c>
       <c r="D39" s="37" t="s">
-        <v>748</v>
+        <v>819</v>
       </c>
       <c r="E39" s="37" t="s">
         <v>68</v>
@@ -8170,13 +8178,13 @@
         <v>1</v>
       </c>
       <c r="B40" s="37" t="s">
-        <v>670</v>
+        <v>772</v>
       </c>
       <c r="C40" s="37" t="s">
-        <v>74</v>
+        <v>763</v>
       </c>
       <c r="D40" s="37" t="s">
-        <v>74</v>
+        <v>747</v>
       </c>
       <c r="E40" s="37" t="s">
         <v>68</v>
@@ -8189,19 +8197,16 @@
         <v>21</v>
       </c>
       <c r="D41" s="31" t="s">
-        <v>341</v>
+        <v>774</v>
       </c>
       <c r="E41" s="31" t="s">
-        <v>75</v>
+        <v>773</v>
       </c>
       <c r="F41" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="G41" s="31" t="s">
-        <v>780</v>
-      </c>
       <c r="H41" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
@@ -8212,37 +8217,37 @@
       <c r="P41" s="39"/>
       <c r="Q41" s="2"/>
     </row>
-    <row r="42" spans="1:17" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="46" t="b">
+    <row r="42" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B42" s="46" t="s">
-        <v>781</v>
-      </c>
-      <c r="C42" s="46" t="s">
-        <v>765</v>
-      </c>
-      <c r="D42" s="46" t="s">
-        <v>782</v>
-      </c>
-      <c r="E42" s="46" t="s">
+      <c r="B42" s="37" t="s">
+        <v>775</v>
+      </c>
+      <c r="C42" s="37" t="s">
+        <v>764</v>
+      </c>
+      <c r="D42" s="37" t="s">
+        <v>748</v>
+      </c>
+      <c r="E42" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G42" s="47"/>
-      <c r="H42" s="47"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="38"/>
     </row>
     <row r="43" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="37" t="b">
         <v>1</v>
       </c>
       <c r="B43" s="37" t="s">
-        <v>783</v>
+        <v>670</v>
       </c>
       <c r="C43" s="37" t="s">
-        <v>766</v>
+        <v>74</v>
       </c>
       <c r="D43" s="37" t="s">
-        <v>749</v>
+        <v>74</v>
       </c>
       <c r="E43" s="37" t="s">
         <v>68</v>
@@ -8255,16 +8260,19 @@
         <v>21</v>
       </c>
       <c r="D44" s="31" t="s">
-        <v>784</v>
+        <v>341</v>
       </c>
       <c r="E44" s="31" t="s">
-        <v>785</v>
+        <v>75</v>
       </c>
       <c r="F44" s="31" t="s">
         <v>619</v>
       </c>
+      <c r="G44" s="31" t="s">
+        <v>780</v>
+      </c>
       <c r="H44" s="31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
@@ -8275,279 +8283,273 @@
       <c r="P44" s="39"/>
       <c r="Q44" s="2"/>
     </row>
-    <row r="45" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="37" t="b">
+    <row r="45" spans="1:17" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="46" t="b">
         <v>1</v>
       </c>
-      <c r="B45" s="37" t="s">
+      <c r="B45" s="46" t="s">
+        <v>781</v>
+      </c>
+      <c r="C45" s="46" t="s">
+        <v>765</v>
+      </c>
+      <c r="D45" s="46" t="s">
+        <v>782</v>
+      </c>
+      <c r="E45" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="G45" s="47"/>
+      <c r="H45" s="47"/>
+    </row>
+    <row r="46" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B46" s="37" t="s">
+        <v>783</v>
+      </c>
+      <c r="C46" s="37" t="s">
+        <v>766</v>
+      </c>
+      <c r="D46" s="37" t="s">
+        <v>749</v>
+      </c>
+      <c r="E46" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G46" s="38"/>
+      <c r="H46" s="38"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B47" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D47" s="31" t="s">
+        <v>784</v>
+      </c>
+      <c r="E47" s="31" t="s">
+        <v>785</v>
+      </c>
+      <c r="F47" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H47" s="31">
+        <v>1</v>
+      </c>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
+      <c r="P47" s="39"/>
+      <c r="Q47" s="2"/>
+    </row>
+    <row r="48" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B48" s="37" t="s">
         <v>786</v>
       </c>
-      <c r="C45" s="37" t="s">
+      <c r="C48" s="37" t="s">
         <v>767</v>
       </c>
-      <c r="D45" s="37" t="s">
+      <c r="D48" s="37" t="s">
         <v>750</v>
       </c>
-      <c r="E45" s="37" t="s">
+      <c r="E48" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G45" s="38"/>
-      <c r="H45" s="38"/>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B46" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D46" s="31" t="s">
+      <c r="G48" s="38"/>
+      <c r="H48" s="38"/>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B49" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D49" s="31" t="s">
         <v>787</v>
       </c>
-      <c r="E46" s="31" t="s">
+      <c r="E49" s="31" t="s">
         <v>788</v>
       </c>
-      <c r="F46" s="31" t="s">
+      <c r="F49" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="H46" s="31">
+      <c r="H49" s="31">
         <v>1</v>
       </c>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
-      <c r="L46" s="3"/>
-      <c r="M46" s="3"/>
-      <c r="N46" s="3"/>
-      <c r="P46" s="39"/>
-      <c r="Q46" s="2"/>
-    </row>
-    <row r="47" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="37" t="b">
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
+      <c r="N49" s="3"/>
+      <c r="P49" s="39"/>
+      <c r="Q49" s="2"/>
+    </row>
+    <row r="50" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B47" s="37" t="s">
+      <c r="B50" s="37" t="s">
         <v>791</v>
       </c>
-      <c r="C47" s="37" t="s">
+      <c r="C50" s="37" t="s">
         <v>768</v>
       </c>
-      <c r="D47" s="37" t="s">
+      <c r="D50" s="37" t="s">
         <v>751</v>
       </c>
-      <c r="E47" s="37" t="s">
+      <c r="E50" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G47" s="38"/>
-      <c r="H47" s="38"/>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B48" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D48" s="31" t="s">
+      <c r="G50" s="38"/>
+      <c r="H50" s="38"/>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B51" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D51" s="31" t="s">
         <v>790</v>
       </c>
-      <c r="E48" s="31" t="s">
+      <c r="E51" s="31" t="s">
         <v>789</v>
       </c>
-      <c r="F48" s="31" t="s">
+      <c r="F51" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="H48" s="31">
+      <c r="H51" s="31">
         <v>1</v>
       </c>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
-      <c r="L48" s="3"/>
-      <c r="M48" s="3"/>
-      <c r="N48" s="3"/>
-      <c r="P48" s="39"/>
-      <c r="Q48" s="2"/>
-    </row>
-    <row r="49" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="37" t="b">
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="3"/>
+      <c r="P51" s="39"/>
+      <c r="Q51" s="2"/>
+    </row>
+    <row r="52" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B49" s="37" t="s">
+      <c r="B52" s="37" t="s">
         <v>792</v>
       </c>
-      <c r="C49" s="37" t="s">
+      <c r="C52" s="37" t="s">
         <v>769</v>
       </c>
-      <c r="D49" s="37" t="s">
+      <c r="D52" s="37" t="s">
         <v>752</v>
       </c>
-      <c r="E49" s="37" t="s">
+      <c r="E52" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G49" s="38"/>
-      <c r="H49" s="38"/>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B50" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D50" s="31" t="s">
+      <c r="G52" s="38"/>
+      <c r="H52" s="38"/>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B53" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D53" s="31" t="s">
         <v>794</v>
       </c>
-      <c r="E50" s="31" t="s">
+      <c r="E53" s="31" t="s">
         <v>793</v>
       </c>
-      <c r="F50" s="31" t="s">
+      <c r="F53" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="H50" s="31">
+      <c r="H53" s="31">
         <v>1</v>
       </c>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
-      <c r="K50" s="3"/>
-      <c r="L50" s="3"/>
-      <c r="M50" s="3"/>
-      <c r="N50" s="3"/>
-      <c r="P50" s="39"/>
-      <c r="Q50" s="2"/>
-    </row>
-    <row r="51" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="37" t="b">
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="3"/>
+      <c r="L53" s="3"/>
+      <c r="M53" s="3"/>
+      <c r="N53" s="3"/>
+      <c r="P53" s="39"/>
+      <c r="Q53" s="2"/>
+    </row>
+    <row r="54" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B51" s="37" t="s">
+      <c r="B54" s="37" t="s">
         <v>815</v>
       </c>
-      <c r="C51" s="37" t="s">
+      <c r="C54" s="37" t="s">
         <v>816</v>
       </c>
-      <c r="D51" s="37" t="s">
+      <c r="D54" s="37" t="s">
         <v>814</v>
       </c>
-      <c r="E51" s="37" t="s">
+      <c r="E54" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G51" s="38"/>
-      <c r="H51" s="38"/>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B52" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D52" s="31" t="s">
+      <c r="G54" s="38"/>
+      <c r="H54" s="38"/>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B55" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D55" s="31" t="s">
         <v>818</v>
       </c>
-      <c r="E52" s="31" t="s">
+      <c r="E55" s="31" t="s">
         <v>817</v>
       </c>
-      <c r="F52" s="31" t="s">
+      <c r="F55" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="H52" s="31">
+      <c r="H55" s="31">
         <v>1</v>
       </c>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
-      <c r="K52" s="3"/>
-      <c r="L52" s="3"/>
-      <c r="M52" s="3"/>
-      <c r="N52" s="3"/>
-      <c r="P52" s="39"/>
-      <c r="Q52" s="2"/>
-    </row>
-    <row r="53" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="37" t="b">
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="3"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3"/>
+      <c r="N55" s="3"/>
+      <c r="P55" s="39"/>
+      <c r="Q55" s="2"/>
+    </row>
+    <row r="56" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B53" s="37" t="s">
+      <c r="B56" s="37" t="s">
         <v>809</v>
       </c>
-      <c r="C53" s="37" t="s">
+      <c r="C56" s="37" t="s">
         <v>811</v>
       </c>
-      <c r="D53" s="37" t="s">
+      <c r="D56" s="37" t="s">
         <v>810</v>
       </c>
-      <c r="E53" s="37" t="s">
+      <c r="E56" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G53" s="38"/>
-      <c r="H53" s="38"/>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B54" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D54" s="31" t="s">
-        <v>813</v>
-      </c>
-      <c r="E54" s="31" t="s">
-        <v>812</v>
-      </c>
-      <c r="F54" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="H54" s="31">
-        <v>1</v>
-      </c>
-      <c r="I54" s="3"/>
-      <c r="J54" s="3"/>
-      <c r="K54" s="3"/>
-      <c r="L54" s="3"/>
-      <c r="M54" s="3"/>
-      <c r="N54" s="3"/>
-      <c r="P54" s="39"/>
-      <c r="Q54" s="2"/>
-    </row>
-    <row r="55" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="B55" s="37" t="s">
-        <v>802</v>
-      </c>
-      <c r="C55" s="37" t="s">
-        <v>804</v>
-      </c>
-      <c r="D55" s="37" t="s">
-        <v>803</v>
-      </c>
-      <c r="E55" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G55" s="38"/>
-      <c r="H55" s="38"/>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B56" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D56" s="31" t="s">
-        <v>807</v>
-      </c>
-      <c r="E56" s="31" t="s">
-        <v>805</v>
-      </c>
-      <c r="F56" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="H56" s="31">
-        <v>1</v>
-      </c>
-      <c r="I56" s="3"/>
-      <c r="J56" s="3"/>
-      <c r="K56" s="3"/>
-      <c r="L56" s="3"/>
-      <c r="M56" s="3"/>
-      <c r="N56" s="3"/>
-      <c r="P56" s="39"/>
-      <c r="Q56" s="2"/>
+      <c r="G56" s="38"/>
+      <c r="H56" s="38"/>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B57" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D57" s="31" t="s">
-        <v>808</v>
+        <v>813</v>
       </c>
       <c r="E57" s="31" t="s">
-        <v>806</v>
+        <v>812</v>
       </c>
       <c r="F57" s="31" t="s">
         <v>619</v>
@@ -8569,13 +8571,13 @@
         <v>1</v>
       </c>
       <c r="B58" s="37" t="s">
-        <v>843</v>
+        <v>802</v>
       </c>
       <c r="C58" s="37" t="s">
-        <v>854</v>
+        <v>804</v>
       </c>
       <c r="D58" s="37" t="s">
-        <v>833</v>
+        <v>803</v>
       </c>
       <c r="E58" s="37" t="s">
         <v>68</v>
@@ -8583,56 +8585,68 @@
       <c r="G58" s="38"/>
       <c r="H58" s="38"/>
     </row>
-    <row r="59" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="37" t="b">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B59" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D59" s="31" t="s">
+        <v>807</v>
+      </c>
+      <c r="E59" s="31" t="s">
+        <v>805</v>
+      </c>
+      <c r="F59" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H59" s="31">
         <v>1</v>
       </c>
-      <c r="B59" s="37" t="s">
-        <v>844</v>
-      </c>
-      <c r="C59" s="37" t="s">
-        <v>855</v>
-      </c>
-      <c r="D59" s="37" t="s">
-        <v>834</v>
-      </c>
-      <c r="E59" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G59" s="38"/>
-      <c r="H59" s="38"/>
-    </row>
-    <row r="60" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="37" t="b">
+      <c r="I59" s="3"/>
+      <c r="J59" s="3"/>
+      <c r="K59" s="3"/>
+      <c r="L59" s="3"/>
+      <c r="M59" s="3"/>
+      <c r="N59" s="3"/>
+      <c r="P59" s="39"/>
+      <c r="Q59" s="2"/>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B60" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D60" s="31" t="s">
+        <v>808</v>
+      </c>
+      <c r="E60" s="31" t="s">
+        <v>806</v>
+      </c>
+      <c r="F60" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H60" s="31">
         <v>1</v>
       </c>
-      <c r="B60" s="37" t="s">
-        <v>845</v>
-      </c>
-      <c r="C60" s="37" t="s">
-        <v>856</v>
-      </c>
-      <c r="D60" s="37" t="s">
-        <v>835</v>
-      </c>
-      <c r="E60" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G60" s="38"/>
-      <c r="H60" s="38"/>
+      <c r="I60" s="3"/>
+      <c r="J60" s="3"/>
+      <c r="K60" s="3"/>
+      <c r="L60" s="3"/>
+      <c r="M60" s="3"/>
+      <c r="N60" s="3"/>
+      <c r="P60" s="39"/>
+      <c r="Q60" s="2"/>
     </row>
     <row r="61" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B61" s="37" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C61" s="37" t="s">
-        <v>857</v>
+        <v>854</v>
       </c>
       <c r="D61" s="37" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="E61" s="37" t="s">
         <v>68</v>
@@ -8642,16 +8656,16 @@
     </row>
     <row r="62" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B62" s="37" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="C62" s="37" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
       <c r="D62" s="37" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="E62" s="37" t="s">
         <v>68</v>
@@ -8661,16 +8675,16 @@
     </row>
     <row r="63" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B63" s="37" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="C63" s="37" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
       <c r="D63" s="37" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
       <c r="E63" s="37" t="s">
         <v>68</v>
@@ -8683,13 +8697,13 @@
         <v>0</v>
       </c>
       <c r="B64" s="37" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="C64" s="37" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="D64" s="37" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
       <c r="E64" s="37" t="s">
         <v>68</v>
@@ -8702,13 +8716,13 @@
         <v>0</v>
       </c>
       <c r="B65" s="37" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
       <c r="C65" s="37" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="D65" s="37" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="E65" s="37" t="s">
         <v>68</v>
@@ -8721,13 +8735,13 @@
         <v>0</v>
       </c>
       <c r="B66" s="37" t="s">
-        <v>851</v>
+        <v>848</v>
       </c>
       <c r="C66" s="37" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="D66" s="37" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="E66" s="37" t="s">
         <v>68</v>
@@ -8740,13 +8754,13 @@
         <v>0</v>
       </c>
       <c r="B67" s="37" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="C67" s="37" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
       <c r="D67" s="37" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="E67" s="37" t="s">
         <v>68</v>
@@ -8756,16 +8770,16 @@
     </row>
     <row r="68" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B68" s="37" t="s">
-        <v>827</v>
+        <v>850</v>
       </c>
       <c r="C68" s="37" t="s">
-        <v>828</v>
+        <v>861</v>
       </c>
       <c r="D68" s="37" t="s">
-        <v>829</v>
+        <v>840</v>
       </c>
       <c r="E68" s="37" t="s">
         <v>68</v>
@@ -8773,17 +8787,62 @@
       <c r="G68" s="38"/>
       <c r="H68" s="38"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H69" s="31"/>
-      <c r="I69" s="31"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H70" s="31"/>
-      <c r="I70" s="31"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H71" s="31"/>
-      <c r="I71" s="31"/>
+    <row r="69" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="37" t="b">
+        <v>0</v>
+      </c>
+      <c r="B69" s="37" t="s">
+        <v>851</v>
+      </c>
+      <c r="C69" s="37" t="s">
+        <v>862</v>
+      </c>
+      <c r="D69" s="37" t="s">
+        <v>841</v>
+      </c>
+      <c r="E69" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G69" s="38"/>
+      <c r="H69" s="38"/>
+    </row>
+    <row r="70" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="37" t="b">
+        <v>0</v>
+      </c>
+      <c r="B70" s="37" t="s">
+        <v>852</v>
+      </c>
+      <c r="C70" s="37" t="s">
+        <v>863</v>
+      </c>
+      <c r="D70" s="37" t="s">
+        <v>842</v>
+      </c>
+      <c r="E70" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G70" s="38"/>
+      <c r="H70" s="38"/>
+    </row>
+    <row r="71" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B71" s="37" t="s">
+        <v>827</v>
+      </c>
+      <c r="C71" s="37" t="s">
+        <v>828</v>
+      </c>
+      <c r="D71" s="37" t="s">
+        <v>829</v>
+      </c>
+      <c r="E71" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G71" s="38"/>
+      <c r="H71" s="38"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H72" s="31"/>
@@ -8993,8 +9052,20 @@
       <c r="H123" s="31"/>
       <c r="I123" s="31"/>
     </row>
+    <row r="124" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H124" s="31"/>
+      <c r="I124" s="31"/>
+    </row>
+    <row r="125" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H125" s="31"/>
+      <c r="I125" s="31"/>
+    </row>
+    <row r="126" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H126" s="31"/>
+      <c r="I126" s="31"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:Z50"/>
+  <autoFilter ref="A2:Z53"/>
   <mergeCells count="1">
     <mergeCell ref="T1:Y1"/>
   </mergeCells>

</xml_diff>

<commit_message>
going back to empty seed model
Still need to look at HVAC schedules, also some updates related to shw,
elevators, and hvac.
</commit_message>
<xml_diff>
--- a/projects/m0.xlsx
+++ b/projects/m0.xlsx
@@ -1996,6 +1996,9 @@
     <t>single_run</t>
   </si>
   <si>
+    <t>../seeds/EmptySeedModel.osm</t>
+  </si>
+  <si>
     <t>Directory</t>
   </si>
   <si>
@@ -2537,9 +2540,6 @@
   </si>
   <si>
     <t>na</t>
-  </si>
-  <si>
-    <t>../seeds/ScheduleSetSeedModel_temp.osm</t>
   </si>
   <si>
     <t>AddSystem01BySpaceType</t>
@@ -6856,8 +6856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6997,7 +6997,7 @@
         <v>39</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>471</v>
@@ -7008,10 +7008,10 @@
         <v>25</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -7019,10 +7019,10 @@
         <v>26</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -7176,7 +7176,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>31</v>
@@ -7189,7 +7189,7 @@
         <v>29</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -7203,7 +7203,7 @@
         <v>38</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="E39" s="13" t="s">
         <v>449</v>
@@ -7217,10 +7217,10 @@
         <v>647</v>
       </c>
       <c r="D40" s="31" t="s">
+        <v>651</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>832</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>831</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -7231,7 +7231,7 @@
         <v>34</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="13" t="s">
@@ -7240,13 +7240,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="B43" s="26" t="s">
+        <v>744</v>
+      </c>
+      <c r="C43" s="25" t="s">
         <v>743</v>
-      </c>
-      <c r="C43" s="25" t="s">
-        <v>742</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -7281,7 +7281,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7439,13 +7439,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>68</v>
@@ -7458,16 +7458,16 @@
         <v>21</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="F5" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
     </row>
     <row r="6" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -7475,16 +7475,16 @@
         <v>21</v>
       </c>
       <c r="D6" s="30" t="s">
+        <v>661</v>
+      </c>
+      <c r="E6" s="30" t="s">
         <v>660</v>
-      </c>
-      <c r="E6" s="30" t="s">
-        <v>659</v>
       </c>
       <c r="F6" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H6" s="31" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
     </row>
     <row r="7" spans="1:25" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -7492,13 +7492,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C7" s="37" t="s">
+        <v>723</v>
+      </c>
+      <c r="D7" s="37" t="s">
         <v>722</v>
-      </c>
-      <c r="D7" s="37" t="s">
-        <v>721</v>
       </c>
       <c r="E7" s="37" t="s">
         <v>68</v>
@@ -7511,16 +7511,16 @@
         <v>21</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="F8" s="31" t="s">
         <v>618</v>
       </c>
       <c r="H8" s="31" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
@@ -7536,10 +7536,10 @@
         <v>21</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="F9" s="31" t="s">
         <v>619</v>
@@ -7559,10 +7559,10 @@
         <v>21</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="F10" s="31" t="s">
         <v>621</v>
@@ -7577,10 +7577,10 @@
         <v>21</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="E11" s="31" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="F11" s="30" t="s">
         <v>104</v>
@@ -7595,13 +7595,13 @@
         <v>1</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="C12" s="37" t="s">
+        <v>723</v>
+      </c>
+      <c r="D12" s="37" t="s">
         <v>722</v>
-      </c>
-      <c r="D12" s="37" t="s">
-        <v>721</v>
       </c>
       <c r="E12" s="37" t="s">
         <v>68</v>
@@ -7614,16 +7614,16 @@
         <v>21</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="F13" s="31" t="s">
         <v>618</v>
       </c>
       <c r="H13" s="31" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
@@ -7639,10 +7639,10 @@
         <v>21</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="F14" s="31" t="s">
         <v>619</v>
@@ -7662,10 +7662,10 @@
         <v>21</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="F15" s="31" t="s">
         <v>621</v>
@@ -7680,16 +7680,16 @@
         <v>21</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="F16" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H16" s="31" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="I16" s="31"/>
     </row>
@@ -7698,13 +7698,13 @@
         <v>1</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="C17" s="37" t="s">
+        <v>723</v>
+      </c>
+      <c r="D17" s="37" t="s">
         <v>722</v>
-      </c>
-      <c r="D17" s="37" t="s">
-        <v>721</v>
       </c>
       <c r="E17" s="37" t="s">
         <v>68</v>
@@ -7717,16 +7717,16 @@
         <v>21</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="F18" s="31" t="s">
         <v>618</v>
       </c>
       <c r="H18" s="31" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
@@ -7742,10 +7742,10 @@
         <v>21</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="E19" s="31" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="F19" s="31" t="s">
         <v>619</v>
@@ -7765,10 +7765,10 @@
         <v>21</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="E20" s="31" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="F20" s="31" t="s">
         <v>621</v>
@@ -7783,10 +7783,10 @@
         <v>21</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="E21" s="31" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="F21" s="30" t="s">
         <v>104</v>
@@ -7801,13 +7801,13 @@
         <v>1</v>
       </c>
       <c r="B22" s="37" t="s">
+        <v>734</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>732</v>
+      </c>
+      <c r="D22" s="37" t="s">
         <v>733</v>
-      </c>
-      <c r="C22" s="37" t="s">
-        <v>731</v>
-      </c>
-      <c r="D22" s="37" t="s">
-        <v>732</v>
       </c>
       <c r="E22" s="37" t="s">
         <v>68</v>
@@ -7820,10 +7820,10 @@
         <v>21</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="E23" s="31" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="F23" s="31" t="s">
         <v>630</v>
@@ -7845,16 +7845,16 @@
         <v>21</v>
       </c>
       <c r="D24" s="31" t="s">
+        <v>737</v>
+      </c>
+      <c r="E24" s="31" t="s">
         <v>736</v>
-      </c>
-      <c r="E24" s="31" t="s">
-        <v>735</v>
       </c>
       <c r="F24" s="31" t="s">
         <v>619</v>
       </c>
       <c r="G24" s="31" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="H24" s="4">
         <v>10</v>
@@ -7871,16 +7871,16 @@
         <v>21</v>
       </c>
       <c r="D25" s="31" t="s">
+        <v>739</v>
+      </c>
+      <c r="E25" s="31" t="s">
         <v>738</v>
-      </c>
-      <c r="E25" s="31" t="s">
-        <v>737</v>
       </c>
       <c r="F25" s="31" t="s">
         <v>619</v>
       </c>
       <c r="G25" s="31" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="H25" s="4">
         <v>10</v>
@@ -7892,10 +7892,10 @@
         <v>21</v>
       </c>
       <c r="D26" s="31" t="s">
+        <v>741</v>
+      </c>
+      <c r="E26" s="31" t="s">
         <v>740</v>
-      </c>
-      <c r="E26" s="31" t="s">
-        <v>739</v>
       </c>
       <c r="F26" s="31" t="s">
         <v>619</v>
@@ -7907,7 +7907,7 @@
     </row>
     <row r="27" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B27" s="37" t="s">
         <v>866</v>
@@ -7929,10 +7929,10 @@
         <v>21</v>
       </c>
       <c r="D28" s="48" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="E28" s="48" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="F28" s="31" t="s">
         <v>619</v>
@@ -7947,10 +7947,10 @@
         <v>21</v>
       </c>
       <c r="D29" s="48" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="E29" s="48" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="F29" s="31" t="s">
         <v>619</v>
@@ -7965,13 +7965,13 @@
         <v>1</v>
       </c>
       <c r="B30" s="37" t="s">
+        <v>755</v>
+      </c>
+      <c r="C30" s="37" t="s">
         <v>754</v>
       </c>
-      <c r="C30" s="37" t="s">
-        <v>753</v>
-      </c>
       <c r="D30" s="37" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="E30" s="37" t="s">
         <v>68</v>
@@ -7984,10 +7984,10 @@
         <v>21</v>
       </c>
       <c r="D31" s="31" t="s">
+        <v>757</v>
+      </c>
+      <c r="E31" s="31" t="s">
         <v>756</v>
-      </c>
-      <c r="E31" s="31" t="s">
-        <v>755</v>
       </c>
       <c r="F31" s="31" t="s">
         <v>619</v>
@@ -8009,13 +8009,13 @@
         <v>1</v>
       </c>
       <c r="B32" s="37" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="C32" s="37" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="D32" s="37" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="E32" s="37" t="s">
         <v>68</v>
@@ -8028,10 +8028,10 @@
         <v>21</v>
       </c>
       <c r="D33" s="31" t="s">
+        <v>759</v>
+      </c>
+      <c r="E33" s="31" t="s">
         <v>758</v>
-      </c>
-      <c r="E33" s="31" t="s">
-        <v>757</v>
       </c>
       <c r="F33" s="31" t="s">
         <v>619</v>
@@ -8053,13 +8053,13 @@
         <v>1</v>
       </c>
       <c r="B34" s="37" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="C34" s="37" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="D34" s="37" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="E34" s="37" t="s">
         <v>68</v>
@@ -8072,10 +8072,10 @@
         <v>21</v>
       </c>
       <c r="D35" s="31" t="s">
+        <v>772</v>
+      </c>
+      <c r="E35" s="31" t="s">
         <v>771</v>
-      </c>
-      <c r="E35" s="31" t="s">
-        <v>770</v>
       </c>
       <c r="F35" s="31" t="s">
         <v>619</v>
@@ -8097,13 +8097,13 @@
         <v>1</v>
       </c>
       <c r="B36" s="49" t="s">
+        <v>824</v>
+      </c>
+      <c r="C36" s="49" t="s">
+        <v>822</v>
+      </c>
+      <c r="D36" s="49" t="s">
         <v>823</v>
-      </c>
-      <c r="C36" s="49" t="s">
-        <v>821</v>
-      </c>
-      <c r="D36" s="49" t="s">
-        <v>822</v>
       </c>
       <c r="E36" s="49" t="s">
         <v>68</v>
@@ -8116,13 +8116,13 @@
         <v>1</v>
       </c>
       <c r="B37" s="37" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="C37" s="37" t="s">
+        <v>821</v>
+      </c>
+      <c r="D37" s="37" t="s">
         <v>820</v>
-      </c>
-      <c r="D37" s="37" t="s">
-        <v>819</v>
       </c>
       <c r="E37" s="37" t="s">
         <v>68</v>
@@ -8135,13 +8135,13 @@
         <v>1</v>
       </c>
       <c r="B38" s="37" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="C38" s="37" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="D38" s="37" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="E38" s="37" t="s">
         <v>68</v>
@@ -8154,10 +8154,10 @@
         <v>21</v>
       </c>
       <c r="D39" s="31" t="s">
+        <v>775</v>
+      </c>
+      <c r="E39" s="31" t="s">
         <v>774</v>
-      </c>
-      <c r="E39" s="31" t="s">
-        <v>773</v>
       </c>
       <c r="F39" s="31" t="s">
         <v>619</v>
@@ -8179,13 +8179,13 @@
         <v>1</v>
       </c>
       <c r="B40" s="37" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="C40" s="37" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="D40" s="37" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="E40" s="37" t="s">
         <v>68</v>
@@ -8198,7 +8198,7 @@
         <v>1</v>
       </c>
       <c r="B41" s="37" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="C41" s="37" t="s">
         <v>74</v>
@@ -8226,7 +8226,7 @@
         <v>619</v>
       </c>
       <c r="G42" s="31" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="H42" s="31">
         <v>0</v>
@@ -8245,13 +8245,13 @@
         <v>1</v>
       </c>
       <c r="B43" s="46" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="C43" s="46" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="D43" s="46" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="E43" s="46" t="s">
         <v>68</v>
@@ -8264,13 +8264,13 @@
         <v>1</v>
       </c>
       <c r="B44" s="37" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="C44" s="37" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="D44" s="37" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="E44" s="37" t="s">
         <v>68</v>
@@ -8283,10 +8283,10 @@
         <v>21</v>
       </c>
       <c r="D45" s="31" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="E45" s="31" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="F45" s="31" t="s">
         <v>619</v>
@@ -8308,13 +8308,13 @@
         <v>1</v>
       </c>
       <c r="B46" s="37" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="C46" s="37" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="D46" s="37" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="E46" s="37" t="s">
         <v>68</v>
@@ -8327,10 +8327,10 @@
         <v>21</v>
       </c>
       <c r="D47" s="31" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="E47" s="31" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="F47" s="31" t="s">
         <v>619</v>
@@ -8352,13 +8352,13 @@
         <v>1</v>
       </c>
       <c r="B48" s="37" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="C48" s="37" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="D48" s="37" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="E48" s="37" t="s">
         <v>68</v>
@@ -8371,10 +8371,10 @@
         <v>21</v>
       </c>
       <c r="D49" s="31" t="s">
+        <v>791</v>
+      </c>
+      <c r="E49" s="31" t="s">
         <v>790</v>
-      </c>
-      <c r="E49" s="31" t="s">
-        <v>789</v>
       </c>
       <c r="F49" s="31" t="s">
         <v>619</v>
@@ -8396,13 +8396,13 @@
         <v>1</v>
       </c>
       <c r="B50" s="37" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="C50" s="37" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="D50" s="37" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="E50" s="37" t="s">
         <v>68</v>
@@ -8415,10 +8415,10 @@
         <v>21</v>
       </c>
       <c r="D51" s="31" t="s">
+        <v>795</v>
+      </c>
+      <c r="E51" s="31" t="s">
         <v>794</v>
-      </c>
-      <c r="E51" s="31" t="s">
-        <v>793</v>
       </c>
       <c r="F51" s="31" t="s">
         <v>619</v>
@@ -8440,13 +8440,13 @@
         <v>1</v>
       </c>
       <c r="B52" s="37" t="s">
+        <v>816</v>
+      </c>
+      <c r="C52" s="37" t="s">
+        <v>817</v>
+      </c>
+      <c r="D52" s="37" t="s">
         <v>815</v>
-      </c>
-      <c r="C52" s="37" t="s">
-        <v>816</v>
-      </c>
-      <c r="D52" s="37" t="s">
-        <v>814</v>
       </c>
       <c r="E52" s="37" t="s">
         <v>68</v>
@@ -8459,10 +8459,10 @@
         <v>21</v>
       </c>
       <c r="D53" s="31" t="s">
+        <v>819</v>
+      </c>
+      <c r="E53" s="31" t="s">
         <v>818</v>
-      </c>
-      <c r="E53" s="31" t="s">
-        <v>817</v>
       </c>
       <c r="F53" s="31" t="s">
         <v>619</v>
@@ -8484,13 +8484,13 @@
         <v>1</v>
       </c>
       <c r="B54" s="37" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="C54" s="37" t="s">
+        <v>812</v>
+      </c>
+      <c r="D54" s="37" t="s">
         <v>811</v>
-      </c>
-      <c r="D54" s="37" t="s">
-        <v>810</v>
       </c>
       <c r="E54" s="37" t="s">
         <v>68</v>
@@ -8503,10 +8503,10 @@
         <v>21</v>
       </c>
       <c r="D55" s="31" t="s">
+        <v>814</v>
+      </c>
+      <c r="E55" s="31" t="s">
         <v>813</v>
-      </c>
-      <c r="E55" s="31" t="s">
-        <v>812</v>
       </c>
       <c r="F55" s="31" t="s">
         <v>619</v>
@@ -8528,13 +8528,13 @@
         <v>1</v>
       </c>
       <c r="B56" s="37" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="C56" s="37" t="s">
+        <v>805</v>
+      </c>
+      <c r="D56" s="37" t="s">
         <v>804</v>
-      </c>
-      <c r="D56" s="37" t="s">
-        <v>803</v>
       </c>
       <c r="E56" s="37" t="s">
         <v>68</v>
@@ -8547,10 +8547,10 @@
         <v>21</v>
       </c>
       <c r="D57" s="31" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="E57" s="31" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="F57" s="31" t="s">
         <v>619</v>
@@ -8572,10 +8572,10 @@
         <v>21</v>
       </c>
       <c r="D58" s="31" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="E58" s="31" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="F58" s="31" t="s">
         <v>619</v>
@@ -8787,13 +8787,13 @@
         <v>1</v>
       </c>
       <c r="B69" s="37" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="C69" s="37" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="D69" s="37" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="E69" s="37" t="s">
         <v>68</v>
@@ -9268,11 +9268,11 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="40" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="B8" s="40"/>
       <c r="C8" s="40" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="D8" s="40" t="s">
         <v>468</v>
@@ -9296,11 +9296,11 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="40" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="B9" s="40"/>
       <c r="C9" s="40" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="D9" s="40" t="s">
         <v>468</v>
@@ -9324,11 +9324,11 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="40" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="B10" s="40"/>
       <c r="C10" s="40" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="D10" s="40" t="s">
         <v>468</v>
@@ -9352,11 +9352,11 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="B11" s="40"/>
       <c r="C11" s="40" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="D11" s="40" t="s">
         <v>468</v>
@@ -9380,11 +9380,11 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="B12" s="40"/>
       <c r="C12" s="40" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="D12" s="40" t="s">
         <v>468</v>
@@ -9408,11 +9408,11 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="40" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="B13" s="40"/>
       <c r="C13" s="40" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="D13" s="40" t="s">
         <v>468</v>
@@ -9436,11 +9436,11 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="40" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="B14" s="40"/>
       <c r="C14" s="40" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="D14" s="40" t="s">
         <v>468</v>
@@ -9464,11 +9464,11 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="40" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="B15" s="40"/>
       <c r="C15" s="40" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="D15" s="40" t="s">
         <v>468</v>
@@ -9492,11 +9492,11 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="40" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B16" s="40"/>
       <c r="C16" s="40" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D16" s="40" t="s">
         <v>468</v>
@@ -9520,11 +9520,11 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="40" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="B17" s="40"/>
       <c r="C17" s="40" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="D17" s="40" t="s">
         <v>468</v>
@@ -9548,11 +9548,11 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="40" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="B18" s="40"/>
       <c r="C18" s="40" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="D18" s="40" t="s">
         <v>468</v>
@@ -9576,11 +9576,11 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="40" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="B19" s="40"/>
       <c r="C19" s="40" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="D19" s="40" t="s">
         <v>468</v>
@@ -9604,11 +9604,11 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="40" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="B20" s="40"/>
       <c r="C20" s="40" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="D20" s="40" t="s">
         <v>468</v>
@@ -9632,11 +9632,11 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="40" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B21" s="40"/>
       <c r="C21" s="40" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="D21" s="40" t="s">
         <v>468</v>
@@ -9660,14 +9660,14 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="40" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="B22" s="40"/>
       <c r="C22" s="40" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="D22" s="40" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="E22" s="40" t="s">
         <v>64</v>
@@ -9688,14 +9688,14 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="40" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="B23" s="40"/>
       <c r="C23" s="40" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="D23" s="40" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="E23" s="40" t="s">
         <v>64</v>
@@ -9716,14 +9716,14 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="40" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="B24" s="40"/>
       <c r="C24" s="40" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="D24" s="40" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="E24" s="40" t="s">
         <v>64</v>
@@ -9744,14 +9744,14 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="40" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="B25" s="40"/>
       <c r="C25" s="40" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="D25" s="40" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="E25" s="40" t="s">
         <v>64</v>
@@ -9772,14 +9772,14 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="40" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="B26" s="40"/>
       <c r="C26" s="40" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="D26" s="40" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="E26" s="40" t="s">
         <v>64</v>
@@ -9800,14 +9800,14 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="40" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="B27" s="40"/>
       <c r="C27" s="40" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D27" s="40" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="E27" s="40" t="s">
         <v>64</v>
@@ -9828,14 +9828,14 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="40" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="B28" s="40"/>
       <c r="C28" s="40" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="D28" s="40" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="E28" s="40" t="s">
         <v>64</v>
@@ -9858,14 +9858,14 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="40" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="B29" s="40"/>
       <c r="C29" s="40" t="s">
+        <v>676</v>
+      </c>
+      <c r="D29" s="40" t="s">
         <v>675</v>
-      </c>
-      <c r="D29" s="40" t="s">
-        <v>674</v>
       </c>
       <c r="E29" s="40" t="s">
         <v>64</v>
@@ -9888,14 +9888,14 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="40" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="B30" s="40"/>
       <c r="C30" s="40" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="D30" s="40" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="E30" s="40" t="s">
         <v>64</v>
@@ -9918,14 +9918,14 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="40" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="B31" s="40"/>
       <c r="C31" s="40" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="D31" s="40" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="E31" s="40" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
fixing measure dir for thermostats
had an inadvertent space.
</commit_message>
<xml_diff>
--- a/projects/m0.xlsx
+++ b/projects/m0.xlsx
@@ -2338,9 +2338,6 @@
     <t>add_internal_mass_to_space_types</t>
   </si>
   <si>
-    <t>add _thermostats</t>
-  </si>
-  <si>
     <t>add_fenestration_and_overhangs_by_space_type</t>
   </si>
   <si>
@@ -2648,6 +2645,9 @@
   </si>
   <si>
     <t>AddSchedulesToModel</t>
+  </si>
+  <si>
+    <t>add_thermostats</t>
   </si>
 </sst>
 </file>
@@ -6856,8 +6856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6915,7 +6915,7 @@
         <v>469</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>614</v>
@@ -7220,7 +7220,7 @@
         <v>651</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -7280,8 +7280,8 @@
   <dimension ref="A1:Y124"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
+      <pane ySplit="3" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7492,7 +7492,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C7" s="37" t="s">
         <v>723</v>
@@ -7559,7 +7559,7 @@
         <v>21</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E10" s="31" t="s">
         <v>726</v>
@@ -7577,16 +7577,16 @@
         <v>21</v>
       </c>
       <c r="D11" s="31" t="s">
+        <v>825</v>
+      </c>
+      <c r="E11" s="31" t="s">
         <v>826</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>827</v>
       </c>
       <c r="F11" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H11" s="31" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="I11" s="31"/>
     </row>
@@ -7595,7 +7595,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C12" s="37" t="s">
         <v>723</v>
@@ -7662,7 +7662,7 @@
         <v>21</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E15" s="31" t="s">
         <v>726</v>
@@ -7680,16 +7680,16 @@
         <v>21</v>
       </c>
       <c r="D16" s="31" t="s">
+        <v>825</v>
+      </c>
+      <c r="E16" s="31" t="s">
         <v>826</v>
-      </c>
-      <c r="E16" s="31" t="s">
-        <v>827</v>
       </c>
       <c r="F16" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H16" s="31" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="I16" s="31"/>
     </row>
@@ -7698,7 +7698,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="C17" s="37" t="s">
         <v>723</v>
@@ -7765,7 +7765,7 @@
         <v>21</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E20" s="31" t="s">
         <v>726</v>
@@ -7783,16 +7783,16 @@
         <v>21</v>
       </c>
       <c r="D21" s="31" t="s">
+        <v>825</v>
+      </c>
+      <c r="E21" s="31" t="s">
         <v>826</v>
-      </c>
-      <c r="E21" s="31" t="s">
-        <v>827</v>
       </c>
       <c r="F21" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H21" s="31" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I21" s="31"/>
     </row>
@@ -7820,7 +7820,7 @@
         <v>21</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E23" s="31" t="s">
         <v>735</v>
@@ -7910,13 +7910,13 @@
         <v>1</v>
       </c>
       <c r="B27" s="37" t="s">
+        <v>865</v>
+      </c>
+      <c r="C27" s="37" t="s">
         <v>866</v>
       </c>
-      <c r="C27" s="37" t="s">
+      <c r="D27" s="37" t="s">
         <v>867</v>
-      </c>
-      <c r="D27" s="37" t="s">
-        <v>868</v>
       </c>
       <c r="E27" s="37" t="s">
         <v>68</v>
@@ -7929,10 +7929,10 @@
         <v>21</v>
       </c>
       <c r="D28" s="48" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="E28" s="48" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="F28" s="31" t="s">
         <v>619</v>
@@ -7947,10 +7947,10 @@
         <v>21</v>
       </c>
       <c r="D29" s="48" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="E29" s="48" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="F29" s="31" t="s">
         <v>619</v>
@@ -8072,10 +8072,10 @@
         <v>21</v>
       </c>
       <c r="D35" s="31" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="E35" s="31" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="F35" s="31" t="s">
         <v>619</v>
@@ -8097,13 +8097,13 @@
         <v>1</v>
       </c>
       <c r="B36" s="49" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="C36" s="49" t="s">
+        <v>821</v>
+      </c>
+      <c r="D36" s="49" t="s">
         <v>822</v>
-      </c>
-      <c r="D36" s="49" t="s">
-        <v>823</v>
       </c>
       <c r="E36" s="49" t="s">
         <v>68</v>
@@ -8116,13 +8116,13 @@
         <v>1</v>
       </c>
       <c r="B37" s="37" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="D37" s="37" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E37" s="37" t="s">
         <v>68</v>
@@ -8135,7 +8135,7 @@
         <v>1</v>
       </c>
       <c r="B38" s="37" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C38" s="37" t="s">
         <v>764</v>
@@ -8154,10 +8154,10 @@
         <v>21</v>
       </c>
       <c r="D39" s="31" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="E39" s="31" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="F39" s="31" t="s">
         <v>619</v>
@@ -8179,10 +8179,10 @@
         <v>1</v>
       </c>
       <c r="B40" s="37" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="C40" s="37" t="s">
-        <v>765</v>
+        <v>868</v>
       </c>
       <c r="D40" s="37" t="s">
         <v>749</v>
@@ -8226,7 +8226,7 @@
         <v>619</v>
       </c>
       <c r="G42" s="31" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="H42" s="31">
         <v>0</v>
@@ -8245,13 +8245,13 @@
         <v>1</v>
       </c>
       <c r="B43" s="46" t="s">
+        <v>781</v>
+      </c>
+      <c r="C43" s="46" t="s">
+        <v>765</v>
+      </c>
+      <c r="D43" s="46" t="s">
         <v>782</v>
-      </c>
-      <c r="C43" s="46" t="s">
-        <v>766</v>
-      </c>
-      <c r="D43" s="46" t="s">
-        <v>783</v>
       </c>
       <c r="E43" s="46" t="s">
         <v>68</v>
@@ -8264,10 +8264,10 @@
         <v>1</v>
       </c>
       <c r="B44" s="37" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="C44" s="37" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="D44" s="37" t="s">
         <v>750</v>
@@ -8283,10 +8283,10 @@
         <v>21</v>
       </c>
       <c r="D45" s="31" t="s">
+        <v>784</v>
+      </c>
+      <c r="E45" s="31" t="s">
         <v>785</v>
-      </c>
-      <c r="E45" s="31" t="s">
-        <v>786</v>
       </c>
       <c r="F45" s="31" t="s">
         <v>619</v>
@@ -8308,10 +8308,10 @@
         <v>1</v>
       </c>
       <c r="B46" s="37" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="C46" s="37" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="D46" s="37" t="s">
         <v>751</v>
@@ -8327,10 +8327,10 @@
         <v>21</v>
       </c>
       <c r="D47" s="31" t="s">
+        <v>787</v>
+      </c>
+      <c r="E47" s="31" t="s">
         <v>788</v>
-      </c>
-      <c r="E47" s="31" t="s">
-        <v>789</v>
       </c>
       <c r="F47" s="31" t="s">
         <v>619</v>
@@ -8352,10 +8352,10 @@
         <v>1</v>
       </c>
       <c r="B48" s="37" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="C48" s="37" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="D48" s="37" t="s">
         <v>752</v>
@@ -8371,10 +8371,10 @@
         <v>21</v>
       </c>
       <c r="D49" s="31" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="E49" s="31" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="F49" s="31" t="s">
         <v>619</v>
@@ -8396,10 +8396,10 @@
         <v>1</v>
       </c>
       <c r="B50" s="37" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="C50" s="37" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="D50" s="37" t="s">
         <v>753</v>
@@ -8415,10 +8415,10 @@
         <v>21</v>
       </c>
       <c r="D51" s="31" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E51" s="31" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F51" s="31" t="s">
         <v>619</v>
@@ -8440,13 +8440,13 @@
         <v>1</v>
       </c>
       <c r="B52" s="37" t="s">
+        <v>815</v>
+      </c>
+      <c r="C52" s="37" t="s">
         <v>816</v>
       </c>
-      <c r="C52" s="37" t="s">
-        <v>817</v>
-      </c>
       <c r="D52" s="37" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="E52" s="37" t="s">
         <v>68</v>
@@ -8459,10 +8459,10 @@
         <v>21</v>
       </c>
       <c r="D53" s="31" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E53" s="31" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="F53" s="31" t="s">
         <v>619</v>
@@ -8484,13 +8484,13 @@
         <v>1</v>
       </c>
       <c r="B54" s="37" t="s">
+        <v>809</v>
+      </c>
+      <c r="C54" s="37" t="s">
+        <v>811</v>
+      </c>
+      <c r="D54" s="37" t="s">
         <v>810</v>
-      </c>
-      <c r="C54" s="37" t="s">
-        <v>812</v>
-      </c>
-      <c r="D54" s="37" t="s">
-        <v>811</v>
       </c>
       <c r="E54" s="37" t="s">
         <v>68</v>
@@ -8503,10 +8503,10 @@
         <v>21</v>
       </c>
       <c r="D55" s="31" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E55" s="31" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="F55" s="31" t="s">
         <v>619</v>
@@ -8528,13 +8528,13 @@
         <v>1</v>
       </c>
       <c r="B56" s="37" t="s">
+        <v>802</v>
+      </c>
+      <c r="C56" s="37" t="s">
+        <v>804</v>
+      </c>
+      <c r="D56" s="37" t="s">
         <v>803</v>
-      </c>
-      <c r="C56" s="37" t="s">
-        <v>805</v>
-      </c>
-      <c r="D56" s="37" t="s">
-        <v>804</v>
       </c>
       <c r="E56" s="37" t="s">
         <v>68</v>
@@ -8547,10 +8547,10 @@
         <v>21</v>
       </c>
       <c r="D57" s="31" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E57" s="31" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="F57" s="31" t="s">
         <v>619</v>
@@ -8572,10 +8572,10 @@
         <v>21</v>
       </c>
       <c r="D58" s="31" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="E58" s="31" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="F58" s="31" t="s">
         <v>619</v>
@@ -8597,13 +8597,13 @@
         <v>1</v>
       </c>
       <c r="B59" s="37" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="C59" s="37" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="D59" s="37" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="E59" s="37" t="s">
         <v>68</v>
@@ -8616,13 +8616,13 @@
         <v>1</v>
       </c>
       <c r="B60" s="37" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C60" s="37" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="D60" s="37" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="E60" s="37" t="s">
         <v>68</v>
@@ -8635,13 +8635,13 @@
         <v>1</v>
       </c>
       <c r="B61" s="37" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C61" s="37" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="D61" s="37" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="E61" s="37" t="s">
         <v>68</v>
@@ -8654,13 +8654,13 @@
         <v>0</v>
       </c>
       <c r="B62" s="37" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="C62" s="37" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="D62" s="37" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="E62" s="37" t="s">
         <v>68</v>
@@ -8673,13 +8673,13 @@
         <v>0</v>
       </c>
       <c r="B63" s="37" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="C63" s="37" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="D63" s="37" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="E63" s="37" t="s">
         <v>68</v>
@@ -8692,13 +8692,13 @@
         <v>0</v>
       </c>
       <c r="B64" s="37" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="C64" s="37" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="D64" s="37" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="E64" s="37" t="s">
         <v>68</v>
@@ -8711,13 +8711,13 @@
         <v>0</v>
       </c>
       <c r="B65" s="37" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C65" s="37" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="D65" s="37" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="E65" s="37" t="s">
         <v>68</v>
@@ -8730,13 +8730,13 @@
         <v>0</v>
       </c>
       <c r="B66" s="37" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C66" s="37" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D66" s="37" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="E66" s="37" t="s">
         <v>68</v>
@@ -8749,13 +8749,13 @@
         <v>0</v>
       </c>
       <c r="B67" s="37" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="C67" s="37" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="D67" s="37" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="E67" s="37" t="s">
         <v>68</v>
@@ -8768,13 +8768,13 @@
         <v>0</v>
       </c>
       <c r="B68" s="37" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="C68" s="37" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="D68" s="37" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="E68" s="37" t="s">
         <v>68</v>
@@ -8787,13 +8787,13 @@
         <v>1</v>
       </c>
       <c r="B69" s="37" t="s">
+        <v>827</v>
+      </c>
+      <c r="C69" s="37" t="s">
         <v>828</v>
       </c>
-      <c r="C69" s="37" t="s">
+      <c r="D69" s="37" t="s">
         <v>829</v>
-      </c>
-      <c r="D69" s="37" t="s">
-        <v>830</v>
       </c>
       <c r="E69" s="37" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
Turning on systems 4 and 5
The measures for these have been updated in the cofee-measures repo.
</commit_message>
<xml_diff>
--- a/projects/m0.xlsx
+++ b/projects/m0.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2419" uniqueCount="869">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2419" uniqueCount="868">
   <si>
     <t>type</t>
   </si>
@@ -2533,9 +2533,6 @@
     <t>AddServiceWaterHeatingSupply</t>
   </si>
   <si>
-    <t>SysType 3</t>
-  </si>
-  <si>
     <t>na</t>
   </si>
   <si>
@@ -2599,9 +2596,6 @@
     <t>Add System 10 By Space Type</t>
   </si>
   <si>
-    <t>SysType 1</t>
-  </si>
-  <si>
     <t>add_system01_by_space_type</t>
   </si>
   <si>
@@ -2635,9 +2629,6 @@
     <t>1.8.0</t>
   </si>
   <si>
-    <t>SysType 2</t>
-  </si>
-  <si>
     <t>Add Schedules to Model</t>
   </si>
   <si>
@@ -2648,6 +2639,12 @@
   </si>
   <si>
     <t>add_thermostats</t>
+  </si>
+  <si>
+    <t>SysType 4</t>
+  </si>
+  <si>
+    <t>SysType 5</t>
   </si>
 </sst>
 </file>
@@ -6915,7 +6912,7 @@
         <v>469</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>614</v>
@@ -7220,7 +7217,7 @@
         <v>651</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -7280,8 +7277,8 @@
   <dimension ref="A1:Y124"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
+      <pane ySplit="3" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7586,7 +7583,7 @@
         <v>104</v>
       </c>
       <c r="H11" s="31" t="s">
-        <v>852</v>
+        <v>866</v>
       </c>
       <c r="I11" s="31"/>
     </row>
@@ -7689,7 +7686,7 @@
         <v>104</v>
       </c>
       <c r="H16" s="31" t="s">
-        <v>830</v>
+        <v>867</v>
       </c>
       <c r="I16" s="31"/>
     </row>
@@ -7792,7 +7789,7 @@
         <v>104</v>
       </c>
       <c r="H21" s="31" t="s">
-        <v>864</v>
+        <v>867</v>
       </c>
       <c r="I21" s="31"/>
     </row>
@@ -7910,13 +7907,13 @@
         <v>1</v>
       </c>
       <c r="B27" s="37" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
       <c r="C27" s="37" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="D27" s="37" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="E27" s="37" t="s">
         <v>68</v>
@@ -8182,7 +8179,7 @@
         <v>775</v>
       </c>
       <c r="C40" s="37" t="s">
-        <v>868</v>
+        <v>865</v>
       </c>
       <c r="D40" s="37" t="s">
         <v>749</v>
@@ -8597,13 +8594,13 @@
         <v>1</v>
       </c>
       <c r="B59" s="37" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="C59" s="37" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="D59" s="37" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="E59" s="37" t="s">
         <v>68</v>
@@ -8616,13 +8613,13 @@
         <v>1</v>
       </c>
       <c r="B60" s="37" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="C60" s="37" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="D60" s="37" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="E60" s="37" t="s">
         <v>68</v>
@@ -8635,13 +8632,13 @@
         <v>1</v>
       </c>
       <c r="B61" s="37" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C61" s="37" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="D61" s="37" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="E61" s="37" t="s">
         <v>68</v>
@@ -8651,16 +8648,16 @@
     </row>
     <row r="62" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B62" s="37" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C62" s="37" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="D62" s="37" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="E62" s="37" t="s">
         <v>68</v>
@@ -8670,16 +8667,16 @@
     </row>
     <row r="63" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B63" s="37" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="C63" s="37" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="D63" s="37" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="E63" s="37" t="s">
         <v>68</v>
@@ -8692,13 +8689,13 @@
         <v>0</v>
       </c>
       <c r="B64" s="37" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="C64" s="37" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="D64" s="37" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="E64" s="37" t="s">
         <v>68</v>
@@ -8711,13 +8708,13 @@
         <v>0</v>
       </c>
       <c r="B65" s="37" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="C65" s="37" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="D65" s="37" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="E65" s="37" t="s">
         <v>68</v>
@@ -8730,13 +8727,13 @@
         <v>0</v>
       </c>
       <c r="B66" s="37" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C66" s="37" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="D66" s="37" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="E66" s="37" t="s">
         <v>68</v>
@@ -8749,13 +8746,13 @@
         <v>0</v>
       </c>
       <c r="B67" s="37" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C67" s="37" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="D67" s="37" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="E67" s="37" t="s">
         <v>68</v>
@@ -8768,13 +8765,13 @@
         <v>0</v>
       </c>
       <c r="B68" s="37" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="C68" s="37" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="D68" s="37" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="E68" s="37" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
System types 1-8 now supported
Still using defaulted HVAC schedules.
</commit_message>
<xml_diff>
--- a/projects/m0.xlsx
+++ b/projects/m0.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2419" uniqueCount="868">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2411" uniqueCount="863">
   <si>
     <t>type</t>
   </si>
@@ -2560,12 +2560,6 @@
     <t>AddSystem08BySpaceType</t>
   </si>
   <si>
-    <t>AddSystem09BySpaceType</t>
-  </si>
-  <si>
-    <t>AddSystem10BySpaceType</t>
-  </si>
-  <si>
     <t>Add System 01 By Space Type</t>
   </si>
   <si>
@@ -2590,10 +2584,7 @@
     <t>Add System 08 By Space Type</t>
   </si>
   <si>
-    <t>Add System 09 By Space Type</t>
-  </si>
-  <si>
-    <t>Add System 10 By Space Type</t>
+    <t>SysType 1</t>
   </si>
   <si>
     <t>add_system01_by_space_type</t>
@@ -2620,12 +2611,6 @@
     <t>add_system08_by_space_type</t>
   </si>
   <si>
-    <t>add_system09_by_space_type</t>
-  </si>
-  <si>
-    <t>add_system10_by_space_type</t>
-  </si>
-  <si>
     <t>1.8.0</t>
   </si>
   <si>
@@ -2641,10 +2626,10 @@
     <t>add_thermostats</t>
   </si>
   <si>
-    <t>SysType 4</t>
-  </si>
-  <si>
-    <t>SysType 5</t>
+    <t>SysType 7</t>
+  </si>
+  <si>
+    <t>SysType 8</t>
   </si>
 </sst>
 </file>
@@ -6912,7 +6897,7 @@
         <v>469</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>861</v>
+        <v>856</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>614</v>
@@ -7274,11 +7259,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y124"/>
+  <dimension ref="A1:Y122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C72" sqref="C72"/>
+      <pane ySplit="3" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7583,7 +7568,7 @@
         <v>104</v>
       </c>
       <c r="H11" s="31" t="s">
-        <v>866</v>
+        <v>861</v>
       </c>
       <c r="I11" s="31"/>
     </row>
@@ -7686,7 +7671,7 @@
         <v>104</v>
       </c>
       <c r="H16" s="31" t="s">
-        <v>867</v>
+        <v>847</v>
       </c>
       <c r="I16" s="31"/>
     </row>
@@ -7789,7 +7774,7 @@
         <v>104</v>
       </c>
       <c r="H21" s="31" t="s">
-        <v>867</v>
+        <v>862</v>
       </c>
       <c r="I21" s="31"/>
     </row>
@@ -7907,13 +7892,13 @@
         <v>1</v>
       </c>
       <c r="B27" s="37" t="s">
-        <v>862</v>
+        <v>857</v>
       </c>
       <c r="C27" s="37" t="s">
-        <v>863</v>
+        <v>858</v>
       </c>
       <c r="D27" s="37" t="s">
-        <v>864</v>
+        <v>859</v>
       </c>
       <c r="E27" s="37" t="s">
         <v>68</v>
@@ -8179,7 +8164,7 @@
         <v>775</v>
       </c>
       <c r="C40" s="37" t="s">
-        <v>865</v>
+        <v>860</v>
       </c>
       <c r="D40" s="37" t="s">
         <v>749</v>
@@ -8594,10 +8579,10 @@
         <v>1</v>
       </c>
       <c r="B59" s="37" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="C59" s="37" t="s">
-        <v>851</v>
+        <v>848</v>
       </c>
       <c r="D59" s="37" t="s">
         <v>831</v>
@@ -8613,10 +8598,10 @@
         <v>1</v>
       </c>
       <c r="B60" s="37" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="C60" s="37" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="D60" s="37" t="s">
         <v>832</v>
@@ -8632,10 +8617,10 @@
         <v>1</v>
       </c>
       <c r="B61" s="37" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="C61" s="37" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
       <c r="D61" s="37" t="s">
         <v>833</v>
@@ -8651,10 +8636,10 @@
         <v>1</v>
       </c>
       <c r="B62" s="37" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C62" s="37" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
       <c r="D62" s="37" t="s">
         <v>834</v>
@@ -8670,10 +8655,10 @@
         <v>1</v>
       </c>
       <c r="B63" s="37" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="C63" s="37" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
       <c r="D63" s="37" t="s">
         <v>835</v>
@@ -8686,13 +8671,13 @@
     </row>
     <row r="64" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B64" s="37" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="C64" s="37" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="D64" s="37" t="s">
         <v>836</v>
@@ -8705,13 +8690,13 @@
     </row>
     <row r="65" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B65" s="37" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="C65" s="37" t="s">
-        <v>857</v>
+        <v>854</v>
       </c>
       <c r="D65" s="37" t="s">
         <v>837</v>
@@ -8724,13 +8709,13 @@
     </row>
     <row r="66" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B66" s="37" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="C66" s="37" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
       <c r="D66" s="37" t="s">
         <v>838</v>
@@ -8743,16 +8728,16 @@
     </row>
     <row r="67" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B67" s="37" t="s">
-        <v>849</v>
+        <v>827</v>
       </c>
       <c r="C67" s="37" t="s">
-        <v>859</v>
+        <v>828</v>
       </c>
       <c r="D67" s="37" t="s">
-        <v>839</v>
+        <v>829</v>
       </c>
       <c r="E67" s="37" t="s">
         <v>68</v>
@@ -8760,43 +8745,13 @@
       <c r="G67" s="38"/>
       <c r="H67" s="38"/>
     </row>
-    <row r="68" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="37" t="b">
-        <v>0</v>
-      </c>
-      <c r="B68" s="37" t="s">
-        <v>850</v>
-      </c>
-      <c r="C68" s="37" t="s">
-        <v>860</v>
-      </c>
-      <c r="D68" s="37" t="s">
-        <v>840</v>
-      </c>
-      <c r="E68" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G68" s="38"/>
-      <c r="H68" s="38"/>
-    </row>
-    <row r="69" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="B69" s="37" t="s">
-        <v>827</v>
-      </c>
-      <c r="C69" s="37" t="s">
-        <v>828</v>
-      </c>
-      <c r="D69" s="37" t="s">
-        <v>829</v>
-      </c>
-      <c r="E69" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G69" s="38"/>
-      <c r="H69" s="38"/>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H68" s="31"/>
+      <c r="I68" s="31"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H69" s="31"/>
+      <c r="I69" s="31"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H70" s="31"/>
@@ -9009,14 +8964,6 @@
     <row r="122" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H122" s="31"/>
       <c r="I122" s="31"/>
-    </row>
-    <row r="123" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H123" s="31"/>
-      <c r="I123" s="31"/>
-    </row>
-    <row r="124" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H124" s="31"/>
-      <c r="I124" s="31"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:Z51"/>

</xml_diff>

<commit_message>
system 6 is running
I turned off all other systems. I need to see why that is happening and
then turn them back on.
</commit_message>
<xml_diff>
--- a/projects/m0.xlsx
+++ b/projects/m0.xlsx
@@ -2623,22 +2623,22 @@
     <t>add_thermostats</t>
   </si>
   <si>
-    <t>ReameSpacesAndThermalZonesByStoryAndStandardsSpaceType</t>
-  </si>
-  <si>
     <t>Rename Spaces and Thermal Zones By Story and Standards Space Type</t>
   </si>
   <si>
     <t>rename_spaces_and_thermal_zones_by_story_and_standards_space_type</t>
   </si>
   <si>
-    <t>SysType 2</t>
-  </si>
-  <si>
     <t>multiplier_wwr</t>
   </si>
   <si>
     <t>Window to Wall Ratio Multiplier</t>
+  </si>
+  <si>
+    <t>SysType 6</t>
+  </si>
+  <si>
+    <t>RenameSpacesAndThermalZonesByStoryAndStandardsSpaceType</t>
   </si>
 </sst>
 </file>
@@ -6848,7 +6848,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7271,8 +7271,8 @@
   <dimension ref="A1:Y125"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D46" sqref="D46"/>
+      <pane ySplit="3" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7577,7 +7577,7 @@
         <v>104</v>
       </c>
       <c r="H11" s="31" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="I11" s="31"/>
     </row>
@@ -7680,7 +7680,7 @@
         <v>104</v>
       </c>
       <c r="H16" s="31" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="I16" s="31"/>
     </row>
@@ -7783,7 +7783,7 @@
         <v>104</v>
       </c>
       <c r="H21" s="31" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="I21" s="31"/>
     </row>
@@ -7901,13 +7901,13 @@
         <v>0</v>
       </c>
       <c r="B27" s="49" t="s">
+        <v>860</v>
+      </c>
+      <c r="C27" s="49" t="s">
         <v>861</v>
       </c>
-      <c r="C27" s="49" t="s">
-        <v>862</v>
-      </c>
       <c r="D27" s="49" t="s">
-        <v>860</v>
+        <v>865</v>
       </c>
       <c r="E27" s="49" t="s">
         <v>68</v>
@@ -8293,10 +8293,10 @@
         <v>21</v>
       </c>
       <c r="D46" s="31" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="E46" s="31" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="F46" s="31" t="s">
         <v>619</v>
@@ -8648,7 +8648,7 @@
     </row>
     <row r="62" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B62" s="37" t="s">
         <v>839</v>
@@ -8667,7 +8667,7 @@
     </row>
     <row r="63" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B63" s="37" t="s">
         <v>840</v>
@@ -8686,7 +8686,7 @@
     </row>
     <row r="64" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B64" s="37" t="s">
         <v>841</v>
@@ -8705,7 +8705,7 @@
     </row>
     <row r="65" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B65" s="37" t="s">
         <v>842</v>
@@ -8724,7 +8724,7 @@
     </row>
     <row r="66" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B66" s="37" t="s">
         <v>843</v>
@@ -8762,7 +8762,7 @@
     </row>
     <row r="68" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B68" s="37" t="s">
         <v>845</v>
@@ -8781,7 +8781,7 @@
     </row>
     <row r="69" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B69" s="37" t="s">
         <v>846</v>

</xml_diff>

<commit_message>
All HVAC systems running again
</commit_message>
<xml_diff>
--- a/projects/m0.xlsx
+++ b/projects/m0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="720" windowWidth="14880" windowHeight="7425" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="780" windowWidth="14880" windowHeight="7365" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -2623,6 +2623,9 @@
     <t>add_thermostats</t>
   </si>
   <si>
+    <t>SysType 7</t>
+  </si>
+  <si>
     <t>Rename Spaces and Thermal Zones By Story and Standards Space Type</t>
   </si>
   <si>
@@ -2633,9 +2636,6 @@
   </si>
   <si>
     <t>Window to Wall Ratio Multiplier</t>
-  </si>
-  <si>
-    <t>SysType 6</t>
   </si>
   <si>
     <t>RenameSpacesAndThermalZonesByStoryAndStandardsSpaceType</t>
@@ -6847,8 +6847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7270,9 +7270,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y125"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7577,7 +7577,7 @@
         <v>104</v>
       </c>
       <c r="H11" s="31" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
       <c r="I11" s="31"/>
     </row>
@@ -7680,7 +7680,7 @@
         <v>104</v>
       </c>
       <c r="H16" s="31" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
       <c r="I16" s="31"/>
     </row>
@@ -7783,7 +7783,7 @@
         <v>104</v>
       </c>
       <c r="H21" s="31" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
       <c r="I21" s="31"/>
     </row>
@@ -7901,10 +7901,10 @@
         <v>0</v>
       </c>
       <c r="B27" s="49" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="C27" s="49" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="D27" s="49" t="s">
         <v>865</v>
@@ -8293,10 +8293,10 @@
         <v>21</v>
       </c>
       <c r="D46" s="31" t="s">
+        <v>864</v>
+      </c>
+      <c r="E46" s="31" t="s">
         <v>863</v>
-      </c>
-      <c r="E46" s="31" t="s">
-        <v>862</v>
       </c>
       <c r="F46" s="31" t="s">
         <v>619</v>
@@ -8648,7 +8648,7 @@
     </row>
     <row r="62" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B62" s="37" t="s">
         <v>839</v>
@@ -8667,7 +8667,7 @@
     </row>
     <row r="63" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B63" s="37" t="s">
         <v>840</v>
@@ -8686,7 +8686,7 @@
     </row>
     <row r="64" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B64" s="37" t="s">
         <v>841</v>
@@ -8705,7 +8705,7 @@
     </row>
     <row r="65" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B65" s="37" t="s">
         <v>842</v>
@@ -8724,7 +8724,7 @@
     </row>
     <row r="66" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B66" s="37" t="s">
         <v>843</v>
@@ -8762,7 +8762,7 @@
     </row>
     <row r="68" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B68" s="37" t="s">
         <v>845</v>
@@ -8781,7 +8781,7 @@
     </row>
     <row r="69" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B69" s="37" t="s">
         <v>846</v>

</xml_diff>

<commit_message>
adding basic reporting measure to model 0 workflow
It is turned off now until I test it later on.
</commit_message>
<xml_diff>
--- a/projects/m0.xlsx
+++ b/projects/m0.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2415" uniqueCount="863">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2419" uniqueCount="866">
   <si>
     <t>type</t>
   </si>
@@ -2630,6 +2630,15 @@
   </si>
   <si>
     <t>Window to Wall Ratio Multiplier</t>
+  </si>
+  <si>
+    <t>coffee_annual_summary_report</t>
+  </si>
+  <si>
+    <t>COFFEE Annual Summary Report</t>
+  </si>
+  <si>
+    <t>COFFEEAnnualSummaryReport</t>
   </si>
 </sst>
 </file>
@@ -7254,7 +7263,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
+      <selection pane="bottomLeft" activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8761,9 +8770,24 @@
       <c r="G68" s="38"/>
       <c r="H68" s="38"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H69" s="31"/>
-      <c r="I69" s="31"/>
+    <row r="69" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="37" t="b">
+        <v>0</v>
+      </c>
+      <c r="B69" s="37" t="s">
+        <v>864</v>
+      </c>
+      <c r="C69" s="37" t="s">
+        <v>863</v>
+      </c>
+      <c r="D69" s="37" t="s">
+        <v>865</v>
+      </c>
+      <c r="E69" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G69" s="38"/>
+      <c r="H69" s="38"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H70" s="31"/>

</xml_diff>

<commit_message>
fixed measure type for reporting measure
Added start of reporting measure to workflow. It runs, but needs more
data and some graphic work
</commit_message>
<xml_diff>
--- a/projects/m0.xlsx
+++ b/projects/m0.xlsx
@@ -7263,7 +7263,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A70" sqref="A70"/>
+      <selection pane="bottomLeft" activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8772,7 +8772,7 @@
     </row>
     <row r="69" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B69" s="37" t="s">
         <v>864</v>
@@ -8784,7 +8784,7 @@
         <v>865</v>
       </c>
       <c r="E69" s="37" t="s">
-        <v>68</v>
+        <v>233</v>
       </c>
       <c r="G69" s="38"/>
       <c r="H69" s="38"/>

</xml_diff>

<commit_message>
adding new fenestration arguments
Updating model 0 spreadsheet to work with updated fenestration measure
arguments.
</commit_message>
<xml_diff>
--- a/projects/m0.xlsx
+++ b/projects/m0.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$55</definedName>
     <definedName name="AnalysisType">Lookups!$A$17:$A$23</definedName>
     <definedName name="instance_defs">Lookups!$A$2:$D$9</definedName>
     <definedName name="instance_types">Lookups!$A$2:$A$9</definedName>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2419" uniqueCount="866">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2431" uniqueCount="872">
   <si>
     <t>type</t>
   </si>
@@ -2639,6 +2639,24 @@
   </si>
   <si>
     <t>COFFEEAnnualSummaryReport</t>
+  </si>
+  <si>
+    <t>multiplier_overhang</t>
+  </si>
+  <si>
+    <t>Overhang Projection Factor Multiplier</t>
+  </si>
+  <si>
+    <t>multiplier_srr</t>
+  </si>
+  <si>
+    <t>Skylight to Roof Ratio Multiplier</t>
+  </si>
+  <si>
+    <t>multiplier_odwr</t>
+  </si>
+  <si>
+    <t>Overhead door to Wall Ratio Multiplier</t>
   </si>
 </sst>
 </file>
@@ -7259,11 +7277,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y123"/>
+  <dimension ref="A1:Y126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D71" sqref="D71"/>
+      <pane ySplit="3" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8266,34 +8284,40 @@
       <c r="P44" s="39"/>
       <c r="Q44" s="2"/>
     </row>
-    <row r="45" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="37" t="b">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B45" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" s="31" t="s">
+        <v>867</v>
+      </c>
+      <c r="E45" s="31" t="s">
+        <v>866</v>
+      </c>
+      <c r="F45" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H45" s="31">
         <v>1</v>
       </c>
-      <c r="B45" s="37" t="s">
-        <v>783</v>
-      </c>
-      <c r="C45" s="37" t="s">
-        <v>766</v>
-      </c>
-      <c r="D45" s="37" t="s">
-        <v>750</v>
-      </c>
-      <c r="E45" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G45" s="38"/>
-      <c r="H45" s="38"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="3"/>
+      <c r="P45" s="39"/>
+      <c r="Q45" s="2"/>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B46" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D46" s="31" t="s">
-        <v>784</v>
+        <v>869</v>
       </c>
       <c r="E46" s="31" t="s">
-        <v>785</v>
+        <v>868</v>
       </c>
       <c r="F46" s="31" t="s">
         <v>619</v>
@@ -8310,279 +8334,279 @@
       <c r="P46" s="39"/>
       <c r="Q46" s="2"/>
     </row>
-    <row r="47" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="37" t="b">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B47" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D47" s="31" t="s">
+        <v>871</v>
+      </c>
+      <c r="E47" s="31" t="s">
+        <v>870</v>
+      </c>
+      <c r="F47" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H47" s="31">
         <v>1</v>
       </c>
-      <c r="B47" s="37" t="s">
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
+      <c r="P47" s="39"/>
+      <c r="Q47" s="2"/>
+    </row>
+    <row r="48" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B48" s="37" t="s">
+        <v>783</v>
+      </c>
+      <c r="C48" s="37" t="s">
+        <v>766</v>
+      </c>
+      <c r="D48" s="37" t="s">
+        <v>750</v>
+      </c>
+      <c r="E48" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G48" s="38"/>
+      <c r="H48" s="38"/>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B49" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D49" s="31" t="s">
+        <v>784</v>
+      </c>
+      <c r="E49" s="31" t="s">
+        <v>785</v>
+      </c>
+      <c r="F49" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H49" s="31">
+        <v>1</v>
+      </c>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
+      <c r="N49" s="3"/>
+      <c r="P49" s="39"/>
+      <c r="Q49" s="2"/>
+    </row>
+    <row r="50" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B50" s="37" t="s">
         <v>786</v>
       </c>
-      <c r="C47" s="37" t="s">
+      <c r="C50" s="37" t="s">
         <v>767</v>
       </c>
-      <c r="D47" s="37" t="s">
+      <c r="D50" s="37" t="s">
         <v>751</v>
       </c>
-      <c r="E47" s="37" t="s">
+      <c r="E50" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G47" s="38"/>
-      <c r="H47" s="38"/>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B48" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D48" s="31" t="s">
+      <c r="G50" s="38"/>
+      <c r="H50" s="38"/>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B51" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D51" s="31" t="s">
         <v>787</v>
       </c>
-      <c r="E48" s="31" t="s">
+      <c r="E51" s="31" t="s">
         <v>788</v>
       </c>
-      <c r="F48" s="31" t="s">
+      <c r="F51" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="H48" s="31">
+      <c r="H51" s="31">
         <v>1</v>
       </c>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
-      <c r="L48" s="3"/>
-      <c r="M48" s="3"/>
-      <c r="N48" s="3"/>
-      <c r="P48" s="39"/>
-      <c r="Q48" s="2"/>
-    </row>
-    <row r="49" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="37" t="b">
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="3"/>
+      <c r="P51" s="39"/>
+      <c r="Q51" s="2"/>
+    </row>
+    <row r="52" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B49" s="37" t="s">
+      <c r="B52" s="37" t="s">
         <v>791</v>
       </c>
-      <c r="C49" s="37" t="s">
+      <c r="C52" s="37" t="s">
         <v>768</v>
       </c>
-      <c r="D49" s="37" t="s">
+      <c r="D52" s="37" t="s">
         <v>752</v>
       </c>
-      <c r="E49" s="37" t="s">
+      <c r="E52" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G49" s="38"/>
-      <c r="H49" s="38"/>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B50" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D50" s="31" t="s">
+      <c r="G52" s="38"/>
+      <c r="H52" s="38"/>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B53" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D53" s="31" t="s">
         <v>790</v>
       </c>
-      <c r="E50" s="31" t="s">
+      <c r="E53" s="31" t="s">
         <v>789</v>
       </c>
-      <c r="F50" s="31" t="s">
+      <c r="F53" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="H50" s="31">
+      <c r="H53" s="31">
         <v>1</v>
       </c>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
-      <c r="K50" s="3"/>
-      <c r="L50" s="3"/>
-      <c r="M50" s="3"/>
-      <c r="N50" s="3"/>
-      <c r="P50" s="39"/>
-      <c r="Q50" s="2"/>
-    </row>
-    <row r="51" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="37" t="b">
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="3"/>
+      <c r="L53" s="3"/>
+      <c r="M53" s="3"/>
+      <c r="N53" s="3"/>
+      <c r="P53" s="39"/>
+      <c r="Q53" s="2"/>
+    </row>
+    <row r="54" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B51" s="37" t="s">
+      <c r="B54" s="37" t="s">
         <v>792</v>
       </c>
-      <c r="C51" s="37" t="s">
+      <c r="C54" s="37" t="s">
         <v>769</v>
       </c>
-      <c r="D51" s="37" t="s">
+      <c r="D54" s="37" t="s">
         <v>753</v>
       </c>
-      <c r="E51" s="37" t="s">
+      <c r="E54" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G51" s="38"/>
-      <c r="H51" s="38"/>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B52" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D52" s="31" t="s">
+      <c r="G54" s="38"/>
+      <c r="H54" s="38"/>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B55" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D55" s="31" t="s">
         <v>794</v>
       </c>
-      <c r="E52" s="31" t="s">
+      <c r="E55" s="31" t="s">
         <v>793</v>
       </c>
-      <c r="F52" s="31" t="s">
+      <c r="F55" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="H52" s="31">
+      <c r="H55" s="31">
         <v>1</v>
       </c>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
-      <c r="K52" s="3"/>
-      <c r="L52" s="3"/>
-      <c r="M52" s="3"/>
-      <c r="N52" s="3"/>
-      <c r="P52" s="39"/>
-      <c r="Q52" s="2"/>
-    </row>
-    <row r="53" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="37" t="b">
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="3"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3"/>
+      <c r="N55" s="3"/>
+      <c r="P55" s="39"/>
+      <c r="Q55" s="2"/>
+    </row>
+    <row r="56" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B53" s="37" t="s">
+      <c r="B56" s="37" t="s">
         <v>815</v>
       </c>
-      <c r="C53" s="37" t="s">
+      <c r="C56" s="37" t="s">
         <v>816</v>
       </c>
-      <c r="D53" s="37" t="s">
+      <c r="D56" s="37" t="s">
         <v>814</v>
       </c>
-      <c r="E53" s="37" t="s">
+      <c r="E56" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G53" s="38"/>
-      <c r="H53" s="38"/>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B54" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D54" s="31" t="s">
+      <c r="G56" s="38"/>
+      <c r="H56" s="38"/>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B57" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D57" s="31" t="s">
         <v>818</v>
       </c>
-      <c r="E54" s="31" t="s">
+      <c r="E57" s="31" t="s">
         <v>817</v>
       </c>
-      <c r="F54" s="31" t="s">
+      <c r="F57" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="H54" s="31">
+      <c r="H57" s="31">
         <v>1</v>
       </c>
-      <c r="I54" s="3"/>
-      <c r="J54" s="3"/>
-      <c r="K54" s="3"/>
-      <c r="L54" s="3"/>
-      <c r="M54" s="3"/>
-      <c r="N54" s="3"/>
-      <c r="P54" s="39"/>
-      <c r="Q54" s="2"/>
-    </row>
-    <row r="55" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="37" t="b">
+      <c r="I57" s="3"/>
+      <c r="J57" s="3"/>
+      <c r="K57" s="3"/>
+      <c r="L57" s="3"/>
+      <c r="M57" s="3"/>
+      <c r="N57" s="3"/>
+      <c r="P57" s="39"/>
+      <c r="Q57" s="2"/>
+    </row>
+    <row r="58" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B55" s="37" t="s">
+      <c r="B58" s="37" t="s">
         <v>809</v>
       </c>
-      <c r="C55" s="37" t="s">
+      <c r="C58" s="37" t="s">
         <v>811</v>
       </c>
-      <c r="D55" s="37" t="s">
+      <c r="D58" s="37" t="s">
         <v>810</v>
       </c>
-      <c r="E55" s="37" t="s">
+      <c r="E58" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G55" s="38"/>
-      <c r="H55" s="38"/>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B56" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D56" s="31" t="s">
-        <v>813</v>
-      </c>
-      <c r="E56" s="31" t="s">
-        <v>812</v>
-      </c>
-      <c r="F56" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="H56" s="31">
-        <v>1</v>
-      </c>
-      <c r="I56" s="3"/>
-      <c r="J56" s="3"/>
-      <c r="K56" s="3"/>
-      <c r="L56" s="3"/>
-      <c r="M56" s="3"/>
-      <c r="N56" s="3"/>
-      <c r="P56" s="39"/>
-      <c r="Q56" s="2"/>
-    </row>
-    <row r="57" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="B57" s="37" t="s">
-        <v>802</v>
-      </c>
-      <c r="C57" s="37" t="s">
-        <v>804</v>
-      </c>
-      <c r="D57" s="37" t="s">
-        <v>803</v>
-      </c>
-      <c r="E57" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G57" s="38"/>
-      <c r="H57" s="38"/>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B58" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D58" s="31" t="s">
-        <v>807</v>
-      </c>
-      <c r="E58" s="31" t="s">
-        <v>805</v>
-      </c>
-      <c r="F58" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="H58" s="31">
-        <v>1</v>
-      </c>
-      <c r="I58" s="3"/>
-      <c r="J58" s="3"/>
-      <c r="K58" s="3"/>
-      <c r="L58" s="3"/>
-      <c r="M58" s="3"/>
-      <c r="N58" s="3"/>
-      <c r="P58" s="39"/>
-      <c r="Q58" s="2"/>
+      <c r="G58" s="38"/>
+      <c r="H58" s="38"/>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B59" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D59" s="31" t="s">
-        <v>808</v>
+        <v>813</v>
       </c>
       <c r="E59" s="31" t="s">
-        <v>806</v>
+        <v>812</v>
       </c>
       <c r="F59" s="31" t="s">
         <v>619</v>
@@ -8604,13 +8628,13 @@
         <v>1</v>
       </c>
       <c r="B60" s="37" t="s">
-        <v>839</v>
+        <v>802</v>
       </c>
       <c r="C60" s="37" t="s">
-        <v>847</v>
+        <v>804</v>
       </c>
       <c r="D60" s="37" t="s">
-        <v>831</v>
+        <v>803</v>
       </c>
       <c r="E60" s="37" t="s">
         <v>68</v>
@@ -8618,56 +8642,68 @@
       <c r="G60" s="38"/>
       <c r="H60" s="38"/>
     </row>
-    <row r="61" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="37" t="b">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B61" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D61" s="31" t="s">
+        <v>807</v>
+      </c>
+      <c r="E61" s="31" t="s">
+        <v>805</v>
+      </c>
+      <c r="F61" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H61" s="31">
         <v>1</v>
       </c>
-      <c r="B61" s="37" t="s">
-        <v>840</v>
-      </c>
-      <c r="C61" s="37" t="s">
-        <v>848</v>
-      </c>
-      <c r="D61" s="37" t="s">
-        <v>832</v>
-      </c>
-      <c r="E61" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G61" s="38"/>
-      <c r="H61" s="38"/>
-    </row>
-    <row r="62" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="37" t="b">
+      <c r="I61" s="3"/>
+      <c r="J61" s="3"/>
+      <c r="K61" s="3"/>
+      <c r="L61" s="3"/>
+      <c r="M61" s="3"/>
+      <c r="N61" s="3"/>
+      <c r="P61" s="39"/>
+      <c r="Q61" s="2"/>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B62" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D62" s="31" t="s">
+        <v>808</v>
+      </c>
+      <c r="E62" s="31" t="s">
+        <v>806</v>
+      </c>
+      <c r="F62" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H62" s="31">
         <v>1</v>
       </c>
-      <c r="B62" s="37" t="s">
-        <v>841</v>
-      </c>
-      <c r="C62" s="37" t="s">
-        <v>849</v>
-      </c>
-      <c r="D62" s="37" t="s">
-        <v>833</v>
-      </c>
-      <c r="E62" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G62" s="38"/>
-      <c r="H62" s="38"/>
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="3"/>
+      <c r="L62" s="3"/>
+      <c r="M62" s="3"/>
+      <c r="N62" s="3"/>
+      <c r="P62" s="39"/>
+      <c r="Q62" s="2"/>
     </row>
     <row r="63" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="37" t="b">
         <v>1</v>
       </c>
       <c r="B63" s="37" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="C63" s="37" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
       <c r="D63" s="37" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="E63" s="37" t="s">
         <v>68</v>
@@ -8680,13 +8716,13 @@
         <v>1</v>
       </c>
       <c r="B64" s="37" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="C64" s="37" t="s">
-        <v>851</v>
+        <v>848</v>
       </c>
       <c r="D64" s="37" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="E64" s="37" t="s">
         <v>68</v>
@@ -8699,13 +8735,13 @@
         <v>1</v>
       </c>
       <c r="B65" s="37" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="C65" s="37" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="D65" s="37" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="E65" s="37" t="s">
         <v>68</v>
@@ -8718,13 +8754,13 @@
         <v>1</v>
       </c>
       <c r="B66" s="37" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="C66" s="37" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
       <c r="D66" s="37" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="E66" s="37" t="s">
         <v>68</v>
@@ -8737,13 +8773,13 @@
         <v>1</v>
       </c>
       <c r="B67" s="37" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C67" s="37" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
       <c r="D67" s="37" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
       <c r="E67" s="37" t="s">
         <v>68</v>
@@ -8756,13 +8792,13 @@
         <v>1</v>
       </c>
       <c r="B68" s="37" t="s">
-        <v>827</v>
+        <v>844</v>
       </c>
       <c r="C68" s="37" t="s">
-        <v>828</v>
+        <v>852</v>
       </c>
       <c r="D68" s="37" t="s">
-        <v>829</v>
+        <v>836</v>
       </c>
       <c r="E68" s="37" t="s">
         <v>68</v>
@@ -8775,31 +8811,76 @@
         <v>1</v>
       </c>
       <c r="B69" s="37" t="s">
-        <v>864</v>
+        <v>845</v>
       </c>
       <c r="C69" s="37" t="s">
-        <v>863</v>
+        <v>853</v>
       </c>
       <c r="D69" s="37" t="s">
-        <v>865</v>
+        <v>837</v>
       </c>
       <c r="E69" s="37" t="s">
-        <v>233</v>
+        <v>68</v>
       </c>
       <c r="G69" s="38"/>
       <c r="H69" s="38"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H70" s="31"/>
-      <c r="I70" s="31"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H71" s="31"/>
-      <c r="I71" s="31"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H72" s="31"/>
-      <c r="I72" s="31"/>
+    <row r="70" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B70" s="37" t="s">
+        <v>846</v>
+      </c>
+      <c r="C70" s="37" t="s">
+        <v>854</v>
+      </c>
+      <c r="D70" s="37" t="s">
+        <v>838</v>
+      </c>
+      <c r="E70" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G70" s="38"/>
+      <c r="H70" s="38"/>
+    </row>
+    <row r="71" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B71" s="37" t="s">
+        <v>827</v>
+      </c>
+      <c r="C71" s="37" t="s">
+        <v>828</v>
+      </c>
+      <c r="D71" s="37" t="s">
+        <v>829</v>
+      </c>
+      <c r="E71" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G71" s="38"/>
+      <c r="H71" s="38"/>
+    </row>
+    <row r="72" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B72" s="37" t="s">
+        <v>864</v>
+      </c>
+      <c r="C72" s="37" t="s">
+        <v>863</v>
+      </c>
+      <c r="D72" s="37" t="s">
+        <v>865</v>
+      </c>
+      <c r="E72" s="37" t="s">
+        <v>233</v>
+      </c>
+      <c r="G72" s="38"/>
+      <c r="H72" s="38"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H73" s="31"/>
@@ -9005,8 +9086,20 @@
       <c r="H123" s="31"/>
       <c r="I123" s="31"/>
     </row>
+    <row r="124" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H124" s="31"/>
+      <c r="I124" s="31"/>
+    </row>
+    <row r="125" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H125" s="31"/>
+      <c r="I125" s="31"/>
+    </row>
+    <row r="126" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H126" s="31"/>
+      <c r="I126" s="31"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:Z52"/>
+  <autoFilter ref="A2:Z55"/>
   <mergeCells count="1">
     <mergeCell ref="T1:Y1"/>
   </mergeCells>

</xml_diff>